<commit_message>
Simplified migration to ExtendedDocumentSupport and removed ExtendedDocumentSupport for reportingPeriod from xlsx
</commit_message>
<xml_diff>
--- a/dataland-framework-toolbox/inputs/eu-taxonomy-financials/eu-taxonomy-financials.xlsx
+++ b/dataland-framework-toolbox/inputs/eu-taxonomy-financials/eu-taxonomy-financials.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d93401\Projects\Dataland\dataland-framework-toolbox\inputs\eu-taxonomy-financials\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d93476\Dataland\dataland-framework-toolbox\inputs\eu-taxonomy-financials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{159681AA-4557-46FB-B76D-B1803E2503B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60D1DB97-0286-43AF-A917-68FA6D547DC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Framework Data Model" sheetId="1" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1040" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1039" uniqueCount="203">
   <si>
     <t>Field Identifier</t>
   </si>
@@ -2116,22 +2116,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L178"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A143" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E158" sqref="E158"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="12.453125" customWidth="1"/>
-    <col min="3" max="3" width="20.26953125" customWidth="1"/>
-    <col min="4" max="4" width="95.1796875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="78.7265625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="40.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.6328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="12" width="14.26953125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.44140625" customWidth="1"/>
+    <col min="3" max="3" width="20.21875" customWidth="1"/>
+    <col min="4" max="4" width="95.21875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="78.77734375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="40.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="12" width="14.21875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="104" t="s">
         <v>0</v>
       </c>
@@ -2169,7 +2169,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="38">
         <v>0</v>
       </c>
@@ -2188,14 +2188,12 @@
       </c>
       <c r="G2" s="42"/>
       <c r="H2" s="43"/>
-      <c r="I2" s="44" t="s">
-        <v>26</v>
-      </c>
+      <c r="I2" s="44"/>
       <c r="J2" s="44"/>
       <c r="K2" s="44"/>
       <c r="L2" s="44"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="38">
         <v>1</v>
       </c>
@@ -2223,7 +2221,7 @@
       <c r="K3" s="44"/>
       <c r="L3" s="44"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="38">
         <v>2</v>
       </c>
@@ -2251,7 +2249,7 @@
       <c r="K4" s="43"/>
       <c r="L4" s="44"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="38">
         <v>3</v>
       </c>
@@ -2277,7 +2275,7 @@
       <c r="K5" s="44"/>
       <c r="L5" s="44"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="38">
         <v>4</v>
       </c>
@@ -2305,7 +2303,7 @@
       <c r="K6" s="44"/>
       <c r="L6" s="44"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="38">
         <v>5</v>
       </c>
@@ -2333,7 +2331,7 @@
       <c r="K7" s="44"/>
       <c r="L7" s="44"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="38">
         <v>6</v>
       </c>
@@ -2359,7 +2357,7 @@
       <c r="K8" s="44"/>
       <c r="L8" s="44"/>
     </row>
-    <row r="9" spans="1:12" s="12" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:12" s="12" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="50">
         <v>7</v>
       </c>
@@ -2385,7 +2383,7 @@
       <c r="K9" s="55"/>
       <c r="L9" s="56"/>
     </row>
-    <row r="10" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="57">
         <v>8</v>
       </c>
@@ -2413,7 +2411,7 @@
       <c r="K10" s="44"/>
       <c r="L10" s="107"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="57">
         <v>9</v>
       </c>
@@ -2441,7 +2439,7 @@
       <c r="K11" s="44"/>
       <c r="L11" s="44"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="57">
         <v>10</v>
       </c>
@@ -2469,7 +2467,7 @@
       <c r="K12" s="44"/>
       <c r="L12" s="44"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="57">
         <v>11</v>
       </c>
@@ -2497,7 +2495,7 @@
       <c r="K13" s="44"/>
       <c r="L13" s="44"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="57">
         <v>12</v>
       </c>
@@ -2525,7 +2523,7 @@
       <c r="K14" s="44"/>
       <c r="L14" s="44"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="57">
         <v>13</v>
       </c>
@@ -2553,7 +2551,7 @@
       <c r="K15" s="44"/>
       <c r="L15" s="44"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="57">
         <v>14</v>
       </c>
@@ -2581,7 +2579,7 @@
       <c r="K16" s="44"/>
       <c r="L16" s="44"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="57">
         <v>15</v>
       </c>
@@ -2609,7 +2607,7 @@
       <c r="K17" s="44"/>
       <c r="L17" s="44"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" s="57">
         <v>16</v>
       </c>
@@ -2637,7 +2635,7 @@
       <c r="K18" s="44"/>
       <c r="L18" s="44"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" s="57">
         <v>17</v>
       </c>
@@ -2665,7 +2663,7 @@
       <c r="K19" s="44"/>
       <c r="L19" s="44"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" s="57">
         <v>18</v>
       </c>
@@ -2693,7 +2691,7 @@
       <c r="K20" s="44"/>
       <c r="L20" s="44"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" s="57">
         <v>19</v>
       </c>
@@ -2721,7 +2719,7 @@
       <c r="K21" s="44"/>
       <c r="L21" s="44"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" s="57">
         <v>20</v>
       </c>
@@ -2749,7 +2747,7 @@
       <c r="K22" s="44"/>
       <c r="L22" s="44"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" s="57">
         <v>21</v>
       </c>
@@ -2777,7 +2775,7 @@
       <c r="K23" s="44"/>
       <c r="L23" s="44"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" s="57">
         <v>22</v>
       </c>
@@ -2805,7 +2803,7 @@
       <c r="K24" s="44"/>
       <c r="L24" s="44"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" s="57">
         <v>23</v>
       </c>
@@ -2833,7 +2831,7 @@
       <c r="K25" s="44"/>
       <c r="L25" s="44"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" s="57">
         <v>24</v>
       </c>
@@ -2861,7 +2859,7 @@
       <c r="K26" s="44"/>
       <c r="L26" s="44"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" s="57">
         <v>25</v>
       </c>
@@ -2889,7 +2887,7 @@
       <c r="K27" s="44"/>
       <c r="L27" s="44"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" s="57">
         <v>26</v>
       </c>
@@ -2917,7 +2915,7 @@
       <c r="K28" s="44"/>
       <c r="L28" s="44"/>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" s="57">
         <v>27</v>
       </c>
@@ -2945,7 +2943,7 @@
       <c r="K29" s="44"/>
       <c r="L29" s="44"/>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" s="57">
         <v>28</v>
       </c>
@@ -2973,7 +2971,7 @@
       <c r="K30" s="44"/>
       <c r="L30" s="44"/>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" s="57">
         <v>29</v>
       </c>
@@ -3001,7 +2999,7 @@
       <c r="K31" s="44"/>
       <c r="L31" s="44"/>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" s="57">
         <v>30</v>
       </c>
@@ -3029,7 +3027,7 @@
       <c r="K32" s="44"/>
       <c r="L32" s="44"/>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33" s="57">
         <v>31</v>
       </c>
@@ -3057,7 +3055,7 @@
       <c r="K33" s="44"/>
       <c r="L33" s="44"/>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34" s="57">
         <v>32</v>
       </c>
@@ -3085,7 +3083,7 @@
       <c r="K34" s="44"/>
       <c r="L34" s="44"/>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35" s="57">
         <v>33</v>
       </c>
@@ -3113,7 +3111,7 @@
       <c r="K35" s="44"/>
       <c r="L35" s="44"/>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36" s="57">
         <v>34</v>
       </c>
@@ -3141,7 +3139,7 @@
       <c r="K36" s="44"/>
       <c r="L36" s="44"/>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37" s="57">
         <v>35</v>
       </c>
@@ -3169,7 +3167,7 @@
       <c r="K37" s="44"/>
       <c r="L37" s="44"/>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38" s="68">
         <v>36</v>
       </c>
@@ -3197,7 +3195,7 @@
       <c r="K38" s="109"/>
       <c r="L38" s="109"/>
     </row>
-    <row r="39" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="129">
         <v>37</v>
       </c>
@@ -3225,7 +3223,7 @@
       <c r="K39" s="111"/>
       <c r="L39" s="111"/>
     </row>
-    <row r="40" spans="1:12" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:12" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A40" s="57">
         <v>38</v>
       </c>
@@ -3253,7 +3251,7 @@
       <c r="K40" s="44"/>
       <c r="L40" s="44"/>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A41" s="57">
         <v>39</v>
       </c>
@@ -3281,7 +3279,7 @@
       <c r="K41" s="44"/>
       <c r="L41" s="44"/>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A42" s="57">
         <v>40</v>
       </c>
@@ -3309,7 +3307,7 @@
       <c r="K42" s="44"/>
       <c r="L42" s="44"/>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A43" s="57">
         <v>41</v>
       </c>
@@ -3337,7 +3335,7 @@
       <c r="K43" s="44"/>
       <c r="L43" s="44"/>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A44" s="57">
         <v>42</v>
       </c>
@@ -3365,7 +3363,7 @@
       <c r="K44" s="44"/>
       <c r="L44" s="44"/>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A45" s="57">
         <v>43</v>
       </c>
@@ -3393,7 +3391,7 @@
       <c r="K45" s="44"/>
       <c r="L45" s="44"/>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A46" s="57">
         <v>44</v>
       </c>
@@ -3421,7 +3419,7 @@
       <c r="K46" s="44"/>
       <c r="L46" s="44"/>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A47" s="57">
         <v>45</v>
       </c>
@@ -3449,7 +3447,7 @@
       <c r="K47" s="44"/>
       <c r="L47" s="44"/>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A48" s="57">
         <v>46</v>
       </c>
@@ -3477,7 +3475,7 @@
       <c r="K48" s="44"/>
       <c r="L48" s="44"/>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A49" s="57">
         <v>47</v>
       </c>
@@ -3505,7 +3503,7 @@
       <c r="K49" s="44"/>
       <c r="L49" s="44"/>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A50" s="57">
         <v>48</v>
       </c>
@@ -3533,7 +3531,7 @@
       <c r="K50" s="44"/>
       <c r="L50" s="44"/>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A51" s="57">
         <v>49</v>
       </c>
@@ -3561,7 +3559,7 @@
       <c r="K51" s="44"/>
       <c r="L51" s="44"/>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A52" s="57">
         <v>50</v>
       </c>
@@ -3589,7 +3587,7 @@
       <c r="K52" s="44"/>
       <c r="L52" s="44"/>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A53" s="57">
         <v>51</v>
       </c>
@@ -3617,7 +3615,7 @@
       <c r="K53" s="44"/>
       <c r="L53" s="44"/>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A54" s="57">
         <v>52</v>
       </c>
@@ -3645,7 +3643,7 @@
       <c r="K54" s="44"/>
       <c r="L54" s="44"/>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A55" s="57">
         <v>53</v>
       </c>
@@ -3673,7 +3671,7 @@
       <c r="K55" s="44"/>
       <c r="L55" s="44"/>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A56" s="57">
         <v>54</v>
       </c>
@@ -3701,7 +3699,7 @@
       <c r="K56" s="44"/>
       <c r="L56" s="44"/>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A57" s="57">
         <v>55</v>
       </c>
@@ -3729,7 +3727,7 @@
       <c r="K57" s="44"/>
       <c r="L57" s="44"/>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A58" s="57">
         <v>56</v>
       </c>
@@ -3757,7 +3755,7 @@
       <c r="K58" s="44"/>
       <c r="L58" s="44"/>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A59" s="57">
         <v>57</v>
       </c>
@@ -3785,7 +3783,7 @@
       <c r="K59" s="44"/>
       <c r="L59" s="44"/>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A60" s="57">
         <v>58</v>
       </c>
@@ -3813,7 +3811,7 @@
       <c r="K60" s="44"/>
       <c r="L60" s="44"/>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A61" s="57">
         <v>59</v>
       </c>
@@ -3841,7 +3839,7 @@
       <c r="K61" s="44"/>
       <c r="L61" s="44"/>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A62" s="57">
         <v>60</v>
       </c>
@@ -3869,7 +3867,7 @@
       <c r="K62" s="44"/>
       <c r="L62" s="44"/>
     </row>
-    <row r="63" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:12" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="57">
         <v>61</v>
       </c>
@@ -3897,7 +3895,7 @@
       <c r="K63" s="44"/>
       <c r="L63" s="44"/>
     </row>
-    <row r="64" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:12" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="57">
         <v>62</v>
       </c>
@@ -3925,7 +3923,7 @@
       <c r="K64" s="44"/>
       <c r="L64" s="44"/>
     </row>
-    <row r="65" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:12" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="57">
         <v>63</v>
       </c>
@@ -3953,7 +3951,7 @@
       <c r="K65" s="44"/>
       <c r="L65" s="44"/>
     </row>
-    <row r="66" spans="1:12" ht="14.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:12" ht="14.55" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A66" s="77">
         <v>64</v>
       </c>
@@ -3981,7 +3979,7 @@
       <c r="K66" s="55"/>
       <c r="L66" s="55"/>
     </row>
-    <row r="67" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:12" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="81">
         <v>65</v>
       </c>
@@ -4009,7 +4007,7 @@
       <c r="K67" s="44"/>
       <c r="L67" s="44"/>
     </row>
-    <row r="68" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:12" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="81">
         <v>66</v>
       </c>
@@ -4037,7 +4035,7 @@
       <c r="K68" s="44"/>
       <c r="L68" s="44"/>
     </row>
-    <row r="69" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:12" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="81">
         <v>67</v>
       </c>
@@ -4065,7 +4063,7 @@
       <c r="K69" s="44"/>
       <c r="L69" s="44"/>
     </row>
-    <row r="70" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:12" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="81">
         <v>68</v>
       </c>
@@ -4093,7 +4091,7 @@
       <c r="K70" s="44"/>
       <c r="L70" s="44"/>
     </row>
-    <row r="71" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:12" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="81">
         <v>69</v>
       </c>
@@ -4121,7 +4119,7 @@
       <c r="K71" s="44"/>
       <c r="L71" s="44"/>
     </row>
-    <row r="72" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:12" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="81">
         <v>70</v>
       </c>
@@ -4149,7 +4147,7 @@
       <c r="K72" s="44"/>
       <c r="L72" s="44"/>
     </row>
-    <row r="73" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:12" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="81">
         <v>71</v>
       </c>
@@ -4177,7 +4175,7 @@
       <c r="K73" s="44"/>
       <c r="L73" s="44"/>
     </row>
-    <row r="74" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:12" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="81">
         <v>72</v>
       </c>
@@ -4205,7 +4203,7 @@
       <c r="K74" s="44"/>
       <c r="L74" s="44"/>
     </row>
-    <row r="75" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:12" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="81">
         <v>73</v>
       </c>
@@ -4233,7 +4231,7 @@
       <c r="K75" s="44"/>
       <c r="L75" s="44"/>
     </row>
-    <row r="76" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:12" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" s="81">
         <v>74</v>
       </c>
@@ -4261,7 +4259,7 @@
       <c r="K76" s="44"/>
       <c r="L76" s="44"/>
     </row>
-    <row r="77" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:12" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="81">
         <v>75</v>
       </c>
@@ -4289,7 +4287,7 @@
       <c r="K77" s="44"/>
       <c r="L77" s="44"/>
     </row>
-    <row r="78" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:12" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="81">
         <v>76</v>
       </c>
@@ -4317,7 +4315,7 @@
       <c r="K78" s="44"/>
       <c r="L78" s="44"/>
     </row>
-    <row r="79" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:12" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" s="81">
         <v>77</v>
       </c>
@@ -4345,7 +4343,7 @@
       <c r="K79" s="109"/>
       <c r="L79" s="109"/>
     </row>
-    <row r="80" spans="1:12" ht="14.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="80" spans="1:12" ht="14.55" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A80" s="83">
         <v>78</v>
       </c>
@@ -4373,7 +4371,7 @@
       <c r="K80" s="114"/>
       <c r="L80" s="115"/>
     </row>
-    <row r="81" spans="1:12" ht="14.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:12" ht="14.55" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A81" s="87">
         <v>79</v>
       </c>
@@ -4401,7 +4399,7 @@
       <c r="K81" s="116"/>
       <c r="L81" s="116"/>
     </row>
-    <row r="82" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:12" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82" s="87">
         <v>80</v>
       </c>
@@ -4429,7 +4427,7 @@
       <c r="K82" s="117"/>
       <c r="L82" s="117"/>
     </row>
-    <row r="83" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:12" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A83" s="87">
         <v>81</v>
       </c>
@@ -4457,7 +4455,7 @@
       <c r="K83" s="117"/>
       <c r="L83" s="117"/>
     </row>
-    <row r="84" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:12" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A84" s="87">
         <v>82</v>
       </c>
@@ -4485,7 +4483,7 @@
       <c r="K84" s="117"/>
       <c r="L84" s="117"/>
     </row>
-    <row r="85" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:12" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85" s="87">
         <v>83</v>
       </c>
@@ -4513,7 +4511,7 @@
       <c r="K85" s="117"/>
       <c r="L85" s="117"/>
     </row>
-    <row r="86" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:12" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A86" s="87">
         <v>84</v>
       </c>
@@ -4541,7 +4539,7 @@
       <c r="K86" s="117"/>
       <c r="L86" s="117"/>
     </row>
-    <row r="87" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:12" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" s="87">
         <v>85</v>
       </c>
@@ -4569,7 +4567,7 @@
       <c r="K87" s="117"/>
       <c r="L87" s="117"/>
     </row>
-    <row r="88" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:12" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A88" s="87">
         <v>86</v>
       </c>
@@ -4597,7 +4595,7 @@
       <c r="K88" s="117"/>
       <c r="L88" s="117"/>
     </row>
-    <row r="89" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:12" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89" s="87">
         <v>87</v>
       </c>
@@ -4625,7 +4623,7 @@
       <c r="K89" s="117"/>
       <c r="L89" s="117"/>
     </row>
-    <row r="90" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:12" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A90" s="87">
         <v>88</v>
       </c>
@@ -4653,7 +4651,7 @@
       <c r="K90" s="117"/>
       <c r="L90" s="117"/>
     </row>
-    <row r="91" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:12" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A91" s="87">
         <v>89</v>
       </c>
@@ -4681,7 +4679,7 @@
       <c r="K91" s="117"/>
       <c r="L91" s="117"/>
     </row>
-    <row r="92" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:12" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A92" s="87">
         <v>90</v>
       </c>
@@ -4709,7 +4707,7 @@
       <c r="K92" s="117"/>
       <c r="L92" s="117"/>
     </row>
-    <row r="93" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:12" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A93" s="87">
         <v>91</v>
       </c>
@@ -4737,7 +4735,7 @@
       <c r="K93" s="117"/>
       <c r="L93" s="117"/>
     </row>
-    <row r="94" spans="1:12" ht="14.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="94" spans="1:12" ht="14.55" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A94" s="93">
         <v>92</v>
       </c>
@@ -4765,7 +4763,7 @@
       <c r="K94" s="118"/>
       <c r="L94" s="118"/>
     </row>
-    <row r="95" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:12" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A95" s="97">
         <v>93</v>
       </c>
@@ -4793,7 +4791,7 @@
       <c r="K95" s="119"/>
       <c r="L95" s="119"/>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A96" s="97">
         <v>94</v>
       </c>
@@ -4821,7 +4819,7 @@
       <c r="K96" s="120"/>
       <c r="L96" s="120"/>
     </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A97" s="97">
         <v>95</v>
       </c>
@@ -4849,7 +4847,7 @@
       <c r="K97" s="120"/>
       <c r="L97" s="120"/>
     </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A98" s="97">
         <v>96</v>
       </c>
@@ -4877,7 +4875,7 @@
       <c r="K98" s="120"/>
       <c r="L98" s="120"/>
     </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A99" s="97">
         <v>97</v>
       </c>
@@ -4905,7 +4903,7 @@
       <c r="K99" s="120"/>
       <c r="L99" s="120"/>
     </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A100" s="97">
         <v>98</v>
       </c>
@@ -4933,7 +4931,7 @@
       <c r="K100" s="120"/>
       <c r="L100" s="120"/>
     </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A101" s="97">
         <v>99</v>
       </c>
@@ -4961,7 +4959,7 @@
       <c r="K101" s="120"/>
       <c r="L101" s="120"/>
     </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A102" s="97">
         <v>100</v>
       </c>
@@ -4989,7 +4987,7 @@
       <c r="K102" s="120"/>
       <c r="L102" s="120"/>
     </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A103" s="97">
         <v>101</v>
       </c>
@@ -5017,7 +5015,7 @@
       <c r="K103" s="120"/>
       <c r="L103" s="120"/>
     </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A104" s="97">
         <v>102</v>
       </c>
@@ -5045,7 +5043,7 @@
       <c r="K104" s="120"/>
       <c r="L104" s="120"/>
     </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A105" s="97">
         <v>103</v>
       </c>
@@ -5073,7 +5071,7 @@
       <c r="K105" s="120"/>
       <c r="L105" s="120"/>
     </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A106" s="97">
         <v>104</v>
       </c>
@@ -5101,7 +5099,7 @@
       <c r="K106" s="120"/>
       <c r="L106" s="120"/>
     </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A107" s="97">
         <v>105</v>
       </c>
@@ -5129,7 +5127,7 @@
       <c r="K107" s="120"/>
       <c r="L107" s="120"/>
     </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A108" s="97">
         <v>106</v>
       </c>
@@ -5157,7 +5155,7 @@
       <c r="K108" s="120"/>
       <c r="L108" s="120"/>
     </row>
-    <row r="109" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="109" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A109" s="100">
         <v>107</v>
       </c>
@@ -5185,7 +5183,7 @@
       <c r="K109" s="121"/>
       <c r="L109" s="121"/>
     </row>
-    <row r="110" spans="1:12" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:12" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A110" s="97">
         <v>108</v>
       </c>
@@ -5213,7 +5211,7 @@
       <c r="K110" s="119"/>
       <c r="L110" s="119"/>
     </row>
-    <row r="111" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A111" s="97">
         <v>109</v>
       </c>
@@ -5241,7 +5239,7 @@
       <c r="K111" s="120"/>
       <c r="L111" s="120"/>
     </row>
-    <row r="112" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A112" s="97">
         <v>110</v>
       </c>
@@ -5269,7 +5267,7 @@
       <c r="K112" s="120"/>
       <c r="L112" s="120"/>
     </row>
-    <row r="113" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A113" s="97">
         <v>111</v>
       </c>
@@ -5297,7 +5295,7 @@
       <c r="K113" s="120"/>
       <c r="L113" s="120"/>
     </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A114" s="97">
         <v>112</v>
       </c>
@@ -5325,7 +5323,7 @@
       <c r="K114" s="120"/>
       <c r="L114" s="120"/>
     </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A115" s="97">
         <v>113</v>
       </c>
@@ -5353,7 +5351,7 @@
       <c r="K115" s="120"/>
       <c r="L115" s="120"/>
     </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A116" s="97">
         <v>114</v>
       </c>
@@ -5381,7 +5379,7 @@
       <c r="K116" s="120"/>
       <c r="L116" s="120"/>
     </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A117" s="97">
         <v>115</v>
       </c>
@@ -5409,7 +5407,7 @@
       <c r="K117" s="120"/>
       <c r="L117" s="120"/>
     </row>
-    <row r="118" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A118" s="97">
         <v>116</v>
       </c>
@@ -5437,7 +5435,7 @@
       <c r="K118" s="120"/>
       <c r="L118" s="120"/>
     </row>
-    <row r="119" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A119" s="97">
         <v>117</v>
       </c>
@@ -5465,7 +5463,7 @@
       <c r="K119" s="120"/>
       <c r="L119" s="120"/>
     </row>
-    <row r="120" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A120" s="97">
         <v>118</v>
       </c>
@@ -5493,7 +5491,7 @@
       <c r="K120" s="120"/>
       <c r="L120" s="120"/>
     </row>
-    <row r="121" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A121" s="97">
         <v>119</v>
       </c>
@@ -5521,7 +5519,7 @@
       <c r="K121" s="120"/>
       <c r="L121" s="120"/>
     </row>
-    <row r="122" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A122" s="97">
         <v>120</v>
       </c>
@@ -5549,7 +5547,7 @@
       <c r="K122" s="120"/>
       <c r="L122" s="120"/>
     </row>
-    <row r="123" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="123" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A123" s="102">
         <v>121</v>
       </c>
@@ -5577,7 +5575,7 @@
       <c r="K123" s="122"/>
       <c r="L123" s="122"/>
     </row>
-    <row r="124" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:12" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A124" s="134">
         <v>122</v>
       </c>
@@ -5605,7 +5603,7 @@
       <c r="K124" s="123"/>
       <c r="L124" s="123"/>
     </row>
-    <row r="125" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:12" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A125" s="134">
         <v>123</v>
       </c>
@@ -5633,7 +5631,7 @@
       <c r="K125" s="123"/>
       <c r="L125" s="123"/>
     </row>
-    <row r="126" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:12" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A126" s="134">
         <v>124</v>
       </c>
@@ -5661,7 +5659,7 @@
       <c r="K126" s="123"/>
       <c r="L126" s="123"/>
     </row>
-    <row r="127" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:12" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A127" s="134">
         <v>125</v>
       </c>
@@ -5689,7 +5687,7 @@
       <c r="K127" s="123"/>
       <c r="L127" s="123"/>
     </row>
-    <row r="128" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:12" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A128" s="134">
         <v>126</v>
       </c>
@@ -5717,7 +5715,7 @@
       <c r="K128" s="123"/>
       <c r="L128" s="123"/>
     </row>
-    <row r="129" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:12" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A129" s="134">
         <v>127</v>
       </c>
@@ -5745,7 +5743,7 @@
       <c r="K129" s="123"/>
       <c r="L129" s="123"/>
     </row>
-    <row r="130" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:12" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A130" s="134">
         <v>128</v>
       </c>
@@ -5773,7 +5771,7 @@
       <c r="K130" s="123"/>
       <c r="L130" s="123"/>
     </row>
-    <row r="131" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:12" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A131" s="134">
         <v>129</v>
       </c>
@@ -5801,7 +5799,7 @@
       <c r="K131" s="123"/>
       <c r="L131" s="123"/>
     </row>
-    <row r="132" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:12" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A132" s="134">
         <v>130</v>
       </c>
@@ -5829,7 +5827,7 @@
       <c r="K132" s="123"/>
       <c r="L132" s="123"/>
     </row>
-    <row r="133" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:12" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A133" s="134">
         <v>131</v>
       </c>
@@ -5857,7 +5855,7 @@
       <c r="K133" s="123"/>
       <c r="L133" s="123"/>
     </row>
-    <row r="134" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:12" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A134" s="134">
         <v>132</v>
       </c>
@@ -5885,7 +5883,7 @@
       <c r="K134" s="123"/>
       <c r="L134" s="123"/>
     </row>
-    <row r="135" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:12" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A135" s="134">
         <v>133</v>
       </c>
@@ -5913,7 +5911,7 @@
       <c r="K135" s="123"/>
       <c r="L135" s="123"/>
     </row>
-    <row r="136" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:12" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A136" s="134">
         <v>134</v>
       </c>
@@ -5941,7 +5939,7 @@
       <c r="K136" s="123"/>
       <c r="L136" s="123"/>
     </row>
-    <row r="137" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:12" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A137" s="134">
         <v>135</v>
       </c>
@@ -5969,7 +5967,7 @@
       <c r="K137" s="123"/>
       <c r="L137" s="123"/>
     </row>
-    <row r="138" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:12" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A138" s="134">
         <v>136</v>
       </c>
@@ -5997,7 +5995,7 @@
       <c r="K138" s="123"/>
       <c r="L138" s="123"/>
     </row>
-    <row r="139" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:12" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A139" s="134">
         <v>137</v>
       </c>
@@ -6025,7 +6023,7 @@
       <c r="K139" s="123"/>
       <c r="L139" s="123"/>
     </row>
-    <row r="140" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:12" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A140" s="134">
         <v>138</v>
       </c>
@@ -6053,7 +6051,7 @@
       <c r="K140" s="123"/>
       <c r="L140" s="123"/>
     </row>
-    <row r="141" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:12" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A141" s="134">
         <v>139</v>
       </c>
@@ -6081,7 +6079,7 @@
       <c r="K141" s="123"/>
       <c r="L141" s="123"/>
     </row>
-    <row r="142" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:12" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A142" s="134">
         <v>140</v>
       </c>
@@ -6109,7 +6107,7 @@
       <c r="K142" s="123"/>
       <c r="L142" s="123"/>
     </row>
-    <row r="143" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:12" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A143" s="134">
         <v>141</v>
       </c>
@@ -6137,7 +6135,7 @@
       <c r="K143" s="123"/>
       <c r="L143" s="123"/>
     </row>
-    <row r="144" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:12" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A144" s="134">
         <v>142</v>
       </c>
@@ -6165,7 +6163,7 @@
       <c r="K144" s="123"/>
       <c r="L144" s="123"/>
     </row>
-    <row r="145" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:12" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A145" s="134">
         <v>143</v>
       </c>
@@ -6193,7 +6191,7 @@
       <c r="K145" s="123"/>
       <c r="L145" s="123"/>
     </row>
-    <row r="146" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:12" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A146" s="134">
         <v>144</v>
       </c>
@@ -6221,7 +6219,7 @@
       <c r="K146" s="123"/>
       <c r="L146" s="123"/>
     </row>
-    <row r="147" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:12" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A147" s="134">
         <v>145</v>
       </c>
@@ -6249,7 +6247,7 @@
       <c r="K147" s="123"/>
       <c r="L147" s="123"/>
     </row>
-    <row r="148" spans="1:12" ht="14.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="148" spans="1:12" ht="14.55" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A148" s="135">
         <v>146</v>
       </c>
@@ -6277,7 +6275,7 @@
       <c r="K148" s="126"/>
       <c r="L148" s="126"/>
     </row>
-    <row r="149" spans="1:12" ht="14.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:12" ht="14.55" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A149" s="134">
         <v>147</v>
       </c>
@@ -6305,7 +6303,7 @@
       <c r="K149" s="123"/>
       <c r="L149" s="123"/>
     </row>
-    <row r="150" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:12" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A150" s="134">
         <v>148</v>
       </c>
@@ -6333,7 +6331,7 @@
       <c r="K150" s="123"/>
       <c r="L150" s="123"/>
     </row>
-    <row r="151" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:12" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A151" s="134">
         <v>149</v>
       </c>
@@ -6361,7 +6359,7 @@
       <c r="K151" s="123"/>
       <c r="L151" s="123"/>
     </row>
-    <row r="152" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:12" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A152" s="134">
         <v>150</v>
       </c>
@@ -6389,7 +6387,7 @@
       <c r="K152" s="123"/>
       <c r="L152" s="123"/>
     </row>
-    <row r="153" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:12" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A153" s="134">
         <v>151</v>
       </c>
@@ -6417,7 +6415,7 @@
       <c r="K153" s="123"/>
       <c r="L153" s="123"/>
     </row>
-    <row r="154" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:12" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A154" s="134">
         <v>152</v>
       </c>
@@ -6445,7 +6443,7 @@
       <c r="K154" s="123"/>
       <c r="L154" s="123"/>
     </row>
-    <row r="155" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:12" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A155" s="134">
         <v>153</v>
       </c>
@@ -6473,7 +6471,7 @@
       <c r="K155" s="123"/>
       <c r="L155" s="123"/>
     </row>
-    <row r="156" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:12" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A156" s="134">
         <v>154</v>
       </c>
@@ -6501,7 +6499,7 @@
       <c r="K156" s="123"/>
       <c r="L156" s="123"/>
     </row>
-    <row r="157" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:12" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A157" s="134">
         <v>155</v>
       </c>
@@ -6529,7 +6527,7 @@
       <c r="K157" s="123"/>
       <c r="L157" s="123"/>
     </row>
-    <row r="158" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:12" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A158" s="134">
         <v>156</v>
       </c>
@@ -6557,7 +6555,7 @@
       <c r="K158" s="123"/>
       <c r="L158" s="123"/>
     </row>
-    <row r="159" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:12" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A159" s="134">
         <v>157</v>
       </c>
@@ -6585,7 +6583,7 @@
       <c r="K159" s="123"/>
       <c r="L159" s="123"/>
     </row>
-    <row r="160" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:12" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A160" s="134">
         <v>158</v>
       </c>
@@ -6613,7 +6611,7 @@
       <c r="K160" s="123"/>
       <c r="L160" s="123"/>
     </row>
-    <row r="161" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:12" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A161" s="134">
         <v>159</v>
       </c>
@@ -6641,7 +6639,7 @@
       <c r="K161" s="123"/>
       <c r="L161" s="123"/>
     </row>
-    <row r="162" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:12" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A162" s="134">
         <v>160</v>
       </c>
@@ -6669,7 +6667,7 @@
       <c r="K162" s="123"/>
       <c r="L162" s="123"/>
     </row>
-    <row r="163" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:12" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A163" s="134">
         <v>161</v>
       </c>
@@ -6697,7 +6695,7 @@
       <c r="K163" s="123"/>
       <c r="L163" s="123"/>
     </row>
-    <row r="164" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:12" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A164" s="134">
         <v>162</v>
       </c>
@@ -6725,7 +6723,7 @@
       <c r="K164" s="123"/>
       <c r="L164" s="123"/>
     </row>
-    <row r="165" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:12" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A165" s="134">
         <v>163</v>
       </c>
@@ -6753,7 +6751,7 @@
       <c r="K165" s="123"/>
       <c r="L165" s="123"/>
     </row>
-    <row r="166" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:12" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A166" s="134">
         <v>164</v>
       </c>
@@ -6781,7 +6779,7 @@
       <c r="K166" s="123"/>
       <c r="L166" s="123"/>
     </row>
-    <row r="167" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:12" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A167" s="134">
         <v>165</v>
       </c>
@@ -6809,7 +6807,7 @@
       <c r="K167" s="123"/>
       <c r="L167" s="123"/>
     </row>
-    <row r="168" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:12" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A168" s="134">
         <v>166</v>
       </c>
@@ -6837,7 +6835,7 @@
       <c r="K168" s="123"/>
       <c r="L168" s="123"/>
     </row>
-    <row r="169" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:12" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A169" s="134">
         <v>167</v>
       </c>
@@ -6865,7 +6863,7 @@
       <c r="K169" s="123"/>
       <c r="L169" s="123"/>
     </row>
-    <row r="170" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:12" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A170" s="134">
         <v>168</v>
       </c>
@@ -6893,7 +6891,7 @@
       <c r="K170" s="123"/>
       <c r="L170" s="123"/>
     </row>
-    <row r="171" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:12" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A171" s="134">
         <v>169</v>
       </c>
@@ -6921,7 +6919,7 @@
       <c r="K171" s="123"/>
       <c r="L171" s="123"/>
     </row>
-    <row r="172" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:12" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A172" s="134">
         <v>170</v>
       </c>
@@ -6949,7 +6947,7 @@
       <c r="K172" s="123"/>
       <c r="L172" s="123"/>
     </row>
-    <row r="173" spans="1:12" ht="14.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="173" spans="1:12" ht="14.55" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A173" s="136">
         <v>171</v>
       </c>
@@ -6977,7 +6975,7 @@
       <c r="K173" s="127"/>
       <c r="L173" s="127"/>
     </row>
-    <row r="174" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A174" s="13"/>
       <c r="B174" s="2"/>
       <c r="C174" s="2"/>
@@ -6991,7 +6989,7 @@
       <c r="K174" s="4"/>
       <c r="L174" s="4"/>
     </row>
-    <row r="175" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A175" s="13"/>
       <c r="B175" s="2"/>
       <c r="C175" s="2"/>
@@ -7005,7 +7003,7 @@
       <c r="K175" s="4"/>
       <c r="L175" s="4"/>
     </row>
-    <row r="176" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A176" s="13"/>
       <c r="B176" s="2"/>
       <c r="C176" s="2"/>
@@ -7019,7 +7017,7 @@
       <c r="K176" s="4"/>
       <c r="L176" s="4"/>
     </row>
-    <row r="177" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A177" s="13"/>
       <c r="B177" s="2"/>
       <c r="C177" s="2"/>
@@ -7033,7 +7031,7 @@
       <c r="K177" s="4"/>
       <c r="L177" s="4"/>
     </row>
-    <row r="178" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A178" s="13"/>
       <c r="B178" s="2"/>
       <c r="C178" s="2"/>

</xml_diff>

<commit_message>
Update framework excel to include naming config for data point types
</commit_message>
<xml_diff>
--- a/dataland-framework-toolbox/inputs/eu-taxonomy-financials/eu-taxonomy-financials.xlsx
+++ b/dataland-framework-toolbox/inputs/eu-taxonomy-financials/eu-taxonomy-financials.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dataland\dataland\dataland-framework-toolbox\inputs\eu-taxonomy-financials\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d92582\Documents\Dataland\Dataland\dataland-framework-toolbox\inputs\eu-taxonomy-financials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4507D023-6539-407B-87D8-3DBB44A1B5AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9076012F-4300-4E6F-A85C-9CC34911F37C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57490" yWindow="-10800" windowWidth="38620" windowHeight="21220" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Framework Data Model" sheetId="1" r:id="rId1"/>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1492" uniqueCount="454">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1940" uniqueCount="457">
   <si>
     <t>Field Identifier</t>
   </si>
@@ -1428,6 +1428,15 @@
   </si>
   <si>
     <t>The date the fiscal year ends.</t>
+  </si>
+  <si>
+    <t>Include Category in Type Name</t>
+  </si>
+  <si>
+    <t>Include Sub-Category in Type Name</t>
+  </si>
+  <si>
+    <t>Yes</t>
   </si>
 </sst>
 </file>
@@ -2917,24 +2926,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L238"/>
+  <dimension ref="A1:N238"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="12.42578125" customWidth="1"/>
     <col min="3" max="3" width="71.5703125" customWidth="1"/>
-    <col min="4" max="4" width="95.140625" customWidth="1"/>
-    <col min="5" max="5" width="78.85546875" customWidth="1"/>
-    <col min="6" max="6" width="40.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="12" width="14.140625" customWidth="1"/>
+    <col min="4" max="4" width="123.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="92" customWidth="1"/>
+    <col min="6" max="6" width="36.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="30.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="107" t="s">
         <v>0</v>
       </c>
@@ -2971,8 +2986,14 @@
       <c r="L1" s="91" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M1" s="91" t="s">
+        <v>454</v>
+      </c>
+      <c r="N1" s="91" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="108">
         <v>1</v>
       </c>
@@ -3001,8 +3022,10 @@
       <c r="J2" s="34"/>
       <c r="K2" s="34"/>
       <c r="L2" s="34"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M2" s="34"/>
+      <c r="N2" s="34"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="108">
         <v>2</v>
       </c>
@@ -3031,8 +3054,10 @@
       <c r="J3" s="33"/>
       <c r="K3" s="33"/>
       <c r="L3" s="34"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M3" s="34"/>
+      <c r="N3" s="34"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="108">
         <v>3</v>
       </c>
@@ -3059,8 +3084,10 @@
       <c r="J4" s="34"/>
       <c r="K4" s="34"/>
       <c r="L4" s="34"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M4" s="34"/>
+      <c r="N4" s="34"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="108">
         <v>4</v>
       </c>
@@ -3089,8 +3116,10 @@
       <c r="J5" s="34"/>
       <c r="K5" s="34"/>
       <c r="L5" s="34"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M5" s="34"/>
+      <c r="N5" s="34"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="108">
         <v>5</v>
       </c>
@@ -3119,8 +3148,10 @@
       <c r="J6" s="34"/>
       <c r="K6" s="34"/>
       <c r="L6" s="34"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M6" s="34"/>
+      <c r="N6" s="34"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="108">
         <v>6</v>
       </c>
@@ -3147,8 +3178,10 @@
       <c r="J7" s="34"/>
       <c r="K7" s="34"/>
       <c r="L7" s="34"/>
-    </row>
-    <row r="8" spans="1:12" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M7" s="34"/>
+      <c r="N7" s="34"/>
+    </row>
+    <row r="8" spans="1:14" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="109">
         <v>7</v>
       </c>
@@ -3175,8 +3208,10 @@
       <c r="J8" s="41"/>
       <c r="K8" s="41"/>
       <c r="L8" s="11"/>
-    </row>
-    <row r="9" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M8" s="11"/>
+      <c r="N8" s="11"/>
+    </row>
+    <row r="9" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="73">
         <v>8</v>
       </c>
@@ -3205,8 +3240,14 @@
       <c r="J9" s="34"/>
       <c r="K9" s="34"/>
       <c r="L9" s="42"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M9" s="42" t="s">
+        <v>456</v>
+      </c>
+      <c r="N9" s="42" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="73">
         <v>9</v>
       </c>
@@ -3235,8 +3276,14 @@
       <c r="J10" s="34"/>
       <c r="K10" s="34"/>
       <c r="L10" s="34"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M10" s="34" t="s">
+        <v>456</v>
+      </c>
+      <c r="N10" s="34" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="73">
         <v>9.1</v>
       </c>
@@ -3265,8 +3312,14 @@
       <c r="J11" s="34"/>
       <c r="K11" s="34"/>
       <c r="L11" s="34"/>
-    </row>
-    <row r="12" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M11" s="34" t="s">
+        <v>456</v>
+      </c>
+      <c r="N11" s="34" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="72" t="s">
         <v>105</v>
       </c>
@@ -3295,8 +3348,14 @@
       <c r="J12" s="34"/>
       <c r="K12" s="34"/>
       <c r="L12" s="42"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M12" s="42" t="s">
+        <v>456</v>
+      </c>
+      <c r="N12" s="42" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="72" t="s">
         <v>106</v>
       </c>
@@ -3325,8 +3384,14 @@
       <c r="J13" s="34"/>
       <c r="K13" s="34"/>
       <c r="L13" s="34"/>
-    </row>
-    <row r="14" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M13" s="34" t="s">
+        <v>456</v>
+      </c>
+      <c r="N13" s="34" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="110" t="s">
         <v>107</v>
       </c>
@@ -3355,8 +3420,14 @@
       <c r="J14" s="41"/>
       <c r="K14" s="41"/>
       <c r="L14" s="41"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M14" s="41" t="s">
+        <v>456</v>
+      </c>
+      <c r="N14" s="41" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="72">
         <v>10</v>
       </c>
@@ -3383,8 +3454,14 @@
       <c r="J15" s="34"/>
       <c r="K15" s="34"/>
       <c r="L15" s="34"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M15" s="34" t="s">
+        <v>456</v>
+      </c>
+      <c r="N15" s="34" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="72">
         <v>10.1</v>
       </c>
@@ -3411,8 +3488,14 @@
       <c r="J16" s="34"/>
       <c r="K16" s="34"/>
       <c r="L16" s="34"/>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M16" s="34" t="s">
+        <v>456</v>
+      </c>
+      <c r="N16" s="34" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="72" t="s">
         <v>108</v>
       </c>
@@ -3439,8 +3522,14 @@
       <c r="J17" s="34"/>
       <c r="K17" s="34"/>
       <c r="L17" s="34"/>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M17" s="34" t="s">
+        <v>456</v>
+      </c>
+      <c r="N17" s="34" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="72" t="s">
         <v>109</v>
       </c>
@@ -3467,8 +3556,14 @@
       <c r="J18" s="34"/>
       <c r="K18" s="34"/>
       <c r="L18" s="34"/>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M18" s="34" t="s">
+        <v>456</v>
+      </c>
+      <c r="N18" s="34" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="72" t="s">
         <v>110</v>
       </c>
@@ -3495,8 +3590,14 @@
       <c r="J19" s="34"/>
       <c r="K19" s="34"/>
       <c r="L19" s="34"/>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M19" s="34" t="s">
+        <v>456</v>
+      </c>
+      <c r="N19" s="34" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="72">
         <v>11</v>
       </c>
@@ -3523,8 +3624,14 @@
       <c r="J20" s="34"/>
       <c r="K20" s="34"/>
       <c r="L20" s="34"/>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M20" s="34" t="s">
+        <v>456</v>
+      </c>
+      <c r="N20" s="34" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="72">
         <v>11.1</v>
       </c>
@@ -3551,8 +3658,14 @@
       <c r="J21" s="34"/>
       <c r="K21" s="34"/>
       <c r="L21" s="34"/>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M21" s="34" t="s">
+        <v>456</v>
+      </c>
+      <c r="N21" s="34" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="72" t="s">
         <v>111</v>
       </c>
@@ -3579,8 +3692,14 @@
       <c r="J22" s="34"/>
       <c r="K22" s="34"/>
       <c r="L22" s="34"/>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M22" s="34" t="s">
+        <v>456</v>
+      </c>
+      <c r="N22" s="34" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="72" t="s">
         <v>112</v>
       </c>
@@ -3607,8 +3726,14 @@
       <c r="J23" s="34"/>
       <c r="K23" s="34"/>
       <c r="L23" s="34"/>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M23" s="34" t="s">
+        <v>456</v>
+      </c>
+      <c r="N23" s="34" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="72" t="s">
         <v>175</v>
       </c>
@@ -3635,8 +3760,14 @@
       <c r="J24" s="34"/>
       <c r="K24" s="34"/>
       <c r="L24" s="34"/>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M24" s="34" t="s">
+        <v>456</v>
+      </c>
+      <c r="N24" s="34" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="72">
         <v>12</v>
       </c>
@@ -3663,8 +3794,14 @@
       <c r="J25" s="34"/>
       <c r="K25" s="34"/>
       <c r="L25" s="34"/>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M25" s="34" t="s">
+        <v>456</v>
+      </c>
+      <c r="N25" s="34" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="72">
         <v>12.1</v>
       </c>
@@ -3691,8 +3828,14 @@
       <c r="J26" s="34"/>
       <c r="K26" s="34"/>
       <c r="L26" s="34"/>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M26" s="34" t="s">
+        <v>456</v>
+      </c>
+      <c r="N26" s="34" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="72" t="s">
         <v>113</v>
       </c>
@@ -3719,8 +3862,14 @@
       <c r="J27" s="34"/>
       <c r="K27" s="34"/>
       <c r="L27" s="34"/>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M27" s="34" t="s">
+        <v>456</v>
+      </c>
+      <c r="N27" s="34" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="72" t="s">
         <v>114</v>
       </c>
@@ -3747,8 +3896,14 @@
       <c r="J28" s="34"/>
       <c r="K28" s="34"/>
       <c r="L28" s="34"/>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M28" s="34" t="s">
+        <v>456</v>
+      </c>
+      <c r="N28" s="34" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="72">
         <v>13</v>
       </c>
@@ -3775,8 +3930,14 @@
       <c r="J29" s="34"/>
       <c r="K29" s="34"/>
       <c r="L29" s="34"/>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M29" s="34" t="s">
+        <v>456</v>
+      </c>
+      <c r="N29" s="34" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="72">
         <v>13.1</v>
       </c>
@@ -3803,8 +3964,14 @@
       <c r="J30" s="34"/>
       <c r="K30" s="34"/>
       <c r="L30" s="34"/>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M30" s="34" t="s">
+        <v>456</v>
+      </c>
+      <c r="N30" s="34" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="72" t="s">
         <v>115</v>
       </c>
@@ -3831,8 +3998,14 @@
       <c r="J31" s="34"/>
       <c r="K31" s="34"/>
       <c r="L31" s="34"/>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M31" s="34" t="s">
+        <v>456</v>
+      </c>
+      <c r="N31" s="34" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="72" t="s">
         <v>116</v>
       </c>
@@ -3859,8 +4032,14 @@
       <c r="J32" s="34"/>
       <c r="K32" s="34"/>
       <c r="L32" s="34"/>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M32" s="34" t="s">
+        <v>456</v>
+      </c>
+      <c r="N32" s="34" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="72">
         <v>14</v>
       </c>
@@ -3887,8 +4066,14 @@
       <c r="J33" s="34"/>
       <c r="K33" s="34"/>
       <c r="L33" s="34"/>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M33" s="34" t="s">
+        <v>456</v>
+      </c>
+      <c r="N33" s="34" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="72">
         <v>14.1</v>
       </c>
@@ -3915,8 +4100,14 @@
       <c r="J34" s="34"/>
       <c r="K34" s="34"/>
       <c r="L34" s="34"/>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M34" s="34" t="s">
+        <v>456</v>
+      </c>
+      <c r="N34" s="34" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="72" t="s">
         <v>117</v>
       </c>
@@ -3943,8 +4134,14 @@
       <c r="J35" s="34"/>
       <c r="K35" s="34"/>
       <c r="L35" s="34"/>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M35" s="34" t="s">
+        <v>456</v>
+      </c>
+      <c r="N35" s="34" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="72" t="s">
         <v>118</v>
       </c>
@@ -3971,8 +4168,14 @@
       <c r="J36" s="34"/>
       <c r="K36" s="34"/>
       <c r="L36" s="34"/>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M36" s="34" t="s">
+        <v>456</v>
+      </c>
+      <c r="N36" s="34" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="72">
         <v>15</v>
       </c>
@@ -3999,8 +4202,14 @@
       <c r="J37" s="34"/>
       <c r="K37" s="34"/>
       <c r="L37" s="34"/>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M37" s="34" t="s">
+        <v>456</v>
+      </c>
+      <c r="N37" s="34" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" s="72">
         <v>15.1</v>
       </c>
@@ -4027,8 +4236,14 @@
       <c r="J38" s="34"/>
       <c r="K38" s="34"/>
       <c r="L38" s="34"/>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M38" s="34" t="s">
+        <v>456</v>
+      </c>
+      <c r="N38" s="34" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" s="43" t="s">
         <v>119</v>
       </c>
@@ -4055,8 +4270,14 @@
       <c r="J39" s="45"/>
       <c r="K39" s="45"/>
       <c r="L39" s="45"/>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M39" s="45" t="s">
+        <v>456</v>
+      </c>
+      <c r="N39" s="45" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" s="72" t="s">
         <v>120</v>
       </c>
@@ -4083,8 +4304,14 @@
       <c r="J40" s="46"/>
       <c r="K40" s="46"/>
       <c r="L40" s="46"/>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M40" s="46" t="s">
+        <v>456</v>
+      </c>
+      <c r="N40" s="46" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" s="72">
         <v>16</v>
       </c>
@@ -4111,8 +4338,14 @@
       <c r="J41" s="34"/>
       <c r="K41" s="34"/>
       <c r="L41" s="34"/>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M41" s="34" t="s">
+        <v>456</v>
+      </c>
+      <c r="N41" s="34" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" s="72">
         <v>16.100000000000001</v>
       </c>
@@ -4139,8 +4372,14 @@
       <c r="J42" s="34"/>
       <c r="K42" s="34"/>
       <c r="L42" s="34"/>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M42" s="34" t="s">
+        <v>456</v>
+      </c>
+      <c r="N42" s="34" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" s="43" t="s">
         <v>121</v>
       </c>
@@ -4167,8 +4406,14 @@
       <c r="J43" s="45"/>
       <c r="K43" s="45"/>
       <c r="L43" s="45"/>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M43" s="45" t="s">
+        <v>456</v>
+      </c>
+      <c r="N43" s="45" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" s="43" t="s">
         <v>122</v>
       </c>
@@ -4195,8 +4440,14 @@
       <c r="J44" s="46"/>
       <c r="K44" s="46"/>
       <c r="L44" s="46"/>
-    </row>
-    <row r="45" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M44" s="46" t="s">
+        <v>456</v>
+      </c>
+      <c r="N44" s="46" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="111" t="s">
         <v>159</v>
       </c>
@@ -4223,8 +4474,14 @@
       <c r="J45" s="50"/>
       <c r="K45" s="50"/>
       <c r="L45" s="50"/>
-    </row>
-    <row r="46" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="M45" s="50" t="s">
+        <v>456</v>
+      </c>
+      <c r="N45" s="50" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A46" s="72">
         <v>20</v>
       </c>
@@ -4251,8 +4508,14 @@
       <c r="J46" s="34"/>
       <c r="K46" s="34"/>
       <c r="L46" s="34"/>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M46" s="34" t="s">
+        <v>456</v>
+      </c>
+      <c r="N46" s="34" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" s="72">
         <v>20.100000000000001</v>
       </c>
@@ -4279,8 +4542,14 @@
       <c r="J47" s="34"/>
       <c r="K47" s="34"/>
       <c r="L47" s="34"/>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M47" s="34" t="s">
+        <v>456</v>
+      </c>
+      <c r="N47" s="34" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48" s="72" t="s">
         <v>129</v>
       </c>
@@ -4307,8 +4576,14 @@
       <c r="J48" s="34"/>
       <c r="K48" s="34"/>
       <c r="L48" s="34"/>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M48" s="34" t="s">
+        <v>456</v>
+      </c>
+      <c r="N48" s="34" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49" s="72" t="s">
         <v>130</v>
       </c>
@@ -4335,8 +4610,14 @@
       <c r="J49" s="34"/>
       <c r="K49" s="34"/>
       <c r="L49" s="34"/>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M49" s="34" t="s">
+        <v>456</v>
+      </c>
+      <c r="N49" s="34" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50" s="72" t="s">
         <v>131</v>
       </c>
@@ -4363,8 +4644,14 @@
       <c r="J50" s="34"/>
       <c r="K50" s="34"/>
       <c r="L50" s="34"/>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M50" s="34" t="s">
+        <v>456</v>
+      </c>
+      <c r="N50" s="34" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51" s="72">
         <v>21</v>
       </c>
@@ -4391,8 +4678,14 @@
       <c r="J51" s="34"/>
       <c r="K51" s="34"/>
       <c r="L51" s="34"/>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M51" s="34" t="s">
+        <v>456</v>
+      </c>
+      <c r="N51" s="34" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52" s="72">
         <v>21.1</v>
       </c>
@@ -4419,8 +4712,14 @@
       <c r="J52" s="34"/>
       <c r="K52" s="34"/>
       <c r="L52" s="34"/>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M52" s="34" t="s">
+        <v>456</v>
+      </c>
+      <c r="N52" s="34" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53" s="72" t="s">
         <v>132</v>
       </c>
@@ -4447,8 +4746,14 @@
       <c r="J53" s="34"/>
       <c r="K53" s="34"/>
       <c r="L53" s="34"/>
-    </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M53" s="34" t="s">
+        <v>456</v>
+      </c>
+      <c r="N53" s="34" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A54" s="72" t="s">
         <v>133</v>
       </c>
@@ -4475,8 +4780,14 @@
       <c r="J54" s="34"/>
       <c r="K54" s="34"/>
       <c r="L54" s="34"/>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M54" s="34" t="s">
+        <v>456</v>
+      </c>
+      <c r="N54" s="34" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55" s="72" t="s">
         <v>178</v>
       </c>
@@ -4503,8 +4814,14 @@
       <c r="J55" s="34"/>
       <c r="K55" s="34"/>
       <c r="L55" s="34"/>
-    </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M55" s="34" t="s">
+        <v>456</v>
+      </c>
+      <c r="N55" s="34" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56" s="72">
         <v>22</v>
       </c>
@@ -4531,8 +4848,14 @@
       <c r="J56" s="34"/>
       <c r="K56" s="34"/>
       <c r="L56" s="34"/>
-    </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M56" s="34" t="s">
+        <v>456</v>
+      </c>
+      <c r="N56" s="34" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A57" s="72">
         <v>22.1</v>
       </c>
@@ -4559,8 +4882,14 @@
       <c r="J57" s="34"/>
       <c r="K57" s="34"/>
       <c r="L57" s="34"/>
-    </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M57" s="34" t="s">
+        <v>456</v>
+      </c>
+      <c r="N57" s="34" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A58" s="72" t="s">
         <v>134</v>
       </c>
@@ -4587,8 +4916,14 @@
       <c r="J58" s="34"/>
       <c r="K58" s="34"/>
       <c r="L58" s="34"/>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M58" s="34" t="s">
+        <v>456</v>
+      </c>
+      <c r="N58" s="34" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A59" s="72" t="s">
         <v>135</v>
       </c>
@@ -4615,8 +4950,14 @@
       <c r="J59" s="34"/>
       <c r="K59" s="34"/>
       <c r="L59" s="34"/>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M59" s="34" t="s">
+        <v>456</v>
+      </c>
+      <c r="N59" s="34" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A60" s="72">
         <v>23</v>
       </c>
@@ -4643,8 +4984,14 @@
       <c r="J60" s="34"/>
       <c r="K60" s="34"/>
       <c r="L60" s="34"/>
-    </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M60" s="34" t="s">
+        <v>456</v>
+      </c>
+      <c r="N60" s="34" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A61" s="72">
         <v>23.1</v>
       </c>
@@ -4671,8 +5018,14 @@
       <c r="J61" s="34"/>
       <c r="K61" s="34"/>
       <c r="L61" s="34"/>
-    </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M61" s="34" t="s">
+        <v>456</v>
+      </c>
+      <c r="N61" s="34" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A62" s="72" t="s">
         <v>136</v>
       </c>
@@ -4699,8 +5052,14 @@
       <c r="J62" s="34"/>
       <c r="K62" s="34"/>
       <c r="L62" s="34"/>
-    </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M62" s="34" t="s">
+        <v>456</v>
+      </c>
+      <c r="N62" s="34" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A63" s="72" t="s">
         <v>137</v>
       </c>
@@ -4727,8 +5086,14 @@
       <c r="J63" s="34"/>
       <c r="K63" s="34"/>
       <c r="L63" s="34"/>
-    </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M63" s="34" t="s">
+        <v>456</v>
+      </c>
+      <c r="N63" s="34" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A64" s="72">
         <v>24</v>
       </c>
@@ -4755,8 +5120,14 @@
       <c r="J64" s="34"/>
       <c r="K64" s="34"/>
       <c r="L64" s="34"/>
-    </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M64" s="34" t="s">
+        <v>456</v>
+      </c>
+      <c r="N64" s="34" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A65" s="72">
         <v>24.1</v>
       </c>
@@ -4783,8 +5154,14 @@
       <c r="J65" s="34"/>
       <c r="K65" s="34"/>
       <c r="L65" s="34"/>
-    </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M65" s="34" t="s">
+        <v>456</v>
+      </c>
+      <c r="N65" s="34" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A66" s="72" t="s">
         <v>138</v>
       </c>
@@ -4811,8 +5188,14 @@
       <c r="J66" s="34"/>
       <c r="K66" s="34"/>
       <c r="L66" s="34"/>
-    </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M66" s="34" t="s">
+        <v>456</v>
+      </c>
+      <c r="N66" s="34" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A67" s="72" t="s">
         <v>139</v>
       </c>
@@ -4839,8 +5222,14 @@
       <c r="J67" s="34"/>
       <c r="K67" s="34"/>
       <c r="L67" s="34"/>
-    </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M67" s="34" t="s">
+        <v>456</v>
+      </c>
+      <c r="N67" s="34" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A68" s="72">
         <v>25</v>
       </c>
@@ -4867,8 +5256,14 @@
       <c r="J68" s="34"/>
       <c r="K68" s="34"/>
       <c r="L68" s="34"/>
-    </row>
-    <row r="69" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M68" s="34" t="s">
+        <v>456</v>
+      </c>
+      <c r="N68" s="34" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="69" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="72">
         <v>25.1</v>
       </c>
@@ -4895,8 +5290,14 @@
       <c r="J69" s="34"/>
       <c r="K69" s="34"/>
       <c r="L69" s="34"/>
-    </row>
-    <row r="70" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M69" s="34" t="s">
+        <v>456</v>
+      </c>
+      <c r="N69" s="34" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="70" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="43" t="s">
         <v>140</v>
       </c>
@@ -4923,8 +5324,14 @@
       <c r="J70" s="34"/>
       <c r="K70" s="34"/>
       <c r="L70" s="34"/>
-    </row>
-    <row r="71" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M70" s="34" t="s">
+        <v>456</v>
+      </c>
+      <c r="N70" s="34" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="71" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="72" t="s">
         <v>141</v>
       </c>
@@ -4951,8 +5358,14 @@
       <c r="J71" s="34"/>
       <c r="K71" s="34"/>
       <c r="L71" s="34"/>
-    </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M71" s="34" t="s">
+        <v>456</v>
+      </c>
+      <c r="N71" s="34" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A72" s="72">
         <v>26</v>
       </c>
@@ -4979,8 +5392,14 @@
       <c r="J72" s="34"/>
       <c r="K72" s="34"/>
       <c r="L72" s="34"/>
-    </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M72" s="34" t="s">
+        <v>456</v>
+      </c>
+      <c r="N72" s="34" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A73" s="72">
         <v>26.1</v>
       </c>
@@ -5007,8 +5426,14 @@
       <c r="J73" s="34"/>
       <c r="K73" s="34"/>
       <c r="L73" s="34"/>
-    </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M73" s="34" t="s">
+        <v>456</v>
+      </c>
+      <c r="N73" s="34" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A74" s="43" t="s">
         <v>142</v>
       </c>
@@ -5035,8 +5460,14 @@
       <c r="J74" s="34"/>
       <c r="K74" s="34"/>
       <c r="L74" s="34"/>
-    </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M74" s="34" t="s">
+        <v>456</v>
+      </c>
+      <c r="N74" s="34" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A75" s="72" t="s">
         <v>143</v>
       </c>
@@ -5063,8 +5494,14 @@
       <c r="J75" s="34"/>
       <c r="K75" s="34"/>
       <c r="L75" s="34"/>
-    </row>
-    <row r="76" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M75" s="34" t="s">
+        <v>456</v>
+      </c>
+      <c r="N75" s="34" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="76" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A76" s="110" t="s">
         <v>144</v>
       </c>
@@ -5091,8 +5528,14 @@
       <c r="J76" s="41"/>
       <c r="K76" s="41"/>
       <c r="L76" s="41"/>
-    </row>
-    <row r="77" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M76" s="41" t="s">
+        <v>456</v>
+      </c>
+      <c r="N76" s="41" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="77" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="56">
         <v>65</v>
       </c>
@@ -5119,8 +5562,12 @@
       <c r="J77" s="34"/>
       <c r="K77" s="34"/>
       <c r="L77" s="34"/>
-    </row>
-    <row r="78" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M77" s="34" t="s">
+        <v>456</v>
+      </c>
+      <c r="N77" s="34"/>
+    </row>
+    <row r="78" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="56">
         <v>66</v>
       </c>
@@ -5147,8 +5594,12 @@
       <c r="J78" s="34"/>
       <c r="K78" s="34"/>
       <c r="L78" s="34"/>
-    </row>
-    <row r="79" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M78" s="34" t="s">
+        <v>456</v>
+      </c>
+      <c r="N78" s="34"/>
+    </row>
+    <row r="79" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="56">
         <v>67</v>
       </c>
@@ -5177,8 +5628,12 @@
       <c r="J79" s="34"/>
       <c r="K79" s="34"/>
       <c r="L79" s="34"/>
-    </row>
-    <row r="80" spans="1:12" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M79" s="34" t="s">
+        <v>456</v>
+      </c>
+      <c r="N79" s="34"/>
+    </row>
+    <row r="80" spans="1:14" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A80" s="112">
         <v>68</v>
       </c>
@@ -5207,8 +5662,12 @@
       <c r="J80" s="85"/>
       <c r="K80" s="85"/>
       <c r="L80" s="85"/>
-    </row>
-    <row r="81" spans="1:12" ht="14.45" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="M80" s="85" t="s">
+        <v>456</v>
+      </c>
+      <c r="N80" s="85"/>
+    </row>
+    <row r="81" spans="1:14" ht="14.45" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A81" s="56">
         <v>69</v>
       </c>
@@ -5235,8 +5694,14 @@
       <c r="J81" s="34"/>
       <c r="K81" s="34"/>
       <c r="L81" s="34"/>
-    </row>
-    <row r="82" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M81" s="34" t="s">
+        <v>456</v>
+      </c>
+      <c r="N81" s="34" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="82" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="56">
         <v>70</v>
       </c>
@@ -5263,8 +5728,14 @@
       <c r="J82" s="34"/>
       <c r="K82" s="34"/>
       <c r="L82" s="34"/>
-    </row>
-    <row r="83" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M82" s="34" t="s">
+        <v>456</v>
+      </c>
+      <c r="N82" s="34" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="83" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="56">
         <v>71</v>
       </c>
@@ -5291,8 +5762,14 @@
       <c r="J83" s="34"/>
       <c r="K83" s="34"/>
       <c r="L83" s="34"/>
-    </row>
-    <row r="84" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M83" s="34" t="s">
+        <v>456</v>
+      </c>
+      <c r="N83" s="34" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="84" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="56">
         <v>72</v>
       </c>
@@ -5319,8 +5796,14 @@
       <c r="J84" s="34"/>
       <c r="K84" s="34"/>
       <c r="L84" s="34"/>
-    </row>
-    <row r="85" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M84" s="34" t="s">
+        <v>456</v>
+      </c>
+      <c r="N84" s="34" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="85" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="56">
         <v>73</v>
       </c>
@@ -5347,8 +5830,14 @@
       <c r="J85" s="34"/>
       <c r="K85" s="34"/>
       <c r="L85" s="34"/>
-    </row>
-    <row r="86" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M85" s="34" t="s">
+        <v>456</v>
+      </c>
+      <c r="N85" s="34" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="86" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="56">
         <v>74</v>
       </c>
@@ -5375,8 +5864,14 @@
       <c r="J86" s="34"/>
       <c r="K86" s="34"/>
       <c r="L86" s="34"/>
-    </row>
-    <row r="87" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M86" s="34" t="s">
+        <v>456</v>
+      </c>
+      <c r="N86" s="34" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="87" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="56">
         <v>75</v>
       </c>
@@ -5403,8 +5898,14 @@
       <c r="J87" s="34"/>
       <c r="K87" s="34"/>
       <c r="L87" s="34"/>
-    </row>
-    <row r="88" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M87" s="34" t="s">
+        <v>456</v>
+      </c>
+      <c r="N87" s="34" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="88" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="56">
         <v>76</v>
       </c>
@@ -5431,8 +5932,14 @@
       <c r="J88" s="34"/>
       <c r="K88" s="34"/>
       <c r="L88" s="34"/>
-    </row>
-    <row r="89" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M88" s="34" t="s">
+        <v>456</v>
+      </c>
+      <c r="N88" s="34" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="89" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="56">
         <v>77</v>
       </c>
@@ -5459,8 +5966,14 @@
       <c r="J89" s="34"/>
       <c r="K89" s="34"/>
       <c r="L89" s="34"/>
-    </row>
-    <row r="90" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M89" s="34" t="s">
+        <v>456</v>
+      </c>
+      <c r="N89" s="34" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="90" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="56">
         <v>78</v>
       </c>
@@ -5487,8 +6000,14 @@
       <c r="J90" s="34"/>
       <c r="K90" s="34"/>
       <c r="L90" s="34"/>
-    </row>
-    <row r="91" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M90" s="34" t="s">
+        <v>456</v>
+      </c>
+      <c r="N90" s="34" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="91" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="56">
         <v>79</v>
       </c>
@@ -5515,8 +6034,14 @@
       <c r="J91" s="34"/>
       <c r="K91" s="34"/>
       <c r="L91" s="34"/>
-    </row>
-    <row r="92" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M91" s="34" t="s">
+        <v>456</v>
+      </c>
+      <c r="N91" s="34" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="92" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="56">
         <v>80</v>
       </c>
@@ -5543,8 +6068,14 @@
       <c r="J92" s="45"/>
       <c r="K92" s="45"/>
       <c r="L92" s="45"/>
-    </row>
-    <row r="93" spans="1:12" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M92" s="45" t="s">
+        <v>456</v>
+      </c>
+      <c r="N92" s="45" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="93" spans="1:14" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A93" s="52">
         <v>81</v>
       </c>
@@ -5571,8 +6102,14 @@
       <c r="J93" s="54"/>
       <c r="K93" s="54"/>
       <c r="L93" s="55"/>
-    </row>
-    <row r="94" spans="1:12" ht="14.45" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="M93" s="55" t="s">
+        <v>456</v>
+      </c>
+      <c r="N93" s="55" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="94" spans="1:14" ht="14.45" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A94" s="56">
         <v>82</v>
       </c>
@@ -5599,8 +6136,14 @@
       <c r="J94" s="57"/>
       <c r="K94" s="57"/>
       <c r="L94" s="57"/>
-    </row>
-    <row r="95" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M94" s="57" t="s">
+        <v>456</v>
+      </c>
+      <c r="N94" s="57" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="95" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="56">
         <v>83</v>
       </c>
@@ -5627,8 +6170,14 @@
       <c r="J95" s="58"/>
       <c r="K95" s="58"/>
       <c r="L95" s="58"/>
-    </row>
-    <row r="96" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M95" s="58" t="s">
+        <v>456</v>
+      </c>
+      <c r="N95" s="58" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="96" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="56">
         <v>84</v>
       </c>
@@ -5655,8 +6204,14 @@
       <c r="J96" s="58"/>
       <c r="K96" s="58"/>
       <c r="L96" s="58"/>
-    </row>
-    <row r="97" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M96" s="58" t="s">
+        <v>456</v>
+      </c>
+      <c r="N96" s="58" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="97" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="56">
         <v>85</v>
       </c>
@@ -5683,8 +6238,14 @@
       <c r="J97" s="58"/>
       <c r="K97" s="58"/>
       <c r="L97" s="58"/>
-    </row>
-    <row r="98" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M97" s="58" t="s">
+        <v>456</v>
+      </c>
+      <c r="N97" s="58" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="98" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="56">
         <v>86</v>
       </c>
@@ -5711,8 +6272,14 @@
       <c r="J98" s="58"/>
       <c r="K98" s="58"/>
       <c r="L98" s="58"/>
-    </row>
-    <row r="99" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M98" s="58" t="s">
+        <v>456</v>
+      </c>
+      <c r="N98" s="58" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="99" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="56">
         <v>87</v>
       </c>
@@ -5739,8 +6306,14 @@
       <c r="J99" s="58"/>
       <c r="K99" s="58"/>
       <c r="L99" s="58"/>
-    </row>
-    <row r="100" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M99" s="58" t="s">
+        <v>456</v>
+      </c>
+      <c r="N99" s="58" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="100" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="56">
         <v>88</v>
       </c>
@@ -5767,8 +6340,14 @@
       <c r="J100" s="58"/>
       <c r="K100" s="58"/>
       <c r="L100" s="58"/>
-    </row>
-    <row r="101" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M100" s="58" t="s">
+        <v>456</v>
+      </c>
+      <c r="N100" s="58" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="101" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="56">
         <v>89</v>
       </c>
@@ -5795,8 +6374,14 @@
       <c r="J101" s="58"/>
       <c r="K101" s="58"/>
       <c r="L101" s="58"/>
-    </row>
-    <row r="102" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M101" s="58" t="s">
+        <v>456</v>
+      </c>
+      <c r="N101" s="58" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="102" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="56">
         <v>90</v>
       </c>
@@ -5823,8 +6408,14 @@
       <c r="J102" s="58"/>
       <c r="K102" s="58"/>
       <c r="L102" s="58"/>
-    </row>
-    <row r="103" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M102" s="58" t="s">
+        <v>456</v>
+      </c>
+      <c r="N102" s="58" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="103" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="56">
         <v>91</v>
       </c>
@@ -5851,8 +6442,14 @@
       <c r="J103" s="58"/>
       <c r="K103" s="58"/>
       <c r="L103" s="58"/>
-    </row>
-    <row r="104" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M103" s="58" t="s">
+        <v>456</v>
+      </c>
+      <c r="N103" s="58" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="104" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="56">
         <v>92</v>
       </c>
@@ -5879,8 +6476,14 @@
       <c r="J104" s="58"/>
       <c r="K104" s="58"/>
       <c r="L104" s="58"/>
-    </row>
-    <row r="105" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M104" s="58" t="s">
+        <v>456</v>
+      </c>
+      <c r="N104" s="58" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="105" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="56">
         <v>93</v>
       </c>
@@ -5907,8 +6510,14 @@
       <c r="J105" s="58"/>
       <c r="K105" s="58"/>
       <c r="L105" s="58"/>
-    </row>
-    <row r="106" spans="1:12" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M105" s="58" t="s">
+        <v>456</v>
+      </c>
+      <c r="N105" s="58" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="106" spans="1:14" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A106" s="59">
         <v>94</v>
       </c>
@@ -5935,8 +6544,14 @@
       <c r="J106" s="60"/>
       <c r="K106" s="60"/>
       <c r="L106" s="60"/>
-    </row>
-    <row r="107" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M106" s="60" t="s">
+        <v>456</v>
+      </c>
+      <c r="N106" s="60" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="107" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="77">
         <v>95</v>
       </c>
@@ -5965,8 +6580,12 @@
       <c r="J107" s="79"/>
       <c r="K107" s="79"/>
       <c r="L107" s="79"/>
-    </row>
-    <row r="108" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M107" s="79" t="s">
+        <v>456</v>
+      </c>
+      <c r="N107" s="79"/>
+    </row>
+    <row r="108" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="75">
         <v>96</v>
       </c>
@@ -5995,8 +6614,12 @@
       <c r="J108" s="62"/>
       <c r="K108" s="62"/>
       <c r="L108" s="62"/>
-    </row>
-    <row r="109" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M108" s="62" t="s">
+        <v>456</v>
+      </c>
+      <c r="N108" s="62"/>
+    </row>
+    <row r="109" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="75">
         <v>97</v>
       </c>
@@ -6025,8 +6648,12 @@
       <c r="J109" s="62"/>
       <c r="K109" s="62"/>
       <c r="L109" s="62"/>
-    </row>
-    <row r="110" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M109" s="62" t="s">
+        <v>456</v>
+      </c>
+      <c r="N109" s="62"/>
+    </row>
+    <row r="110" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="75">
         <v>98</v>
       </c>
@@ -6053,8 +6680,12 @@
       <c r="J110" s="62"/>
       <c r="K110" s="62"/>
       <c r="L110" s="62"/>
-    </row>
-    <row r="111" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M110" s="62" t="s">
+        <v>456</v>
+      </c>
+      <c r="N110" s="62"/>
+    </row>
+    <row r="111" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="75">
         <v>99</v>
       </c>
@@ -6081,8 +6712,12 @@
       <c r="J111" s="62"/>
       <c r="K111" s="62"/>
       <c r="L111" s="62"/>
-    </row>
-    <row r="112" spans="1:12" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M111" s="62" t="s">
+        <v>456</v>
+      </c>
+      <c r="N111" s="62"/>
+    </row>
+    <row r="112" spans="1:14" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A112" s="52">
         <v>100</v>
       </c>
@@ -6109,8 +6744,12 @@
       <c r="J112" s="81"/>
       <c r="K112" s="81"/>
       <c r="L112" s="81"/>
-    </row>
-    <row r="113" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="M112" s="81" t="s">
+        <v>456</v>
+      </c>
+      <c r="N112" s="81"/>
+    </row>
+    <row r="113" spans="1:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A113" s="75">
         <v>101</v>
       </c>
@@ -6137,8 +6776,12 @@
       <c r="J113" s="34"/>
       <c r="K113" s="34"/>
       <c r="L113" s="34"/>
-    </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M113" s="34" t="s">
+        <v>456</v>
+      </c>
+      <c r="N113" s="34"/>
+    </row>
+    <row r="114" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A114" s="75">
         <v>102</v>
       </c>
@@ -6165,8 +6808,12 @@
       <c r="J114" s="34"/>
       <c r="K114" s="34"/>
       <c r="L114" s="34"/>
-    </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M114" s="34" t="s">
+        <v>456</v>
+      </c>
+      <c r="N114" s="34"/>
+    </row>
+    <row r="115" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A115" s="75">
         <v>103</v>
       </c>
@@ -6195,8 +6842,12 @@
       <c r="J115" s="34"/>
       <c r="K115" s="34"/>
       <c r="L115" s="34"/>
-    </row>
-    <row r="116" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M115" s="34" t="s">
+        <v>456</v>
+      </c>
+      <c r="N115" s="34"/>
+    </row>
+    <row r="116" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A116" s="52">
         <v>104</v>
       </c>
@@ -6225,8 +6876,12 @@
       <c r="J116" s="85"/>
       <c r="K116" s="85"/>
       <c r="L116" s="85"/>
-    </row>
-    <row r="117" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="M116" s="85" t="s">
+        <v>456</v>
+      </c>
+      <c r="N116" s="85"/>
+    </row>
+    <row r="117" spans="1:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A117" s="61">
         <v>105</v>
       </c>
@@ -6253,8 +6908,14 @@
       <c r="J117" s="62"/>
       <c r="K117" s="62"/>
       <c r="L117" s="62"/>
-    </row>
-    <row r="118" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M117" s="62" t="s">
+        <v>456</v>
+      </c>
+      <c r="N117" s="62" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="118" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A118" s="61">
         <v>106</v>
       </c>
@@ -6281,8 +6942,14 @@
       <c r="J118" s="63"/>
       <c r="K118" s="63"/>
       <c r="L118" s="63"/>
-    </row>
-    <row r="119" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M118" s="63" t="s">
+        <v>456</v>
+      </c>
+      <c r="N118" s="63" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="119" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A119" s="61">
         <v>107</v>
       </c>
@@ -6309,8 +6976,14 @@
       <c r="J119" s="63"/>
       <c r="K119" s="63"/>
       <c r="L119" s="63"/>
-    </row>
-    <row r="120" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M119" s="63" t="s">
+        <v>456</v>
+      </c>
+      <c r="N119" s="63" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="120" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A120" s="61">
         <v>108</v>
       </c>
@@ -6337,8 +7010,14 @@
       <c r="J120" s="63"/>
       <c r="K120" s="63"/>
       <c r="L120" s="63"/>
-    </row>
-    <row r="121" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M120" s="63" t="s">
+        <v>456</v>
+      </c>
+      <c r="N120" s="63" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="121" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A121" s="61">
         <v>109</v>
       </c>
@@ -6365,8 +7044,14 @@
       <c r="J121" s="63"/>
       <c r="K121" s="63"/>
       <c r="L121" s="63"/>
-    </row>
-    <row r="122" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M121" s="63" t="s">
+        <v>456</v>
+      </c>
+      <c r="N121" s="63" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="122" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A122" s="61">
         <v>110</v>
       </c>
@@ -6393,8 +7078,14 @@
       <c r="J122" s="63"/>
       <c r="K122" s="63"/>
       <c r="L122" s="63"/>
-    </row>
-    <row r="123" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M122" s="63" t="s">
+        <v>456</v>
+      </c>
+      <c r="N122" s="63" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="123" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A123" s="61">
         <v>111</v>
       </c>
@@ -6421,8 +7112,14 @@
       <c r="J123" s="63"/>
       <c r="K123" s="63"/>
       <c r="L123" s="63"/>
-    </row>
-    <row r="124" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M123" s="63" t="s">
+        <v>456</v>
+      </c>
+      <c r="N123" s="63" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="124" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A124" s="61">
         <v>112</v>
       </c>
@@ -6449,8 +7146,14 @@
       <c r="J124" s="63"/>
       <c r="K124" s="63"/>
       <c r="L124" s="63"/>
-    </row>
-    <row r="125" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M124" s="63" t="s">
+        <v>456</v>
+      </c>
+      <c r="N124" s="63" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="125" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A125" s="61">
         <v>113</v>
       </c>
@@ -6477,8 +7180,14 @@
       <c r="J125" s="63"/>
       <c r="K125" s="63"/>
       <c r="L125" s="63"/>
-    </row>
-    <row r="126" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M125" s="63" t="s">
+        <v>456</v>
+      </c>
+      <c r="N125" s="63" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="126" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A126" s="61">
         <v>114</v>
       </c>
@@ -6505,8 +7214,14 @@
       <c r="J126" s="63"/>
       <c r="K126" s="63"/>
       <c r="L126" s="63"/>
-    </row>
-    <row r="127" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M126" s="63" t="s">
+        <v>456</v>
+      </c>
+      <c r="N126" s="63" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="127" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A127" s="61">
         <v>115</v>
       </c>
@@ -6533,8 +7248,14 @@
       <c r="J127" s="63"/>
       <c r="K127" s="63"/>
       <c r="L127" s="63"/>
-    </row>
-    <row r="128" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M127" s="63" t="s">
+        <v>456</v>
+      </c>
+      <c r="N127" s="63" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="128" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A128" s="61">
         <v>116</v>
       </c>
@@ -6561,8 +7282,14 @@
       <c r="J128" s="63"/>
       <c r="K128" s="63"/>
       <c r="L128" s="63"/>
-    </row>
-    <row r="129" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M128" s="63" t="s">
+        <v>456</v>
+      </c>
+      <c r="N128" s="63" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="129" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A129" s="52">
         <v>117</v>
       </c>
@@ -6589,8 +7316,14 @@
       <c r="J129" s="64"/>
       <c r="K129" s="64"/>
       <c r="L129" s="64"/>
-    </row>
-    <row r="130" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="M129" s="64" t="s">
+        <v>456</v>
+      </c>
+      <c r="N129" s="64" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="130" spans="1:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A130" s="61">
         <v>118</v>
       </c>
@@ -6617,8 +7350,14 @@
       <c r="J130" s="62"/>
       <c r="K130" s="62"/>
       <c r="L130" s="62"/>
-    </row>
-    <row r="131" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M130" s="62" t="s">
+        <v>456</v>
+      </c>
+      <c r="N130" s="62" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="131" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A131" s="61">
         <v>119</v>
       </c>
@@ -6645,8 +7384,14 @@
       <c r="J131" s="63"/>
       <c r="K131" s="63"/>
       <c r="L131" s="63"/>
-    </row>
-    <row r="132" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M131" s="63" t="s">
+        <v>456</v>
+      </c>
+      <c r="N131" s="63" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="132" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A132" s="61">
         <v>120</v>
       </c>
@@ -6673,8 +7418,14 @@
       <c r="J132" s="63"/>
       <c r="K132" s="63"/>
       <c r="L132" s="63"/>
-    </row>
-    <row r="133" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M132" s="63" t="s">
+        <v>456</v>
+      </c>
+      <c r="N132" s="63" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="133" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A133" s="61">
         <v>121</v>
       </c>
@@ -6701,8 +7452,14 @@
       <c r="J133" s="63"/>
       <c r="K133" s="63"/>
       <c r="L133" s="63"/>
-    </row>
-    <row r="134" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M133" s="63" t="s">
+        <v>456</v>
+      </c>
+      <c r="N133" s="63" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="134" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A134" s="61">
         <v>122</v>
       </c>
@@ -6729,8 +7486,14 @@
       <c r="J134" s="63"/>
       <c r="K134" s="63"/>
       <c r="L134" s="63"/>
-    </row>
-    <row r="135" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M134" s="63" t="s">
+        <v>456</v>
+      </c>
+      <c r="N134" s="63" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="135" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A135" s="61">
         <v>123</v>
       </c>
@@ -6757,8 +7520,14 @@
       <c r="J135" s="63"/>
       <c r="K135" s="63"/>
       <c r="L135" s="63"/>
-    </row>
-    <row r="136" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M135" s="63" t="s">
+        <v>456</v>
+      </c>
+      <c r="N135" s="63" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="136" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A136" s="61">
         <v>124</v>
       </c>
@@ -6785,8 +7554,14 @@
       <c r="J136" s="63"/>
       <c r="K136" s="63"/>
       <c r="L136" s="63"/>
-    </row>
-    <row r="137" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M136" s="63" t="s">
+        <v>456</v>
+      </c>
+      <c r="N136" s="63" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="137" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A137" s="61">
         <v>125</v>
       </c>
@@ -6813,8 +7588,14 @@
       <c r="J137" s="63"/>
       <c r="K137" s="63"/>
       <c r="L137" s="63"/>
-    </row>
-    <row r="138" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M137" s="63" t="s">
+        <v>456</v>
+      </c>
+      <c r="N137" s="63" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="138" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A138" s="61">
         <v>126</v>
       </c>
@@ -6841,8 +7622,14 @@
       <c r="J138" s="63"/>
       <c r="K138" s="63"/>
       <c r="L138" s="63"/>
-    </row>
-    <row r="139" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M138" s="63" t="s">
+        <v>456</v>
+      </c>
+      <c r="N138" s="63" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="139" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A139" s="61">
         <v>127</v>
       </c>
@@ -6869,8 +7656,14 @@
       <c r="J139" s="63"/>
       <c r="K139" s="63"/>
       <c r="L139" s="63"/>
-    </row>
-    <row r="140" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M139" s="63" t="s">
+        <v>456</v>
+      </c>
+      <c r="N139" s="63" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="140" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A140" s="61">
         <v>128</v>
       </c>
@@ -6897,8 +7690,14 @@
       <c r="J140" s="63"/>
       <c r="K140" s="63"/>
       <c r="L140" s="63"/>
-    </row>
-    <row r="141" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M140" s="63" t="s">
+        <v>456</v>
+      </c>
+      <c r="N140" s="63" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="141" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A141" s="61">
         <v>129</v>
       </c>
@@ -6925,8 +7724,14 @@
       <c r="J141" s="63"/>
       <c r="K141" s="63"/>
       <c r="L141" s="63"/>
-    </row>
-    <row r="142" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M141" s="63" t="s">
+        <v>456</v>
+      </c>
+      <c r="N141" s="63" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="142" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A142" s="59">
         <v>130</v>
       </c>
@@ -6953,8 +7758,14 @@
       <c r="J142" s="65"/>
       <c r="K142" s="65"/>
       <c r="L142" s="65"/>
-    </row>
-    <row r="143" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M142" s="65" t="s">
+        <v>456</v>
+      </c>
+      <c r="N142" s="65" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="143" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" s="113">
         <v>131</v>
       </c>
@@ -6983,8 +7794,14 @@
       <c r="J143" s="66"/>
       <c r="K143" s="66"/>
       <c r="L143" s="66"/>
-    </row>
-    <row r="144" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M143" s="66" t="s">
+        <v>456</v>
+      </c>
+      <c r="N143" s="66" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="144" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" s="113">
         <v>132</v>
       </c>
@@ -7011,8 +7828,14 @@
       <c r="J144" s="66"/>
       <c r="K144" s="66"/>
       <c r="L144" s="66"/>
-    </row>
-    <row r="145" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M144" s="66" t="s">
+        <v>456</v>
+      </c>
+      <c r="N144" s="66" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="145" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A145" s="113">
         <v>133</v>
       </c>
@@ -7039,8 +7862,14 @@
       <c r="J145" s="66"/>
       <c r="K145" s="66"/>
       <c r="L145" s="66"/>
-    </row>
-    <row r="146" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M145" s="66" t="s">
+        <v>456</v>
+      </c>
+      <c r="N145" s="66" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="146" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A146" s="113">
         <v>134</v>
       </c>
@@ -7067,8 +7896,14 @@
       <c r="J146" s="66"/>
       <c r="K146" s="66"/>
       <c r="L146" s="66"/>
-    </row>
-    <row r="147" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M146" s="66" t="s">
+        <v>456</v>
+      </c>
+      <c r="N146" s="66" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="147" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A147" s="113">
         <v>135</v>
       </c>
@@ -7095,8 +7930,14 @@
       <c r="J147" s="66"/>
       <c r="K147" s="66"/>
       <c r="L147" s="66"/>
-    </row>
-    <row r="148" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M147" s="66" t="s">
+        <v>456</v>
+      </c>
+      <c r="N147" s="66" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="148" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A148" s="113">
         <v>136</v>
       </c>
@@ -7123,8 +7964,14 @@
       <c r="J148" s="66"/>
       <c r="K148" s="66"/>
       <c r="L148" s="66"/>
-    </row>
-    <row r="149" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M148" s="66" t="s">
+        <v>456</v>
+      </c>
+      <c r="N148" s="66" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="149" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A149" s="113">
         <v>137</v>
       </c>
@@ -7151,8 +7998,14 @@
       <c r="J149" s="66"/>
       <c r="K149" s="66"/>
       <c r="L149" s="66"/>
-    </row>
-    <row r="150" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M149" s="66" t="s">
+        <v>456</v>
+      </c>
+      <c r="N149" s="66" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="150" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A150" s="113">
         <v>138</v>
       </c>
@@ -7179,8 +8032,14 @@
       <c r="J150" s="66"/>
       <c r="K150" s="66"/>
       <c r="L150" s="66"/>
-    </row>
-    <row r="151" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M150" s="66" t="s">
+        <v>456</v>
+      </c>
+      <c r="N150" s="66" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="151" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A151" s="113">
         <v>139</v>
       </c>
@@ -7207,8 +8066,14 @@
       <c r="J151" s="66"/>
       <c r="K151" s="66"/>
       <c r="L151" s="66"/>
-    </row>
-    <row r="152" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M151" s="66" t="s">
+        <v>456</v>
+      </c>
+      <c r="N151" s="66" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="152" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A152" s="113">
         <v>140</v>
       </c>
@@ -7235,8 +8100,14 @@
       <c r="J152" s="66"/>
       <c r="K152" s="66"/>
       <c r="L152" s="66"/>
-    </row>
-    <row r="153" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M152" s="66" t="s">
+        <v>456</v>
+      </c>
+      <c r="N152" s="66" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="153" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A153" s="113">
         <v>141</v>
       </c>
@@ -7263,8 +8134,14 @@
       <c r="J153" s="66"/>
       <c r="K153" s="66"/>
       <c r="L153" s="66"/>
-    </row>
-    <row r="154" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M153" s="66" t="s">
+        <v>456</v>
+      </c>
+      <c r="N153" s="66" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="154" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A154" s="113">
         <v>142</v>
       </c>
@@ -7291,8 +8168,14 @@
       <c r="J154" s="66"/>
       <c r="K154" s="66"/>
       <c r="L154" s="66"/>
-    </row>
-    <row r="155" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M154" s="66" t="s">
+        <v>456</v>
+      </c>
+      <c r="N154" s="66" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="155" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A155" s="113">
         <v>143</v>
       </c>
@@ -7319,8 +8202,14 @@
       <c r="J155" s="66"/>
       <c r="K155" s="66"/>
       <c r="L155" s="66"/>
-    </row>
-    <row r="156" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M155" s="66" t="s">
+        <v>456</v>
+      </c>
+      <c r="N155" s="66" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="156" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A156" s="113">
         <v>144</v>
       </c>
@@ -7347,8 +8236,14 @@
       <c r="J156" s="66"/>
       <c r="K156" s="66"/>
       <c r="L156" s="66"/>
-    </row>
-    <row r="157" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M156" s="66" t="s">
+        <v>456</v>
+      </c>
+      <c r="N156" s="66" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="157" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A157" s="113">
         <v>145</v>
       </c>
@@ -7375,8 +8270,14 @@
       <c r="J157" s="66"/>
       <c r="K157" s="66"/>
       <c r="L157" s="66"/>
-    </row>
-    <row r="158" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M157" s="66" t="s">
+        <v>456</v>
+      </c>
+      <c r="N157" s="66" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="158" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A158" s="113">
         <v>146</v>
       </c>
@@ -7403,8 +8304,14 @@
       <c r="J158" s="66"/>
       <c r="K158" s="66"/>
       <c r="L158" s="66"/>
-    </row>
-    <row r="159" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M158" s="66" t="s">
+        <v>456</v>
+      </c>
+      <c r="N158" s="66" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="159" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A159" s="113">
         <v>147</v>
       </c>
@@ -7431,8 +8338,14 @@
       <c r="J159" s="66"/>
       <c r="K159" s="66"/>
       <c r="L159" s="66"/>
-    </row>
-    <row r="160" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M159" s="66" t="s">
+        <v>456</v>
+      </c>
+      <c r="N159" s="66" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="160" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A160" s="113">
         <v>148</v>
       </c>
@@ -7459,8 +8372,14 @@
       <c r="J160" s="66"/>
       <c r="K160" s="66"/>
       <c r="L160" s="66"/>
-    </row>
-    <row r="161" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M160" s="66" t="s">
+        <v>456</v>
+      </c>
+      <c r="N160" s="66" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="161" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A161" s="113">
         <v>149</v>
       </c>
@@ -7487,8 +8406,14 @@
       <c r="J161" s="66"/>
       <c r="K161" s="66"/>
       <c r="L161" s="66"/>
-    </row>
-    <row r="162" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M161" s="66" t="s">
+        <v>456</v>
+      </c>
+      <c r="N161" s="66" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="162" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A162" s="113">
         <v>150</v>
       </c>
@@ -7515,8 +8440,14 @@
       <c r="J162" s="66"/>
       <c r="K162" s="66"/>
       <c r="L162" s="66"/>
-    </row>
-    <row r="163" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M162" s="66" t="s">
+        <v>456</v>
+      </c>
+      <c r="N162" s="66" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="163" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A163" s="113">
         <v>151</v>
       </c>
@@ -7543,8 +8474,14 @@
       <c r="J163" s="66"/>
       <c r="K163" s="66"/>
       <c r="L163" s="66"/>
-    </row>
-    <row r="164" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M163" s="66" t="s">
+        <v>456</v>
+      </c>
+      <c r="N163" s="66" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="164" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A164" s="113">
         <v>152</v>
       </c>
@@ -7571,8 +8508,14 @@
       <c r="J164" s="66"/>
       <c r="K164" s="66"/>
       <c r="L164" s="66"/>
-    </row>
-    <row r="165" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M164" s="66" t="s">
+        <v>456</v>
+      </c>
+      <c r="N164" s="66" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="165" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A165" s="113">
         <v>153</v>
       </c>
@@ -7599,8 +8542,14 @@
       <c r="J165" s="66"/>
       <c r="K165" s="66"/>
       <c r="L165" s="66"/>
-    </row>
-    <row r="166" spans="1:12" s="83" customFormat="1" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M165" s="66" t="s">
+        <v>456</v>
+      </c>
+      <c r="N165" s="66" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="166" spans="1:14" s="83" customFormat="1" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A166" s="114">
         <v>154</v>
       </c>
@@ -7627,8 +8576,14 @@
       <c r="J166" s="68"/>
       <c r="K166" s="68"/>
       <c r="L166" s="68"/>
-    </row>
-    <row r="167" spans="1:12" ht="14.45" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="M166" s="68" t="s">
+        <v>456</v>
+      </c>
+      <c r="N166" s="68" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="167" spans="1:14" ht="14.45" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A167" s="113">
         <v>155</v>
       </c>
@@ -7657,8 +8612,14 @@
       <c r="J167" s="66"/>
       <c r="K167" s="66"/>
       <c r="L167" s="66"/>
-    </row>
-    <row r="168" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M167" s="66" t="s">
+        <v>456</v>
+      </c>
+      <c r="N167" s="66" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="168" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A168" s="113">
         <v>156</v>
       </c>
@@ -7685,8 +8646,14 @@
       <c r="J168" s="66"/>
       <c r="K168" s="66"/>
       <c r="L168" s="66"/>
-    </row>
-    <row r="169" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M168" s="66" t="s">
+        <v>456</v>
+      </c>
+      <c r="N168" s="66" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="169" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A169" s="113">
         <v>157</v>
       </c>
@@ -7713,8 +8680,14 @@
       <c r="J169" s="66"/>
       <c r="K169" s="66"/>
       <c r="L169" s="66"/>
-    </row>
-    <row r="170" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M169" s="66" t="s">
+        <v>456</v>
+      </c>
+      <c r="N169" s="66" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="170" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A170" s="113">
         <v>158</v>
       </c>
@@ -7741,8 +8714,14 @@
       <c r="J170" s="66"/>
       <c r="K170" s="66"/>
       <c r="L170" s="66"/>
-    </row>
-    <row r="171" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M170" s="66" t="s">
+        <v>456</v>
+      </c>
+      <c r="N170" s="66" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="171" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A171" s="113">
         <v>159</v>
       </c>
@@ -7769,8 +8748,14 @@
       <c r="J171" s="66"/>
       <c r="K171" s="66"/>
       <c r="L171" s="66"/>
-    </row>
-    <row r="172" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M171" s="66" t="s">
+        <v>456</v>
+      </c>
+      <c r="N171" s="66" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="172" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A172" s="113">
         <v>160</v>
       </c>
@@ -7797,8 +8782,14 @@
       <c r="J172" s="66"/>
       <c r="K172" s="66"/>
       <c r="L172" s="66"/>
-    </row>
-    <row r="173" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M172" s="66" t="s">
+        <v>456</v>
+      </c>
+      <c r="N172" s="66" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="173" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A173" s="113">
         <v>161</v>
       </c>
@@ -7825,8 +8816,14 @@
       <c r="J173" s="66"/>
       <c r="K173" s="66"/>
       <c r="L173" s="66"/>
-    </row>
-    <row r="174" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M173" s="66" t="s">
+        <v>456</v>
+      </c>
+      <c r="N173" s="66" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="174" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A174" s="113">
         <v>162</v>
       </c>
@@ -7853,8 +8850,14 @@
       <c r="J174" s="66"/>
       <c r="K174" s="66"/>
       <c r="L174" s="66"/>
-    </row>
-    <row r="175" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M174" s="66" t="s">
+        <v>456</v>
+      </c>
+      <c r="N174" s="66" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="175" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A175" s="113">
         <v>163</v>
       </c>
@@ -7881,8 +8884,14 @@
       <c r="J175" s="66"/>
       <c r="K175" s="66"/>
       <c r="L175" s="66"/>
-    </row>
-    <row r="176" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M175" s="66" t="s">
+        <v>456</v>
+      </c>
+      <c r="N175" s="66" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="176" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A176" s="113">
         <v>164</v>
       </c>
@@ -7909,8 +8918,14 @@
       <c r="J176" s="66"/>
       <c r="K176" s="66"/>
       <c r="L176" s="66"/>
-    </row>
-    <row r="177" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M176" s="66" t="s">
+        <v>456</v>
+      </c>
+      <c r="N176" s="66" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="177" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A177" s="113">
         <v>165</v>
       </c>
@@ -7937,8 +8952,14 @@
       <c r="J177" s="66"/>
       <c r="K177" s="66"/>
       <c r="L177" s="66"/>
-    </row>
-    <row r="178" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M177" s="66" t="s">
+        <v>456</v>
+      </c>
+      <c r="N177" s="66" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="178" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A178" s="113">
         <v>166</v>
       </c>
@@ -7965,8 +8986,14 @@
       <c r="J178" s="66"/>
       <c r="K178" s="66"/>
       <c r="L178" s="66"/>
-    </row>
-    <row r="179" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M178" s="66" t="s">
+        <v>456</v>
+      </c>
+      <c r="N178" s="66" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="179" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A179" s="113">
         <v>167</v>
       </c>
@@ -7993,8 +9020,14 @@
       <c r="J179" s="66"/>
       <c r="K179" s="66"/>
       <c r="L179" s="66"/>
-    </row>
-    <row r="180" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M179" s="66" t="s">
+        <v>456</v>
+      </c>
+      <c r="N179" s="66" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="180" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A180" s="113">
         <v>168</v>
       </c>
@@ -8021,8 +9054,14 @@
       <c r="J180" s="66"/>
       <c r="K180" s="66"/>
       <c r="L180" s="66"/>
-    </row>
-    <row r="181" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M180" s="66" t="s">
+        <v>456</v>
+      </c>
+      <c r="N180" s="66" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="181" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A181" s="113">
         <v>169</v>
       </c>
@@ -8049,8 +9088,14 @@
       <c r="J181" s="66"/>
       <c r="K181" s="66"/>
       <c r="L181" s="66"/>
-    </row>
-    <row r="182" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M181" s="66" t="s">
+        <v>456</v>
+      </c>
+      <c r="N181" s="66" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="182" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A182" s="113">
         <v>170</v>
       </c>
@@ -8077,8 +9122,14 @@
       <c r="J182" s="66"/>
       <c r="K182" s="66"/>
       <c r="L182" s="66"/>
-    </row>
-    <row r="183" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M182" s="66" t="s">
+        <v>456</v>
+      </c>
+      <c r="N182" s="66" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="183" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A183" s="113">
         <v>171</v>
       </c>
@@ -8105,8 +9156,14 @@
       <c r="J183" s="66"/>
       <c r="K183" s="66"/>
       <c r="L183" s="66"/>
-    </row>
-    <row r="184" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M183" s="66" t="s">
+        <v>456</v>
+      </c>
+      <c r="N183" s="66" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="184" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A184" s="113">
         <v>172</v>
       </c>
@@ -8133,8 +9190,14 @@
       <c r="J184" s="66"/>
       <c r="K184" s="66"/>
       <c r="L184" s="66"/>
-    </row>
-    <row r="185" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M184" s="66" t="s">
+        <v>456</v>
+      </c>
+      <c r="N184" s="66" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="185" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A185" s="113">
         <v>173</v>
       </c>
@@ -8161,8 +9224,14 @@
       <c r="J185" s="66"/>
       <c r="K185" s="66"/>
       <c r="L185" s="66"/>
-    </row>
-    <row r="186" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M185" s="66" t="s">
+        <v>456</v>
+      </c>
+      <c r="N185" s="66" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="186" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A186" s="113">
         <v>174</v>
       </c>
@@ -8189,8 +9258,14 @@
       <c r="J186" s="66"/>
       <c r="K186" s="66"/>
       <c r="L186" s="66"/>
-    </row>
-    <row r="187" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M186" s="66" t="s">
+        <v>456</v>
+      </c>
+      <c r="N186" s="66" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="187" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A187" s="113">
         <v>175</v>
       </c>
@@ -8217,8 +9292,14 @@
       <c r="J187" s="66"/>
       <c r="K187" s="66"/>
       <c r="L187" s="66"/>
-    </row>
-    <row r="188" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M187" s="66" t="s">
+        <v>456</v>
+      </c>
+      <c r="N187" s="66" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="188" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A188" s="113">
         <v>176</v>
       </c>
@@ -8245,8 +9326,14 @@
       <c r="J188" s="66"/>
       <c r="K188" s="66"/>
       <c r="L188" s="66"/>
-    </row>
-    <row r="189" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M188" s="66" t="s">
+        <v>456</v>
+      </c>
+      <c r="N188" s="66" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="189" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A189" s="113">
         <v>177</v>
       </c>
@@ -8273,8 +9360,14 @@
       <c r="J189" s="66"/>
       <c r="K189" s="66"/>
       <c r="L189" s="66"/>
-    </row>
-    <row r="190" spans="1:12" s="83" customFormat="1" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M189" s="66" t="s">
+        <v>456</v>
+      </c>
+      <c r="N189" s="66" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="190" spans="1:14" s="83" customFormat="1" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A190" s="114">
         <v>178</v>
       </c>
@@ -8301,8 +9394,14 @@
       <c r="J190" s="68"/>
       <c r="K190" s="68"/>
       <c r="L190" s="68"/>
-    </row>
-    <row r="191" spans="1:12" ht="14.45" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="M190" s="68" t="s">
+        <v>456</v>
+      </c>
+      <c r="N190" s="68" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="191" spans="1:14" ht="14.45" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A191" s="113">
         <v>179</v>
       </c>
@@ -8331,8 +9430,14 @@
       <c r="J191" s="66"/>
       <c r="K191" s="66"/>
       <c r="L191" s="66"/>
-    </row>
-    <row r="192" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M191" s="66" t="s">
+        <v>456</v>
+      </c>
+      <c r="N191" s="66" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="192" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A192" s="113">
         <v>180</v>
       </c>
@@ -8359,8 +9464,14 @@
       <c r="J192" s="66"/>
       <c r="K192" s="66"/>
       <c r="L192" s="66"/>
-    </row>
-    <row r="193" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M192" s="66" t="s">
+        <v>456</v>
+      </c>
+      <c r="N192" s="66" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="193" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A193" s="113">
         <v>181</v>
       </c>
@@ -8387,8 +9498,14 @@
       <c r="J193" s="66"/>
       <c r="K193" s="66"/>
       <c r="L193" s="66"/>
-    </row>
-    <row r="194" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M193" s="66" t="s">
+        <v>456</v>
+      </c>
+      <c r="N193" s="66" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="194" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A194" s="113">
         <v>182</v>
       </c>
@@ -8415,8 +9532,14 @@
       <c r="J194" s="66"/>
       <c r="K194" s="66"/>
       <c r="L194" s="66"/>
-    </row>
-    <row r="195" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M194" s="66" t="s">
+        <v>456</v>
+      </c>
+      <c r="N194" s="66" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="195" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A195" s="113">
         <v>183</v>
       </c>
@@ -8443,8 +9566,14 @@
       <c r="J195" s="66"/>
       <c r="K195" s="66"/>
       <c r="L195" s="66"/>
-    </row>
-    <row r="196" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M195" s="66" t="s">
+        <v>456</v>
+      </c>
+      <c r="N195" s="66" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="196" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A196" s="113">
         <v>184</v>
       </c>
@@ -8471,8 +9600,14 @@
       <c r="J196" s="66"/>
       <c r="K196" s="66"/>
       <c r="L196" s="66"/>
-    </row>
-    <row r="197" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M196" s="66" t="s">
+        <v>456</v>
+      </c>
+      <c r="N196" s="66" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="197" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A197" s="113">
         <v>185</v>
       </c>
@@ -8499,8 +9634,14 @@
       <c r="J197" s="66"/>
       <c r="K197" s="66"/>
       <c r="L197" s="66"/>
-    </row>
-    <row r="198" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M197" s="66" t="s">
+        <v>456</v>
+      </c>
+      <c r="N197" s="66" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="198" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A198" s="113">
         <v>186</v>
       </c>
@@ -8527,8 +9668,14 @@
       <c r="J198" s="66"/>
       <c r="K198" s="66"/>
       <c r="L198" s="66"/>
-    </row>
-    <row r="199" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M198" s="66" t="s">
+        <v>456</v>
+      </c>
+      <c r="N198" s="66" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="199" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A199" s="113">
         <v>187</v>
       </c>
@@ -8555,8 +9702,14 @@
       <c r="J199" s="66"/>
       <c r="K199" s="66"/>
       <c r="L199" s="66"/>
-    </row>
-    <row r="200" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M199" s="66" t="s">
+        <v>456</v>
+      </c>
+      <c r="N199" s="66" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="200" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A200" s="113">
         <v>188</v>
       </c>
@@ -8583,8 +9736,14 @@
       <c r="J200" s="66"/>
       <c r="K200" s="66"/>
       <c r="L200" s="66"/>
-    </row>
-    <row r="201" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M200" s="66" t="s">
+        <v>456</v>
+      </c>
+      <c r="N200" s="66" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="201" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A201" s="113">
         <v>189</v>
       </c>
@@ -8611,8 +9770,14 @@
       <c r="J201" s="66"/>
       <c r="K201" s="66"/>
       <c r="L201" s="66"/>
-    </row>
-    <row r="202" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M201" s="66" t="s">
+        <v>456</v>
+      </c>
+      <c r="N201" s="66" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="202" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A202" s="113">
         <v>190</v>
       </c>
@@ -8639,8 +9804,14 @@
       <c r="J202" s="66"/>
       <c r="K202" s="66"/>
       <c r="L202" s="66"/>
-    </row>
-    <row r="203" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M202" s="66" t="s">
+        <v>456</v>
+      </c>
+      <c r="N202" s="66" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="203" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A203" s="113">
         <v>191</v>
       </c>
@@ -8667,8 +9838,14 @@
       <c r="J203" s="66"/>
       <c r="K203" s="66"/>
       <c r="L203" s="66"/>
-    </row>
-    <row r="204" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M203" s="66" t="s">
+        <v>456</v>
+      </c>
+      <c r="N203" s="66" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="204" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A204" s="113">
         <v>192</v>
       </c>
@@ -8695,8 +9872,14 @@
       <c r="J204" s="66"/>
       <c r="K204" s="66"/>
       <c r="L204" s="66"/>
-    </row>
-    <row r="205" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M204" s="66" t="s">
+        <v>456</v>
+      </c>
+      <c r="N204" s="66" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="205" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A205" s="113">
         <v>193</v>
       </c>
@@ -8723,8 +9906,14 @@
       <c r="J205" s="66"/>
       <c r="K205" s="66"/>
       <c r="L205" s="66"/>
-    </row>
-    <row r="206" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M205" s="66" t="s">
+        <v>456</v>
+      </c>
+      <c r="N205" s="66" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="206" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A206" s="113">
         <v>194</v>
       </c>
@@ -8751,8 +9940,14 @@
       <c r="J206" s="66"/>
       <c r="K206" s="66"/>
       <c r="L206" s="66"/>
-    </row>
-    <row r="207" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M206" s="66" t="s">
+        <v>456</v>
+      </c>
+      <c r="N206" s="66" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="207" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A207" s="113">
         <v>195</v>
       </c>
@@ -8779,8 +9974,14 @@
       <c r="J207" s="66"/>
       <c r="K207" s="66"/>
       <c r="L207" s="66"/>
-    </row>
-    <row r="208" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M207" s="66" t="s">
+        <v>456</v>
+      </c>
+      <c r="N207" s="66" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="208" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A208" s="113">
         <v>196</v>
       </c>
@@ -8807,8 +10008,14 @@
       <c r="J208" s="66"/>
       <c r="K208" s="66"/>
       <c r="L208" s="66"/>
-    </row>
-    <row r="209" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M208" s="66" t="s">
+        <v>456</v>
+      </c>
+      <c r="N208" s="66" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="209" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A209" s="113">
         <v>197</v>
       </c>
@@ -8835,8 +10042,14 @@
       <c r="J209" s="66"/>
       <c r="K209" s="66"/>
       <c r="L209" s="66"/>
-    </row>
-    <row r="210" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M209" s="66" t="s">
+        <v>456</v>
+      </c>
+      <c r="N209" s="66" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="210" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A210" s="113">
         <v>198</v>
       </c>
@@ -8863,8 +10076,14 @@
       <c r="J210" s="66"/>
       <c r="K210" s="66"/>
       <c r="L210" s="66"/>
-    </row>
-    <row r="211" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M210" s="66" t="s">
+        <v>456</v>
+      </c>
+      <c r="N210" s="66" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="211" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A211" s="113">
         <v>199</v>
       </c>
@@ -8891,8 +10110,14 @@
       <c r="J211" s="66"/>
       <c r="K211" s="66"/>
       <c r="L211" s="66"/>
-    </row>
-    <row r="212" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M211" s="66" t="s">
+        <v>456</v>
+      </c>
+      <c r="N211" s="66" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="212" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A212" s="113">
         <v>200</v>
       </c>
@@ -8919,8 +10144,14 @@
       <c r="J212" s="66"/>
       <c r="K212" s="66"/>
       <c r="L212" s="66"/>
-    </row>
-    <row r="213" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M212" s="66" t="s">
+        <v>456</v>
+      </c>
+      <c r="N212" s="66" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="213" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A213" s="113">
         <v>201</v>
       </c>
@@ -8947,8 +10178,14 @@
       <c r="J213" s="66"/>
       <c r="K213" s="66"/>
       <c r="L213" s="66"/>
-    </row>
-    <row r="214" spans="1:12" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M213" s="66" t="s">
+        <v>456</v>
+      </c>
+      <c r="N213" s="66" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="214" spans="1:14" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A214" s="114">
         <v>202</v>
       </c>
@@ -8975,8 +10212,14 @@
       <c r="J214" s="68"/>
       <c r="K214" s="68"/>
       <c r="L214" s="68"/>
-    </row>
-    <row r="215" spans="1:12" ht="14.45" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="M214" s="68" t="s">
+        <v>456</v>
+      </c>
+      <c r="N214" s="68" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="215" spans="1:14" ht="14.45" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A215" s="113">
         <v>203</v>
       </c>
@@ -9005,8 +10248,14 @@
       <c r="J215" s="66"/>
       <c r="K215" s="66"/>
       <c r="L215" s="66"/>
-    </row>
-    <row r="216" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M215" s="66" t="s">
+        <v>456</v>
+      </c>
+      <c r="N215" s="66" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="216" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A216" s="113">
         <v>204</v>
       </c>
@@ -9033,8 +10282,14 @@
       <c r="J216" s="66"/>
       <c r="K216" s="66"/>
       <c r="L216" s="66"/>
-    </row>
-    <row r="217" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M216" s="66" t="s">
+        <v>456</v>
+      </c>
+      <c r="N216" s="66" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="217" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A217" s="113">
         <v>205</v>
       </c>
@@ -9061,8 +10316,14 @@
       <c r="J217" s="66"/>
       <c r="K217" s="66"/>
       <c r="L217" s="66"/>
-    </row>
-    <row r="218" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M217" s="66" t="s">
+        <v>456</v>
+      </c>
+      <c r="N217" s="66" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="218" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A218" s="113">
         <v>206</v>
       </c>
@@ -9089,8 +10350,14 @@
       <c r="J218" s="66"/>
       <c r="K218" s="66"/>
       <c r="L218" s="66"/>
-    </row>
-    <row r="219" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M218" s="66" t="s">
+        <v>456</v>
+      </c>
+      <c r="N218" s="66" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="219" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A219" s="113">
         <v>207</v>
       </c>
@@ -9117,8 +10384,14 @@
       <c r="J219" s="66"/>
       <c r="K219" s="66"/>
       <c r="L219" s="66"/>
-    </row>
-    <row r="220" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M219" s="66" t="s">
+        <v>456</v>
+      </c>
+      <c r="N219" s="66" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="220" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A220" s="113">
         <v>208</v>
       </c>
@@ -9145,8 +10418,14 @@
       <c r="J220" s="66"/>
       <c r="K220" s="66"/>
       <c r="L220" s="66"/>
-    </row>
-    <row r="221" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M220" s="66" t="s">
+        <v>456</v>
+      </c>
+      <c r="N220" s="66" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="221" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A221" s="113">
         <v>209</v>
       </c>
@@ -9173,8 +10452,14 @@
       <c r="J221" s="66"/>
       <c r="K221" s="66"/>
       <c r="L221" s="66"/>
-    </row>
-    <row r="222" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M221" s="66" t="s">
+        <v>456</v>
+      </c>
+      <c r="N221" s="66" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="222" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A222" s="113">
         <v>210</v>
       </c>
@@ -9201,8 +10486,14 @@
       <c r="J222" s="66"/>
       <c r="K222" s="66"/>
       <c r="L222" s="66"/>
-    </row>
-    <row r="223" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M222" s="66" t="s">
+        <v>456</v>
+      </c>
+      <c r="N222" s="66" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="223" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A223" s="113">
         <v>211</v>
       </c>
@@ -9229,8 +10520,14 @@
       <c r="J223" s="66"/>
       <c r="K223" s="66"/>
       <c r="L223" s="66"/>
-    </row>
-    <row r="224" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M223" s="66" t="s">
+        <v>456</v>
+      </c>
+      <c r="N223" s="66" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="224" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A224" s="113">
         <v>212</v>
       </c>
@@ -9257,8 +10554,14 @@
       <c r="J224" s="66"/>
       <c r="K224" s="66"/>
       <c r="L224" s="66"/>
-    </row>
-    <row r="225" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M224" s="66" t="s">
+        <v>456</v>
+      </c>
+      <c r="N224" s="66" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="225" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A225" s="113">
         <v>213</v>
       </c>
@@ -9285,8 +10588,14 @@
       <c r="J225" s="66"/>
       <c r="K225" s="66"/>
       <c r="L225" s="66"/>
-    </row>
-    <row r="226" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M225" s="66" t="s">
+        <v>456</v>
+      </c>
+      <c r="N225" s="66" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="226" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A226" s="113">
         <v>214</v>
       </c>
@@ -9313,8 +10622,14 @@
       <c r="J226" s="66"/>
       <c r="K226" s="66"/>
       <c r="L226" s="66"/>
-    </row>
-    <row r="227" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M226" s="66" t="s">
+        <v>456</v>
+      </c>
+      <c r="N226" s="66" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="227" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A227" s="113">
         <v>215</v>
       </c>
@@ -9341,8 +10656,14 @@
       <c r="J227" s="66"/>
       <c r="K227" s="66"/>
       <c r="L227" s="66"/>
-    </row>
-    <row r="228" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M227" s="66" t="s">
+        <v>456</v>
+      </c>
+      <c r="N227" s="66" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="228" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A228" s="113">
         <v>216</v>
       </c>
@@ -9369,8 +10690,14 @@
       <c r="J228" s="66"/>
       <c r="K228" s="66"/>
       <c r="L228" s="66"/>
-    </row>
-    <row r="229" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M228" s="66" t="s">
+        <v>456</v>
+      </c>
+      <c r="N228" s="66" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="229" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A229" s="113">
         <v>217</v>
       </c>
@@ -9397,8 +10724,14 @@
       <c r="J229" s="66"/>
       <c r="K229" s="66"/>
       <c r="L229" s="66"/>
-    </row>
-    <row r="230" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M229" s="66" t="s">
+        <v>456</v>
+      </c>
+      <c r="N229" s="66" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="230" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A230" s="113">
         <v>218</v>
       </c>
@@ -9425,8 +10758,14 @@
       <c r="J230" s="66"/>
       <c r="K230" s="66"/>
       <c r="L230" s="66"/>
-    </row>
-    <row r="231" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M230" s="66" t="s">
+        <v>456</v>
+      </c>
+      <c r="N230" s="66" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="231" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A231" s="113">
         <v>219</v>
       </c>
@@ -9453,8 +10792,14 @@
       <c r="J231" s="66"/>
       <c r="K231" s="66"/>
       <c r="L231" s="66"/>
-    </row>
-    <row r="232" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M231" s="66" t="s">
+        <v>456</v>
+      </c>
+      <c r="N231" s="66" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="232" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A232" s="113">
         <v>220</v>
       </c>
@@ -9481,8 +10826,14 @@
       <c r="J232" s="66"/>
       <c r="K232" s="66"/>
       <c r="L232" s="66"/>
-    </row>
-    <row r="233" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M232" s="66" t="s">
+        <v>456</v>
+      </c>
+      <c r="N232" s="66" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="233" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A233" s="113">
         <v>221</v>
       </c>
@@ -9509,8 +10860,14 @@
       <c r="J233" s="66"/>
       <c r="K233" s="66"/>
       <c r="L233" s="66"/>
-    </row>
-    <row r="234" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M233" s="66" t="s">
+        <v>456</v>
+      </c>
+      <c r="N233" s="66" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="234" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A234" s="113">
         <v>222</v>
       </c>
@@ -9537,8 +10894,14 @@
       <c r="J234" s="66"/>
       <c r="K234" s="66"/>
       <c r="L234" s="66"/>
-    </row>
-    <row r="235" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M234" s="66" t="s">
+        <v>456</v>
+      </c>
+      <c r="N234" s="66" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="235" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A235" s="113">
         <v>223</v>
       </c>
@@ -9565,8 +10928,14 @@
       <c r="J235" s="66"/>
       <c r="K235" s="66"/>
       <c r="L235" s="66"/>
-    </row>
-    <row r="236" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M235" s="66" t="s">
+        <v>456</v>
+      </c>
+      <c r="N235" s="66" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="236" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A236" s="113">
         <v>224</v>
       </c>
@@ -9593,8 +10962,14 @@
       <c r="J236" s="66"/>
       <c r="K236" s="66"/>
       <c r="L236" s="66"/>
-    </row>
-    <row r="237" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M236" s="66" t="s">
+        <v>456</v>
+      </c>
+      <c r="N236" s="66" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="237" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A237" s="113">
         <v>225</v>
       </c>
@@ -9621,8 +10996,14 @@
       <c r="J237" s="66"/>
       <c r="K237" s="66"/>
       <c r="L237" s="66"/>
-    </row>
-    <row r="238" spans="1:12" s="26" customFormat="1" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M237" s="66" t="s">
+        <v>456</v>
+      </c>
+      <c r="N237" s="66" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="238" spans="1:14" s="26" customFormat="1" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A238" s="115">
         <v>226</v>
       </c>
@@ -9649,6 +11030,12 @@
       <c r="J238" s="69"/>
       <c r="K238" s="69"/>
       <c r="L238" s="69"/>
+      <c r="M238" s="69" t="s">
+        <v>456</v>
+      </c>
+      <c r="N238" s="69" t="s">
+        <v>456</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:L119" xr:uid="{00000000-0001-0000-0000-000000000000}"/>

</xml_diff>

<commit_message>
Changed name of AllEntitiesCovered Field to be EuTaxonomy Specific
</commit_message>
<xml_diff>
--- a/dataland-framework-toolbox/inputs/eu-taxonomy-financials/eu-taxonomy-financials.xlsx
+++ b/dataland-framework-toolbox/inputs/eu-taxonomy-financials/eu-taxonomy-financials.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d92582\Documents\Dataland\Dataland\dataland-framework-toolbox\inputs\eu-taxonomy-financials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9076012F-4300-4E6F-A85C-9CC34911F37C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4D7B9A1-4543-44A9-9DA9-FE4D4AB72B92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Framework Data Model" sheetId="1" r:id="rId1"/>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1940" uniqueCount="457">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1942" uniqueCount="459">
   <si>
     <t>Field Identifier</t>
   </si>
@@ -1437,6 +1437,12 @@
   </si>
   <si>
     <t>Yes</t>
+  </si>
+  <si>
+    <t>Data Point Type Name Overwrite</t>
+  </si>
+  <si>
+    <t>AreAllGroupEntitiesCoveredByEuTaxonomyReports</t>
   </si>
 </sst>
 </file>
@@ -2232,7 +2238,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="144">
+  <cellXfs count="145">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="7" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2581,9 +2587,6 @@
     <xf numFmtId="0" fontId="6" fillId="8" borderId="5" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="9" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="11" borderId="5" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -2651,6 +2654,12 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="10" borderId="24" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="5" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="9" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -2926,30 +2935,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N238"/>
+  <dimension ref="A1:O238"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="12.42578125" customWidth="1"/>
-    <col min="3" max="3" width="71.5703125" customWidth="1"/>
-    <col min="4" max="4" width="123.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.3984375" customWidth="1"/>
+    <col min="3" max="3" width="71.59765625" customWidth="1"/>
+    <col min="4" max="4" width="123.3984375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="92" customWidth="1"/>
-    <col min="6" max="6" width="36.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="26.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="36.3984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.86328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.3984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.73046875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.265625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.59765625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.1328125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="26.3984375" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="30.265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="107" t="s">
         <v>0</v>
       </c>
@@ -2992,8 +3001,11 @@
       <c r="N1" s="91" t="s">
         <v>455</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O1" s="91" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A2" s="108">
         <v>1</v>
       </c>
@@ -3024,8 +3036,9 @@
       <c r="L2" s="34"/>
       <c r="M2" s="34"/>
       <c r="N2" s="34"/>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O2" s="34"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A3" s="108">
         <v>2</v>
       </c>
@@ -3056,8 +3069,9 @@
       <c r="L3" s="34"/>
       <c r="M3" s="34"/>
       <c r="N3" s="34"/>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O3" s="34"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A4" s="108">
         <v>3</v>
       </c>
@@ -3086,8 +3100,9 @@
       <c r="L4" s="34"/>
       <c r="M4" s="34"/>
       <c r="N4" s="34"/>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O4" s="34"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A5" s="108">
         <v>4</v>
       </c>
@@ -3097,7 +3112,7 @@
       <c r="C5" s="103" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="119" t="s">
+      <c r="D5" s="143" t="s">
         <v>162</v>
       </c>
       <c r="E5" s="9" t="s">
@@ -3118,8 +3133,11 @@
       <c r="L5" s="34"/>
       <c r="M5" s="34"/>
       <c r="N5" s="34"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O5" s="34" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A6" s="108">
         <v>5</v>
       </c>
@@ -3150,8 +3168,9 @@
       <c r="L6" s="34"/>
       <c r="M6" s="34"/>
       <c r="N6" s="34"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O6" s="34"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A7" s="108">
         <v>6</v>
       </c>
@@ -3180,8 +3199,9 @@
       <c r="L7" s="34"/>
       <c r="M7" s="34"/>
       <c r="N7" s="34"/>
-    </row>
-    <row r="8" spans="1:14" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O7" s="34"/>
+    </row>
+    <row r="8" spans="1:15" s="1" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A8" s="109">
         <v>7</v>
       </c>
@@ -3191,7 +3211,7 @@
       <c r="C8" s="105" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="120" t="s">
+      <c r="D8" s="144" t="s">
         <v>23</v>
       </c>
       <c r="E8" s="10" t="s">
@@ -3210,18 +3230,19 @@
       <c r="L8" s="11"/>
       <c r="M8" s="11"/>
       <c r="N8" s="11"/>
-    </row>
-    <row r="9" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="O8" s="11"/>
+    </row>
+    <row r="9" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A9" s="73">
         <v>8</v>
       </c>
       <c r="B9" s="100" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="141" t="s">
+      <c r="C9" s="140" t="s">
         <v>158</v>
       </c>
-      <c r="D9" s="121" t="s">
+      <c r="D9" s="120" t="s">
         <v>160</v>
       </c>
       <c r="E9" s="27" t="s">
@@ -3246,18 +3267,19 @@
       <c r="N9" s="42" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O9" s="42"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A10" s="73">
         <v>9</v>
       </c>
       <c r="B10" s="100" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="141" t="s">
+      <c r="C10" s="140" t="s">
         <v>158</v>
       </c>
-      <c r="D10" s="122" t="s">
+      <c r="D10" s="121" t="s">
         <v>94</v>
       </c>
       <c r="E10" s="28" t="s">
@@ -3282,18 +3304,19 @@
       <c r="N10" s="34" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O10" s="34"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A11" s="73">
         <v>9.1</v>
       </c>
       <c r="B11" s="100" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="141" t="s">
+      <c r="C11" s="140" t="s">
         <v>158</v>
       </c>
-      <c r="D11" s="123" t="s">
+      <c r="D11" s="122" t="s">
         <v>95</v>
       </c>
       <c r="E11" s="28" t="s">
@@ -3318,18 +3341,19 @@
       <c r="N11" s="34" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="O11" s="34"/>
+    </row>
+    <row r="12" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A12" s="72" t="s">
         <v>105</v>
       </c>
       <c r="B12" s="100" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="141" t="s">
+      <c r="C12" s="140" t="s">
         <v>158</v>
       </c>
-      <c r="D12" s="121" t="s">
+      <c r="D12" s="120" t="s">
         <v>96</v>
       </c>
       <c r="E12" s="28" t="s">
@@ -3354,18 +3378,19 @@
       <c r="N12" s="42" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O12" s="42"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A13" s="72" t="s">
         <v>106</v>
       </c>
       <c r="B13" s="100" t="s">
         <v>31</v>
       </c>
-      <c r="C13" s="141" t="s">
+      <c r="C13" s="140" t="s">
         <v>158</v>
       </c>
-      <c r="D13" s="122" t="s">
+      <c r="D13" s="121" t="s">
         <v>97</v>
       </c>
       <c r="E13" s="28" t="s">
@@ -3390,18 +3415,19 @@
       <c r="N13" s="34" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O13" s="34"/>
+    </row>
+    <row r="14" spans="1:15" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A14" s="110" t="s">
         <v>107</v>
       </c>
       <c r="B14" s="117" t="s">
         <v>31</v>
       </c>
-      <c r="C14" s="142" t="s">
+      <c r="C14" s="141" t="s">
         <v>158</v>
       </c>
-      <c r="D14" s="124" t="s">
+      <c r="D14" s="123" t="s">
         <v>98</v>
       </c>
       <c r="E14" s="29" t="s">
@@ -3426,15 +3452,16 @@
       <c r="N14" s="41" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O14" s="41"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A15" s="72">
         <v>10</v>
       </c>
       <c r="B15" s="100" t="s">
         <v>31</v>
       </c>
-      <c r="C15" s="141" t="s">
+      <c r="C15" s="140" t="s">
         <v>32</v>
       </c>
       <c r="D15" s="119" t="s">
@@ -3460,15 +3487,16 @@
       <c r="N15" s="34" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O15" s="34"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A16" s="72">
         <v>10.1</v>
       </c>
       <c r="B16" s="100" t="s">
         <v>31</v>
       </c>
-      <c r="C16" s="141" t="s">
+      <c r="C16" s="140" t="s">
         <v>32</v>
       </c>
       <c r="D16" s="14" t="s">
@@ -3494,15 +3522,16 @@
       <c r="N16" s="34" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O16" s="34"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A17" s="72" t="s">
         <v>108</v>
       </c>
       <c r="B17" s="100" t="s">
         <v>31</v>
       </c>
-      <c r="C17" s="141" t="s">
+      <c r="C17" s="140" t="s">
         <v>32</v>
       </c>
       <c r="D17" s="14" t="s">
@@ -3528,15 +3557,16 @@
       <c r="N17" s="34" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O17" s="34"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A18" s="72" t="s">
         <v>109</v>
       </c>
       <c r="B18" s="100" t="s">
         <v>31</v>
       </c>
-      <c r="C18" s="141" t="s">
+      <c r="C18" s="140" t="s">
         <v>32</v>
       </c>
       <c r="D18" s="14" t="s">
@@ -3562,15 +3592,16 @@
       <c r="N18" s="34" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O18" s="34"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A19" s="72" t="s">
         <v>110</v>
       </c>
       <c r="B19" s="100" t="s">
         <v>31</v>
       </c>
-      <c r="C19" s="141" t="s">
+      <c r="C19" s="140" t="s">
         <v>32</v>
       </c>
       <c r="D19" s="14" t="s">
@@ -3596,15 +3627,16 @@
       <c r="N19" s="34" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O19" s="34"/>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A20" s="72">
         <v>11</v>
       </c>
       <c r="B20" s="100" t="s">
         <v>31</v>
       </c>
-      <c r="C20" s="141" t="s">
+      <c r="C20" s="140" t="s">
         <v>32</v>
       </c>
       <c r="D20" s="14" t="s">
@@ -3630,15 +3662,16 @@
       <c r="N20" s="34" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O20" s="34"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A21" s="72">
         <v>11.1</v>
       </c>
       <c r="B21" s="100" t="s">
         <v>31</v>
       </c>
-      <c r="C21" s="141" t="s">
+      <c r="C21" s="140" t="s">
         <v>32</v>
       </c>
       <c r="D21" s="14" t="s">
@@ -3664,15 +3697,16 @@
       <c r="N21" s="34" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O21" s="34"/>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A22" s="72" t="s">
         <v>111</v>
       </c>
       <c r="B22" s="100" t="s">
         <v>31</v>
       </c>
-      <c r="C22" s="141" t="s">
+      <c r="C22" s="140" t="s">
         <v>32</v>
       </c>
       <c r="D22" s="14" t="s">
@@ -3698,18 +3732,19 @@
       <c r="N22" s="34" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O22" s="34"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A23" s="72" t="s">
         <v>112</v>
       </c>
       <c r="B23" s="100" t="s">
         <v>31</v>
       </c>
-      <c r="C23" s="141" t="s">
+      <c r="C23" s="140" t="s">
         <v>32</v>
       </c>
-      <c r="D23" s="125" t="s">
+      <c r="D23" s="124" t="s">
         <v>150</v>
       </c>
       <c r="E23" s="16" t="s">
@@ -3732,18 +3767,19 @@
       <c r="N23" s="34" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O23" s="34"/>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A24" s="72" t="s">
         <v>175</v>
       </c>
       <c r="B24" s="100" t="s">
         <v>31</v>
       </c>
-      <c r="C24" s="141" t="s">
+      <c r="C24" s="140" t="s">
         <v>32</v>
       </c>
-      <c r="D24" s="125" t="s">
+      <c r="D24" s="124" t="s">
         <v>177</v>
       </c>
       <c r="E24" s="16" t="s">
@@ -3766,18 +3802,19 @@
       <c r="N24" s="34" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O24" s="34"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A25" s="72">
         <v>12</v>
       </c>
       <c r="B25" s="100" t="s">
         <v>31</v>
       </c>
-      <c r="C25" s="141" t="s">
+      <c r="C25" s="140" t="s">
         <v>32</v>
       </c>
-      <c r="D25" s="125" t="s">
+      <c r="D25" s="124" t="s">
         <v>38</v>
       </c>
       <c r="E25" s="16" t="s">
@@ -3800,18 +3837,19 @@
       <c r="N25" s="34" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O25" s="34"/>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A26" s="72">
         <v>12.1</v>
       </c>
       <c r="B26" s="100" t="s">
         <v>31</v>
       </c>
-      <c r="C26" s="141" t="s">
+      <c r="C26" s="140" t="s">
         <v>32</v>
       </c>
-      <c r="D26" s="125" t="s">
+      <c r="D26" s="124" t="s">
         <v>39</v>
       </c>
       <c r="E26" s="16" t="s">
@@ -3834,18 +3872,19 @@
       <c r="N26" s="34" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O26" s="34"/>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A27" s="72" t="s">
         <v>113</v>
       </c>
       <c r="B27" s="100" t="s">
         <v>31</v>
       </c>
-      <c r="C27" s="141" t="s">
+      <c r="C27" s="140" t="s">
         <v>32</v>
       </c>
-      <c r="D27" s="125" t="s">
+      <c r="D27" s="124" t="s">
         <v>68</v>
       </c>
       <c r="E27" s="16" t="s">
@@ -3868,18 +3907,19 @@
       <c r="N27" s="34" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O27" s="34"/>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A28" s="72" t="s">
         <v>114</v>
       </c>
       <c r="B28" s="100" t="s">
         <v>31</v>
       </c>
-      <c r="C28" s="141" t="s">
+      <c r="C28" s="140" t="s">
         <v>32</v>
       </c>
-      <c r="D28" s="125" t="s">
+      <c r="D28" s="124" t="s">
         <v>151</v>
       </c>
       <c r="E28" s="16" t="s">
@@ -3902,18 +3942,19 @@
       <c r="N28" s="34" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O28" s="34"/>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A29" s="72">
         <v>13</v>
       </c>
       <c r="B29" s="100" t="s">
         <v>31</v>
       </c>
-      <c r="C29" s="141" t="s">
+      <c r="C29" s="140" t="s">
         <v>32</v>
       </c>
-      <c r="D29" s="125" t="s">
+      <c r="D29" s="124" t="s">
         <v>40</v>
       </c>
       <c r="E29" s="16" t="s">
@@ -3936,18 +3977,19 @@
       <c r="N29" s="34" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O29" s="34"/>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A30" s="72">
         <v>13.1</v>
       </c>
       <c r="B30" s="100" t="s">
         <v>31</v>
       </c>
-      <c r="C30" s="141" t="s">
+      <c r="C30" s="140" t="s">
         <v>32</v>
       </c>
-      <c r="D30" s="125" t="s">
+      <c r="D30" s="124" t="s">
         <v>41</v>
       </c>
       <c r="E30" s="16" t="s">
@@ -3970,18 +4012,19 @@
       <c r="N30" s="34" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O30" s="34"/>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A31" s="72" t="s">
         <v>115</v>
       </c>
       <c r="B31" s="100" t="s">
         <v>31</v>
       </c>
-      <c r="C31" s="141" t="s">
+      <c r="C31" s="140" t="s">
         <v>32</v>
       </c>
-      <c r="D31" s="125" t="s">
+      <c r="D31" s="124" t="s">
         <v>69</v>
       </c>
       <c r="E31" s="16" t="s">
@@ -4004,18 +4047,19 @@
       <c r="N31" s="34" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O31" s="34"/>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A32" s="72" t="s">
         <v>116</v>
       </c>
       <c r="B32" s="100" t="s">
         <v>31</v>
       </c>
-      <c r="C32" s="141" t="s">
+      <c r="C32" s="140" t="s">
         <v>32</v>
       </c>
-      <c r="D32" s="125" t="s">
+      <c r="D32" s="124" t="s">
         <v>152</v>
       </c>
       <c r="E32" s="16" t="s">
@@ -4038,18 +4082,19 @@
       <c r="N32" s="34" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O32" s="34"/>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A33" s="72">
         <v>14</v>
       </c>
       <c r="B33" s="100" t="s">
         <v>31</v>
       </c>
-      <c r="C33" s="141" t="s">
+      <c r="C33" s="140" t="s">
         <v>32</v>
       </c>
-      <c r="D33" s="125" t="s">
+      <c r="D33" s="124" t="s">
         <v>42</v>
       </c>
       <c r="E33" s="16" t="s">
@@ -4072,18 +4117,19 @@
       <c r="N33" s="34" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O33" s="34"/>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A34" s="72">
         <v>14.1</v>
       </c>
       <c r="B34" s="100" t="s">
         <v>31</v>
       </c>
-      <c r="C34" s="141" t="s">
+      <c r="C34" s="140" t="s">
         <v>32</v>
       </c>
-      <c r="D34" s="125" t="s">
+      <c r="D34" s="124" t="s">
         <v>43</v>
       </c>
       <c r="E34" s="16" t="s">
@@ -4106,18 +4152,19 @@
       <c r="N34" s="34" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O34" s="34"/>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A35" s="72" t="s">
         <v>117</v>
       </c>
       <c r="B35" s="100" t="s">
         <v>31</v>
       </c>
-      <c r="C35" s="141" t="s">
+      <c r="C35" s="140" t="s">
         <v>32</v>
       </c>
-      <c r="D35" s="125" t="s">
+      <c r="D35" s="124" t="s">
         <v>70</v>
       </c>
       <c r="E35" s="16" t="s">
@@ -4140,18 +4187,19 @@
       <c r="N35" s="34" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O35" s="34"/>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A36" s="72" t="s">
         <v>118</v>
       </c>
       <c r="B36" s="100" t="s">
         <v>31</v>
       </c>
-      <c r="C36" s="141" t="s">
+      <c r="C36" s="140" t="s">
         <v>32</v>
       </c>
-      <c r="D36" s="125" t="s">
+      <c r="D36" s="124" t="s">
         <v>153</v>
       </c>
       <c r="E36" s="16" t="s">
@@ -4174,18 +4222,19 @@
       <c r="N36" s="34" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O36" s="34"/>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A37" s="72">
         <v>15</v>
       </c>
       <c r="B37" s="100" t="s">
         <v>31</v>
       </c>
-      <c r="C37" s="141" t="s">
+      <c r="C37" s="140" t="s">
         <v>32</v>
       </c>
-      <c r="D37" s="125" t="s">
+      <c r="D37" s="124" t="s">
         <v>44</v>
       </c>
       <c r="E37" s="16" t="s">
@@ -4208,18 +4257,19 @@
       <c r="N37" s="34" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O37" s="34"/>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A38" s="72">
         <v>15.1</v>
       </c>
       <c r="B38" s="100" t="s">
         <v>31</v>
       </c>
-      <c r="C38" s="141" t="s">
+      <c r="C38" s="140" t="s">
         <v>32</v>
       </c>
-      <c r="D38" s="125" t="s">
+      <c r="D38" s="124" t="s">
         <v>45</v>
       </c>
       <c r="E38" s="16" t="s">
@@ -4242,18 +4292,19 @@
       <c r="N38" s="34" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O38" s="34"/>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A39" s="43" t="s">
         <v>119</v>
       </c>
       <c r="B39" s="100" t="s">
         <v>31</v>
       </c>
-      <c r="C39" s="141" t="s">
+      <c r="C39" s="140" t="s">
         <v>32</v>
       </c>
-      <c r="D39" s="126" t="s">
+      <c r="D39" s="125" t="s">
         <v>71</v>
       </c>
       <c r="E39" s="17" t="s">
@@ -4276,18 +4327,19 @@
       <c r="N39" s="45" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O39" s="45"/>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A40" s="72" t="s">
         <v>120</v>
       </c>
       <c r="B40" s="100" t="s">
         <v>31</v>
       </c>
-      <c r="C40" s="141" t="s">
+      <c r="C40" s="140" t="s">
         <v>32</v>
       </c>
-      <c r="D40" s="127" t="s">
+      <c r="D40" s="126" t="s">
         <v>154</v>
       </c>
       <c r="E40" s="30" t="s">
@@ -4310,18 +4362,19 @@
       <c r="N40" s="46" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O40" s="46"/>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A41" s="72">
         <v>16</v>
       </c>
       <c r="B41" s="100" t="s">
         <v>31</v>
       </c>
-      <c r="C41" s="141" t="s">
+      <c r="C41" s="140" t="s">
         <v>32</v>
       </c>
-      <c r="D41" s="125" t="s">
+      <c r="D41" s="124" t="s">
         <v>123</v>
       </c>
       <c r="E41" s="16" t="s">
@@ -4344,18 +4397,19 @@
       <c r="N41" s="34" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O41" s="34"/>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A42" s="72">
         <v>16.100000000000001</v>
       </c>
       <c r="B42" s="100" t="s">
         <v>31</v>
       </c>
-      <c r="C42" s="141" t="s">
+      <c r="C42" s="140" t="s">
         <v>32</v>
       </c>
-      <c r="D42" s="125" t="s">
+      <c r="D42" s="124" t="s">
         <v>124</v>
       </c>
       <c r="E42" s="16" t="s">
@@ -4378,15 +4432,16 @@
       <c r="N42" s="34" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O42" s="34"/>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A43" s="43" t="s">
         <v>121</v>
       </c>
       <c r="B43" s="100" t="s">
         <v>31</v>
       </c>
-      <c r="C43" s="141" t="s">
+      <c r="C43" s="140" t="s">
         <v>32</v>
       </c>
       <c r="D43" s="74" t="s">
@@ -4412,18 +4467,19 @@
       <c r="N43" s="45" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O43" s="45"/>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A44" s="43" t="s">
         <v>122</v>
       </c>
       <c r="B44" s="100" t="s">
         <v>31</v>
       </c>
-      <c r="C44" s="141" t="s">
+      <c r="C44" s="140" t="s">
         <v>32</v>
       </c>
-      <c r="D44" s="127" t="s">
+      <c r="D44" s="126" t="s">
         <v>155</v>
       </c>
       <c r="E44" s="30" t="s">
@@ -4446,18 +4502,19 @@
       <c r="N44" s="46" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="45" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O44" s="46"/>
+    </row>
+    <row r="45" spans="1:15" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A45" s="111" t="s">
         <v>159</v>
       </c>
       <c r="B45" s="118" t="s">
         <v>31</v>
       </c>
-      <c r="C45" s="143" t="s">
+      <c r="C45" s="142" t="s">
         <v>32</v>
       </c>
-      <c r="D45" s="128" t="s">
+      <c r="D45" s="127" t="s">
         <v>157</v>
       </c>
       <c r="E45" s="18" t="s">
@@ -4480,15 +4537,16 @@
       <c r="N45" s="50" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="46" spans="1:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="O45" s="50"/>
+    </row>
+    <row r="46" spans="1:15" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
       <c r="A46" s="72">
         <v>20</v>
       </c>
       <c r="B46" s="100" t="s">
         <v>31</v>
       </c>
-      <c r="C46" s="141" t="s">
+      <c r="C46" s="140" t="s">
         <v>33</v>
       </c>
       <c r="D46" s="119" t="s">
@@ -4514,15 +4572,16 @@
       <c r="N46" s="34" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O46" s="34"/>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A47" s="72">
         <v>20.100000000000001</v>
       </c>
       <c r="B47" s="100" t="s">
         <v>31</v>
       </c>
-      <c r="C47" s="141" t="s">
+      <c r="C47" s="140" t="s">
         <v>33</v>
       </c>
       <c r="D47" s="14" t="s">
@@ -4548,15 +4607,16 @@
       <c r="N47" s="34" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O47" s="34"/>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A48" s="72" t="s">
         <v>129</v>
       </c>
       <c r="B48" s="100" t="s">
         <v>31</v>
       </c>
-      <c r="C48" s="141" t="s">
+      <c r="C48" s="140" t="s">
         <v>33</v>
       </c>
       <c r="D48" s="14" t="s">
@@ -4582,15 +4642,16 @@
       <c r="N48" s="34" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O48" s="34"/>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A49" s="72" t="s">
         <v>130</v>
       </c>
       <c r="B49" s="100" t="s">
         <v>31</v>
       </c>
-      <c r="C49" s="141" t="s">
+      <c r="C49" s="140" t="s">
         <v>33</v>
       </c>
       <c r="D49" s="14" t="s">
@@ -4616,15 +4677,16 @@
       <c r="N49" s="34" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O49" s="34"/>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A50" s="72" t="s">
         <v>131</v>
       </c>
       <c r="B50" s="100" t="s">
         <v>31</v>
       </c>
-      <c r="C50" s="141" t="s">
+      <c r="C50" s="140" t="s">
         <v>33</v>
       </c>
       <c r="D50" s="14" t="s">
@@ -4650,15 +4712,16 @@
       <c r="N50" s="34" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O50" s="34"/>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A51" s="72">
         <v>21</v>
       </c>
       <c r="B51" s="100" t="s">
         <v>31</v>
       </c>
-      <c r="C51" s="141" t="s">
+      <c r="C51" s="140" t="s">
         <v>33</v>
       </c>
       <c r="D51" s="14" t="s">
@@ -4684,15 +4747,16 @@
       <c r="N51" s="34" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O51" s="34"/>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A52" s="72">
         <v>21.1</v>
       </c>
       <c r="B52" s="100" t="s">
         <v>31</v>
       </c>
-      <c r="C52" s="141" t="s">
+      <c r="C52" s="140" t="s">
         <v>33</v>
       </c>
       <c r="D52" s="14" t="s">
@@ -4718,15 +4782,16 @@
       <c r="N52" s="34" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O52" s="34"/>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A53" s="72" t="s">
         <v>132</v>
       </c>
       <c r="B53" s="100" t="s">
         <v>31</v>
       </c>
-      <c r="C53" s="141" t="s">
+      <c r="C53" s="140" t="s">
         <v>33</v>
       </c>
       <c r="D53" s="14" t="s">
@@ -4752,18 +4817,19 @@
       <c r="N53" s="34" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O53" s="34"/>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A54" s="72" t="s">
         <v>133</v>
       </c>
       <c r="B54" s="100" t="s">
         <v>31</v>
       </c>
-      <c r="C54" s="141" t="s">
+      <c r="C54" s="140" t="s">
         <v>33</v>
       </c>
-      <c r="D54" s="125" t="s">
+      <c r="D54" s="124" t="s">
         <v>150</v>
       </c>
       <c r="E54" s="16" t="s">
@@ -4786,18 +4852,19 @@
       <c r="N54" s="34" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O54" s="34"/>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A55" s="72" t="s">
         <v>178</v>
       </c>
       <c r="B55" s="100" t="s">
         <v>31</v>
       </c>
-      <c r="C55" s="141" t="s">
+      <c r="C55" s="140" t="s">
         <v>33</v>
       </c>
-      <c r="D55" s="125" t="s">
+      <c r="D55" s="124" t="s">
         <v>177</v>
       </c>
       <c r="E55" s="16" t="s">
@@ -4820,18 +4887,19 @@
       <c r="N55" s="34" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O55" s="34"/>
+    </row>
+    <row r="56" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A56" s="72">
         <v>22</v>
       </c>
       <c r="B56" s="100" t="s">
         <v>31</v>
       </c>
-      <c r="C56" s="141" t="s">
+      <c r="C56" s="140" t="s">
         <v>33</v>
       </c>
-      <c r="D56" s="125" t="s">
+      <c r="D56" s="124" t="s">
         <v>38</v>
       </c>
       <c r="E56" s="16" t="s">
@@ -4854,18 +4922,19 @@
       <c r="N56" s="34" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O56" s="34"/>
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A57" s="72">
         <v>22.1</v>
       </c>
       <c r="B57" s="100" t="s">
         <v>31</v>
       </c>
-      <c r="C57" s="141" t="s">
+      <c r="C57" s="140" t="s">
         <v>33</v>
       </c>
-      <c r="D57" s="125" t="s">
+      <c r="D57" s="124" t="s">
         <v>39</v>
       </c>
       <c r="E57" s="16" t="s">
@@ -4888,18 +4957,19 @@
       <c r="N57" s="34" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O57" s="34"/>
+    </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A58" s="72" t="s">
         <v>134</v>
       </c>
       <c r="B58" s="100" t="s">
         <v>31</v>
       </c>
-      <c r="C58" s="141" t="s">
+      <c r="C58" s="140" t="s">
         <v>33</v>
       </c>
-      <c r="D58" s="125" t="s">
+      <c r="D58" s="124" t="s">
         <v>68</v>
       </c>
       <c r="E58" s="15" t="s">
@@ -4922,18 +4992,19 @@
       <c r="N58" s="34" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O58" s="34"/>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A59" s="72" t="s">
         <v>135</v>
       </c>
       <c r="B59" s="100" t="s">
         <v>31</v>
       </c>
-      <c r="C59" s="141" t="s">
+      <c r="C59" s="140" t="s">
         <v>33</v>
       </c>
-      <c r="D59" s="125" t="s">
+      <c r="D59" s="124" t="s">
         <v>151</v>
       </c>
       <c r="E59" s="15" t="s">
@@ -4956,18 +5027,19 @@
       <c r="N59" s="34" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O59" s="34"/>
+    </row>
+    <row r="60" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A60" s="72">
         <v>23</v>
       </c>
       <c r="B60" s="100" t="s">
         <v>31</v>
       </c>
-      <c r="C60" s="141" t="s">
+      <c r="C60" s="140" t="s">
         <v>33</v>
       </c>
-      <c r="D60" s="125" t="s">
+      <c r="D60" s="124" t="s">
         <v>40</v>
       </c>
       <c r="E60" s="15" t="s">
@@ -4990,18 +5062,19 @@
       <c r="N60" s="34" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O60" s="34"/>
+    </row>
+    <row r="61" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A61" s="72">
         <v>23.1</v>
       </c>
       <c r="B61" s="100" t="s">
         <v>31</v>
       </c>
-      <c r="C61" s="141" t="s">
+      <c r="C61" s="140" t="s">
         <v>33</v>
       </c>
-      <c r="D61" s="125" t="s">
+      <c r="D61" s="124" t="s">
         <v>41</v>
       </c>
       <c r="E61" s="15" t="s">
@@ -5024,18 +5097,19 @@
       <c r="N61" s="34" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O61" s="34"/>
+    </row>
+    <row r="62" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A62" s="72" t="s">
         <v>136</v>
       </c>
       <c r="B62" s="100" t="s">
         <v>31</v>
       </c>
-      <c r="C62" s="141" t="s">
+      <c r="C62" s="140" t="s">
         <v>33</v>
       </c>
-      <c r="D62" s="125" t="s">
+      <c r="D62" s="124" t="s">
         <v>69</v>
       </c>
       <c r="E62" s="15" t="s">
@@ -5058,18 +5132,19 @@
       <c r="N62" s="34" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O62" s="34"/>
+    </row>
+    <row r="63" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A63" s="72" t="s">
         <v>137</v>
       </c>
       <c r="B63" s="100" t="s">
         <v>31</v>
       </c>
-      <c r="C63" s="141" t="s">
+      <c r="C63" s="140" t="s">
         <v>33</v>
       </c>
-      <c r="D63" s="125" t="s">
+      <c r="D63" s="124" t="s">
         <v>152</v>
       </c>
       <c r="E63" s="15" t="s">
@@ -5092,18 +5167,19 @@
       <c r="N63" s="34" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O63" s="34"/>
+    </row>
+    <row r="64" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A64" s="72">
         <v>24</v>
       </c>
       <c r="B64" s="100" t="s">
         <v>31</v>
       </c>
-      <c r="C64" s="141" t="s">
+      <c r="C64" s="140" t="s">
         <v>33</v>
       </c>
-      <c r="D64" s="125" t="s">
+      <c r="D64" s="124" t="s">
         <v>42</v>
       </c>
       <c r="E64" s="15" t="s">
@@ -5126,18 +5202,19 @@
       <c r="N64" s="34" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O64" s="34"/>
+    </row>
+    <row r="65" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A65" s="72">
         <v>24.1</v>
       </c>
       <c r="B65" s="100" t="s">
         <v>31</v>
       </c>
-      <c r="C65" s="141" t="s">
+      <c r="C65" s="140" t="s">
         <v>33</v>
       </c>
-      <c r="D65" s="125" t="s">
+      <c r="D65" s="124" t="s">
         <v>43</v>
       </c>
       <c r="E65" s="15" t="s">
@@ -5160,18 +5237,19 @@
       <c r="N65" s="34" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O65" s="34"/>
+    </row>
+    <row r="66" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A66" s="72" t="s">
         <v>138</v>
       </c>
       <c r="B66" s="100" t="s">
         <v>31</v>
       </c>
-      <c r="C66" s="141" t="s">
+      <c r="C66" s="140" t="s">
         <v>33</v>
       </c>
-      <c r="D66" s="125" t="s">
+      <c r="D66" s="124" t="s">
         <v>70</v>
       </c>
       <c r="E66" s="15" t="s">
@@ -5194,18 +5272,19 @@
       <c r="N66" s="34" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O66" s="34"/>
+    </row>
+    <row r="67" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A67" s="72" t="s">
         <v>139</v>
       </c>
       <c r="B67" s="100" t="s">
         <v>31</v>
       </c>
-      <c r="C67" s="141" t="s">
+      <c r="C67" s="140" t="s">
         <v>33</v>
       </c>
-      <c r="D67" s="125" t="s">
+      <c r="D67" s="124" t="s">
         <v>153</v>
       </c>
       <c r="E67" s="15" t="s">
@@ -5228,18 +5307,19 @@
       <c r="N67" s="34" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O67" s="34"/>
+    </row>
+    <row r="68" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A68" s="72">
         <v>25</v>
       </c>
       <c r="B68" s="100" t="s">
         <v>31</v>
       </c>
-      <c r="C68" s="141" t="s">
+      <c r="C68" s="140" t="s">
         <v>33</v>
       </c>
-      <c r="D68" s="125" t="s">
+      <c r="D68" s="124" t="s">
         <v>44</v>
       </c>
       <c r="E68" s="15" t="s">
@@ -5262,18 +5342,19 @@
       <c r="N68" s="34" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="69" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O68" s="34"/>
+    </row>
+    <row r="69" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A69" s="72">
         <v>25.1</v>
       </c>
       <c r="B69" s="100" t="s">
         <v>31</v>
       </c>
-      <c r="C69" s="141" t="s">
+      <c r="C69" s="140" t="s">
         <v>33</v>
       </c>
-      <c r="D69" s="125" t="s">
+      <c r="D69" s="124" t="s">
         <v>45</v>
       </c>
       <c r="E69" s="15" t="s">
@@ -5296,18 +5377,19 @@
       <c r="N69" s="34" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="70" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O69" s="34"/>
+    </row>
+    <row r="70" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A70" s="43" t="s">
         <v>140</v>
       </c>
       <c r="B70" s="100" t="s">
         <v>31</v>
       </c>
-      <c r="C70" s="141" t="s">
+      <c r="C70" s="140" t="s">
         <v>33</v>
       </c>
-      <c r="D70" s="126" t="s">
+      <c r="D70" s="125" t="s">
         <v>71</v>
       </c>
       <c r="E70" s="15" t="s">
@@ -5330,18 +5412,19 @@
       <c r="N70" s="34" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="71" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O70" s="34"/>
+    </row>
+    <row r="71" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A71" s="72" t="s">
         <v>141</v>
       </c>
       <c r="B71" s="100" t="s">
         <v>31</v>
       </c>
-      <c r="C71" s="141" t="s">
+      <c r="C71" s="140" t="s">
         <v>33</v>
       </c>
-      <c r="D71" s="127" t="s">
+      <c r="D71" s="126" t="s">
         <v>154</v>
       </c>
       <c r="E71" s="15" t="s">
@@ -5364,18 +5447,19 @@
       <c r="N71" s="34" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O71" s="34"/>
+    </row>
+    <row r="72" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A72" s="72">
         <v>26</v>
       </c>
       <c r="B72" s="100" t="s">
         <v>31</v>
       </c>
-      <c r="C72" s="141" t="s">
+      <c r="C72" s="140" t="s">
         <v>33</v>
       </c>
-      <c r="D72" s="125" t="s">
+      <c r="D72" s="124" t="s">
         <v>123</v>
       </c>
       <c r="E72" s="16" t="s">
@@ -5398,18 +5482,19 @@
       <c r="N72" s="34" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O72" s="34"/>
+    </row>
+    <row r="73" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A73" s="72">
         <v>26.1</v>
       </c>
       <c r="B73" s="100" t="s">
         <v>31</v>
       </c>
-      <c r="C73" s="141" t="s">
+      <c r="C73" s="140" t="s">
         <v>33</v>
       </c>
-      <c r="D73" s="125" t="s">
+      <c r="D73" s="124" t="s">
         <v>124</v>
       </c>
       <c r="E73" s="16" t="s">
@@ -5432,15 +5517,16 @@
       <c r="N73" s="34" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O73" s="34"/>
+    </row>
+    <row r="74" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A74" s="43" t="s">
         <v>142</v>
       </c>
       <c r="B74" s="100" t="s">
         <v>31</v>
       </c>
-      <c r="C74" s="141" t="s">
+      <c r="C74" s="140" t="s">
         <v>33</v>
       </c>
       <c r="D74" s="74" t="s">
@@ -5466,18 +5552,19 @@
       <c r="N74" s="34" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O74" s="34"/>
+    </row>
+    <row r="75" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A75" s="72" t="s">
         <v>143</v>
       </c>
       <c r="B75" s="100" t="s">
         <v>31</v>
       </c>
-      <c r="C75" s="141" t="s">
+      <c r="C75" s="140" t="s">
         <v>33</v>
       </c>
-      <c r="D75" s="127" t="s">
+      <c r="D75" s="126" t="s">
         <v>155</v>
       </c>
       <c r="E75" s="30" t="s">
@@ -5500,18 +5587,19 @@
       <c r="N75" s="34" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="76" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O75" s="34"/>
+    </row>
+    <row r="76" spans="1:15" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A76" s="110" t="s">
         <v>144</v>
       </c>
       <c r="B76" s="117" t="s">
         <v>31</v>
       </c>
-      <c r="C76" s="142" t="s">
+      <c r="C76" s="141" t="s">
         <v>33</v>
       </c>
-      <c r="D76" s="129" t="s">
+      <c r="D76" s="128" t="s">
         <v>157</v>
       </c>
       <c r="E76" s="70" t="s">
@@ -5534,8 +5622,9 @@
       <c r="N76" s="41" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="77" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O76" s="41"/>
+    </row>
+    <row r="77" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A77" s="56">
         <v>65</v>
       </c>
@@ -5545,7 +5634,7 @@
       <c r="C77" s="19" t="s">
         <v>180</v>
       </c>
-      <c r="D77" s="130" t="s">
+      <c r="D77" s="129" t="s">
         <v>185</v>
       </c>
       <c r="E77" s="71" t="s">
@@ -5566,8 +5655,9 @@
         <v>456</v>
       </c>
       <c r="N77" s="34"/>
-    </row>
-    <row r="78" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O77" s="34"/>
+    </row>
+    <row r="78" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A78" s="56">
         <v>66</v>
       </c>
@@ -5577,7 +5667,7 @@
       <c r="C78" s="19" t="s">
         <v>180</v>
       </c>
-      <c r="D78" s="130" t="s">
+      <c r="D78" s="129" t="s">
         <v>186</v>
       </c>
       <c r="E78" s="71" t="s">
@@ -5598,8 +5688,9 @@
         <v>456</v>
       </c>
       <c r="N78" s="34"/>
-    </row>
-    <row r="79" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O78" s="34"/>
+    </row>
+    <row r="79" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A79" s="56">
         <v>67</v>
       </c>
@@ -5609,7 +5700,7 @@
       <c r="C79" s="19" t="s">
         <v>180</v>
       </c>
-      <c r="D79" s="130" t="s">
+      <c r="D79" s="129" t="s">
         <v>187</v>
       </c>
       <c r="E79" s="71" t="s">
@@ -5632,8 +5723,9 @@
         <v>456</v>
       </c>
       <c r="N79" s="34"/>
-    </row>
-    <row r="80" spans="1:14" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O79" s="34"/>
+    </row>
+    <row r="80" spans="1:15" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A80" s="112">
         <v>68</v>
       </c>
@@ -5643,7 +5735,7 @@
       <c r="C80" s="101" t="s">
         <v>180</v>
       </c>
-      <c r="D80" s="131" t="s">
+      <c r="D80" s="130" t="s">
         <v>188</v>
       </c>
       <c r="E80" s="84" t="s">
@@ -5666,8 +5758,9 @@
         <v>456</v>
       </c>
       <c r="N80" s="85"/>
-    </row>
-    <row r="81" spans="1:14" ht="14.45" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="O80" s="85"/>
+    </row>
+    <row r="81" spans="1:15" ht="14.45" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
       <c r="A81" s="56">
         <v>69</v>
       </c>
@@ -5677,7 +5770,7 @@
       <c r="C81" s="19" t="s">
         <v>190</v>
       </c>
-      <c r="D81" s="130" t="s">
+      <c r="D81" s="129" t="s">
         <v>419</v>
       </c>
       <c r="E81" s="71" t="s">
@@ -5700,8 +5793,9 @@
       <c r="N81" s="34" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="82" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O81" s="34"/>
+    </row>
+    <row r="82" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A82" s="56">
         <v>70</v>
       </c>
@@ -5711,7 +5805,7 @@
       <c r="C82" s="19" t="s">
         <v>190</v>
       </c>
-      <c r="D82" s="130" t="s">
+      <c r="D82" s="129" t="s">
         <v>420</v>
       </c>
       <c r="E82" s="71" t="s">
@@ -5734,8 +5828,9 @@
       <c r="N82" s="34" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="83" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O82" s="34"/>
+    </row>
+    <row r="83" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A83" s="56">
         <v>71</v>
       </c>
@@ -5745,7 +5840,7 @@
       <c r="C83" s="19" t="s">
         <v>190</v>
       </c>
-      <c r="D83" s="130" t="s">
+      <c r="D83" s="129" t="s">
         <v>421</v>
       </c>
       <c r="E83" s="71" t="s">
@@ -5768,8 +5863,9 @@
       <c r="N83" s="34" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="84" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O83" s="34"/>
+    </row>
+    <row r="84" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A84" s="56">
         <v>72</v>
       </c>
@@ -5779,7 +5875,7 @@
       <c r="C84" s="19" t="s">
         <v>190</v>
       </c>
-      <c r="D84" s="130" t="s">
+      <c r="D84" s="129" t="s">
         <v>422</v>
       </c>
       <c r="E84" s="71" t="s">
@@ -5802,8 +5898,9 @@
       <c r="N84" s="34" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="85" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O84" s="34"/>
+    </row>
+    <row r="85" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A85" s="56">
         <v>73</v>
       </c>
@@ -5813,7 +5910,7 @@
       <c r="C85" s="19" t="s">
         <v>190</v>
       </c>
-      <c r="D85" s="130" t="s">
+      <c r="D85" s="129" t="s">
         <v>423</v>
       </c>
       <c r="E85" s="71" t="s">
@@ -5836,8 +5933,9 @@
       <c r="N85" s="34" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="86" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O85" s="34"/>
+    </row>
+    <row r="86" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A86" s="56">
         <v>74</v>
       </c>
@@ -5847,7 +5945,7 @@
       <c r="C86" s="19" t="s">
         <v>190</v>
       </c>
-      <c r="D86" s="130" t="s">
+      <c r="D86" s="129" t="s">
         <v>424</v>
       </c>
       <c r="E86" s="2" t="s">
@@ -5870,8 +5968,9 @@
       <c r="N86" s="34" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="87" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O86" s="34"/>
+    </row>
+    <row r="87" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A87" s="56">
         <v>75</v>
       </c>
@@ -5881,7 +5980,7 @@
       <c r="C87" s="19" t="s">
         <v>190</v>
       </c>
-      <c r="D87" s="130" t="s">
+      <c r="D87" s="129" t="s">
         <v>425</v>
       </c>
       <c r="E87" s="2" t="s">
@@ -5904,8 +6003,9 @@
       <c r="N87" s="34" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="88" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O87" s="34"/>
+    </row>
+    <row r="88" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A88" s="56">
         <v>76</v>
       </c>
@@ -5915,7 +6015,7 @@
       <c r="C88" s="19" t="s">
         <v>190</v>
       </c>
-      <c r="D88" s="130" t="s">
+      <c r="D88" s="129" t="s">
         <v>426</v>
       </c>
       <c r="E88" s="2" t="s">
@@ -5938,8 +6038,9 @@
       <c r="N88" s="34" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="89" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O88" s="34"/>
+    </row>
+    <row r="89" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A89" s="56">
         <v>77</v>
       </c>
@@ -5949,7 +6050,7 @@
       <c r="C89" s="19" t="s">
         <v>190</v>
       </c>
-      <c r="D89" s="130" t="s">
+      <c r="D89" s="129" t="s">
         <v>427</v>
       </c>
       <c r="E89" s="2" t="s">
@@ -5972,8 +6073,9 @@
       <c r="N89" s="34" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="90" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O89" s="34"/>
+    </row>
+    <row r="90" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A90" s="56">
         <v>78</v>
       </c>
@@ -5983,7 +6085,7 @@
       <c r="C90" s="19" t="s">
         <v>190</v>
       </c>
-      <c r="D90" s="130" t="s">
+      <c r="D90" s="129" t="s">
         <v>428</v>
       </c>
       <c r="E90" s="2" t="s">
@@ -6006,8 +6108,9 @@
       <c r="N90" s="34" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="91" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O90" s="34"/>
+    </row>
+    <row r="91" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A91" s="56">
         <v>79</v>
       </c>
@@ -6017,7 +6120,7 @@
       <c r="C91" s="19" t="s">
         <v>190</v>
       </c>
-      <c r="D91" s="130" t="s">
+      <c r="D91" s="129" t="s">
         <v>429</v>
       </c>
       <c r="E91" s="2" t="s">
@@ -6040,8 +6143,9 @@
       <c r="N91" s="34" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="92" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O91" s="34"/>
+    </row>
+    <row r="92" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A92" s="56">
         <v>80</v>
       </c>
@@ -6051,7 +6155,7 @@
       <c r="C92" s="19" t="s">
         <v>190</v>
       </c>
-      <c r="D92" s="132" t="s">
+      <c r="D92" s="131" t="s">
         <v>430</v>
       </c>
       <c r="E92" s="4" t="s">
@@ -6074,8 +6178,9 @@
       <c r="N92" s="45" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="93" spans="1:14" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O92" s="45"/>
+    </row>
+    <row r="93" spans="1:15" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A93" s="52">
         <v>81</v>
       </c>
@@ -6085,7 +6190,7 @@
       <c r="C93" s="101" t="s">
         <v>190</v>
       </c>
-      <c r="D93" s="133" t="s">
+      <c r="D93" s="132" t="s">
         <v>431</v>
       </c>
       <c r="E93" s="24" t="s">
@@ -6108,8 +6213,9 @@
       <c r="N93" s="55" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="94" spans="1:14" ht="14.45" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="O93" s="55"/>
+    </row>
+    <row r="94" spans="1:15" ht="14.45" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
       <c r="A94" s="56">
         <v>82</v>
       </c>
@@ -6119,7 +6225,7 @@
       <c r="C94" s="19" t="s">
         <v>189</v>
       </c>
-      <c r="D94" s="130" t="s">
+      <c r="D94" s="129" t="s">
         <v>432</v>
       </c>
       <c r="E94" s="71" t="s">
@@ -6142,8 +6248,9 @@
       <c r="N94" s="57" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="95" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O94" s="57"/>
+    </row>
+    <row r="95" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A95" s="56">
         <v>83</v>
       </c>
@@ -6153,7 +6260,7 @@
       <c r="C95" s="19" t="s">
         <v>189</v>
       </c>
-      <c r="D95" s="130" t="s">
+      <c r="D95" s="129" t="s">
         <v>433</v>
       </c>
       <c r="E95" s="71" t="s">
@@ -6176,8 +6283,9 @@
       <c r="N95" s="58" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="96" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O95" s="58"/>
+    </row>
+    <row r="96" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A96" s="56">
         <v>84</v>
       </c>
@@ -6187,7 +6295,7 @@
       <c r="C96" s="19" t="s">
         <v>189</v>
       </c>
-      <c r="D96" s="130" t="s">
+      <c r="D96" s="129" t="s">
         <v>434</v>
       </c>
       <c r="E96" s="71" t="s">
@@ -6210,8 +6318,9 @@
       <c r="N96" s="58" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="97" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O96" s="58"/>
+    </row>
+    <row r="97" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A97" s="56">
         <v>85</v>
       </c>
@@ -6221,7 +6330,7 @@
       <c r="C97" s="19" t="s">
         <v>189</v>
       </c>
-      <c r="D97" s="130" t="s">
+      <c r="D97" s="129" t="s">
         <v>435</v>
       </c>
       <c r="E97" s="71" t="s">
@@ -6244,8 +6353,9 @@
       <c r="N97" s="58" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="98" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O97" s="58"/>
+    </row>
+    <row r="98" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A98" s="56">
         <v>86</v>
       </c>
@@ -6255,7 +6365,7 @@
       <c r="C98" s="19" t="s">
         <v>189</v>
       </c>
-      <c r="D98" s="130" t="s">
+      <c r="D98" s="129" t="s">
         <v>436</v>
       </c>
       <c r="E98" s="71" t="s">
@@ -6278,8 +6388,9 @@
       <c r="N98" s="58" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="99" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O98" s="58"/>
+    </row>
+    <row r="99" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A99" s="56">
         <v>87</v>
       </c>
@@ -6289,7 +6400,7 @@
       <c r="C99" s="19" t="s">
         <v>189</v>
       </c>
-      <c r="D99" s="130" t="s">
+      <c r="D99" s="129" t="s">
         <v>437</v>
       </c>
       <c r="E99" s="2" t="s">
@@ -6312,8 +6423,9 @@
       <c r="N99" s="58" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="100" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O99" s="58"/>
+    </row>
+    <row r="100" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A100" s="56">
         <v>88</v>
       </c>
@@ -6323,7 +6435,7 @@
       <c r="C100" s="19" t="s">
         <v>189</v>
       </c>
-      <c r="D100" s="130" t="s">
+      <c r="D100" s="129" t="s">
         <v>438</v>
       </c>
       <c r="E100" s="2" t="s">
@@ -6346,8 +6458,9 @@
       <c r="N100" s="58" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="101" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O100" s="58"/>
+    </row>
+    <row r="101" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A101" s="56">
         <v>89</v>
       </c>
@@ -6357,7 +6470,7 @@
       <c r="C101" s="19" t="s">
         <v>189</v>
       </c>
-      <c r="D101" s="130" t="s">
+      <c r="D101" s="129" t="s">
         <v>439</v>
       </c>
       <c r="E101" s="2" t="s">
@@ -6380,8 +6493,9 @@
       <c r="N101" s="58" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="102" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O101" s="58"/>
+    </row>
+    <row r="102" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A102" s="56">
         <v>90</v>
       </c>
@@ -6391,7 +6505,7 @@
       <c r="C102" s="19" t="s">
         <v>189</v>
       </c>
-      <c r="D102" s="130" t="s">
+      <c r="D102" s="129" t="s">
         <v>440</v>
       </c>
       <c r="E102" s="2" t="s">
@@ -6414,8 +6528,9 @@
       <c r="N102" s="58" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="103" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O102" s="58"/>
+    </row>
+    <row r="103" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A103" s="56">
         <v>91</v>
       </c>
@@ -6425,7 +6540,7 @@
       <c r="C103" s="19" t="s">
         <v>189</v>
       </c>
-      <c r="D103" s="130" t="s">
+      <c r="D103" s="129" t="s">
         <v>441</v>
       </c>
       <c r="E103" s="2" t="s">
@@ -6448,8 +6563,9 @@
       <c r="N103" s="58" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="104" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O103" s="58"/>
+    </row>
+    <row r="104" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A104" s="56">
         <v>92</v>
       </c>
@@ -6459,7 +6575,7 @@
       <c r="C104" s="19" t="s">
         <v>189</v>
       </c>
-      <c r="D104" s="130" t="s">
+      <c r="D104" s="129" t="s">
         <v>442</v>
       </c>
       <c r="E104" s="2" t="s">
@@ -6482,8 +6598,9 @@
       <c r="N104" s="58" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="105" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O104" s="58"/>
+    </row>
+    <row r="105" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A105" s="56">
         <v>93</v>
       </c>
@@ -6493,7 +6610,7 @@
       <c r="C105" s="19" t="s">
         <v>189</v>
       </c>
-      <c r="D105" s="132" t="s">
+      <c r="D105" s="131" t="s">
         <v>443</v>
       </c>
       <c r="E105" s="4" t="s">
@@ -6516,8 +6633,9 @@
       <c r="N105" s="58" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="106" spans="1:14" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O105" s="58"/>
+    </row>
+    <row r="106" spans="1:15" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A106" s="59">
         <v>94</v>
       </c>
@@ -6527,7 +6645,7 @@
       <c r="C106" s="22" t="s">
         <v>189</v>
       </c>
-      <c r="D106" s="134" t="s">
+      <c r="D106" s="133" t="s">
         <v>444</v>
       </c>
       <c r="E106" s="76" t="s">
@@ -6550,8 +6668,9 @@
       <c r="N106" s="60" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="107" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O106" s="60"/>
+    </row>
+    <row r="107" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A107" s="77">
         <v>95</v>
       </c>
@@ -6561,7 +6680,7 @@
       <c r="C107" s="102" t="s">
         <v>212</v>
       </c>
-      <c r="D107" s="135" t="s">
+      <c r="D107" s="134" t="s">
         <v>213</v>
       </c>
       <c r="E107" s="92" t="s">
@@ -6584,8 +6703,9 @@
         <v>456</v>
       </c>
       <c r="N107" s="79"/>
-    </row>
-    <row r="108" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O107" s="79"/>
+    </row>
+    <row r="108" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A108" s="75">
         <v>96</v>
       </c>
@@ -6595,7 +6715,7 @@
       <c r="C108" s="103" t="s">
         <v>212</v>
       </c>
-      <c r="D108" s="136" t="s">
+      <c r="D108" s="135" t="s">
         <v>215</v>
       </c>
       <c r="E108" s="94" t="s">
@@ -6618,8 +6738,9 @@
         <v>456</v>
       </c>
       <c r="N108" s="62"/>
-    </row>
-    <row r="109" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O108" s="62"/>
+    </row>
+    <row r="109" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A109" s="75">
         <v>97</v>
       </c>
@@ -6629,7 +6750,7 @@
       <c r="C109" s="103" t="s">
         <v>212</v>
       </c>
-      <c r="D109" s="136" t="s">
+      <c r="D109" s="135" t="s">
         <v>217</v>
       </c>
       <c r="E109" s="93" t="s">
@@ -6652,8 +6773,9 @@
         <v>456</v>
       </c>
       <c r="N109" s="62"/>
-    </row>
-    <row r="110" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O109" s="62"/>
+    </row>
+    <row r="110" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A110" s="75">
         <v>98</v>
       </c>
@@ -6663,7 +6785,7 @@
       <c r="C110" s="103" t="s">
         <v>212</v>
       </c>
-      <c r="D110" s="136" t="s">
+      <c r="D110" s="135" t="s">
         <v>219</v>
       </c>
       <c r="E110" s="93" t="s">
@@ -6684,8 +6806,9 @@
         <v>456</v>
       </c>
       <c r="N110" s="62"/>
-    </row>
-    <row r="111" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O110" s="62"/>
+    </row>
+    <row r="111" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A111" s="75">
         <v>99</v>
       </c>
@@ -6695,7 +6818,7 @@
       <c r="C111" s="103" t="s">
         <v>212</v>
       </c>
-      <c r="D111" s="136" t="s">
+      <c r="D111" s="135" t="s">
         <v>220</v>
       </c>
       <c r="E111" s="94" t="s">
@@ -6716,8 +6839,9 @@
         <v>456</v>
       </c>
       <c r="N111" s="62"/>
-    </row>
-    <row r="112" spans="1:14" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O111" s="62"/>
+    </row>
+    <row r="112" spans="1:15" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A112" s="52">
         <v>100</v>
       </c>
@@ -6727,7 +6851,7 @@
       <c r="C112" s="104" t="s">
         <v>212</v>
       </c>
-      <c r="D112" s="137" t="s">
+      <c r="D112" s="136" t="s">
         <v>221</v>
       </c>
       <c r="E112" s="95" t="s">
@@ -6748,8 +6872,9 @@
         <v>456</v>
       </c>
       <c r="N112" s="81"/>
-    </row>
-    <row r="113" spans="1:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="O112" s="81"/>
+    </row>
+    <row r="113" spans="1:15" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
       <c r="A113" s="75">
         <v>101</v>
       </c>
@@ -6759,7 +6884,7 @@
       <c r="C113" s="19" t="s">
         <v>180</v>
       </c>
-      <c r="D113" s="130" t="s">
+      <c r="D113" s="129" t="s">
         <v>185</v>
       </c>
       <c r="E113" s="71" t="s">
@@ -6780,8 +6905,9 @@
         <v>456</v>
       </c>
       <c r="N113" s="34"/>
-    </row>
-    <row r="114" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O113" s="34"/>
+    </row>
+    <row r="114" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A114" s="75">
         <v>102</v>
       </c>
@@ -6791,7 +6917,7 @@
       <c r="C114" s="19" t="s">
         <v>180</v>
       </c>
-      <c r="D114" s="130" t="s">
+      <c r="D114" s="129" t="s">
         <v>186</v>
       </c>
       <c r="E114" s="71" t="s">
@@ -6812,8 +6938,9 @@
         <v>456</v>
       </c>
       <c r="N114" s="34"/>
-    </row>
-    <row r="115" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O114" s="34"/>
+    </row>
+    <row r="115" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A115" s="75">
         <v>103</v>
       </c>
@@ -6823,7 +6950,7 @@
       <c r="C115" s="19" t="s">
         <v>180</v>
       </c>
-      <c r="D115" s="130" t="s">
+      <c r="D115" s="129" t="s">
         <v>187</v>
       </c>
       <c r="E115" s="71" t="s">
@@ -6846,8 +6973,9 @@
         <v>456</v>
       </c>
       <c r="N115" s="34"/>
-    </row>
-    <row r="116" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O115" s="34"/>
+    </row>
+    <row r="116" spans="1:15" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A116" s="52">
         <v>104</v>
       </c>
@@ -6857,7 +6985,7 @@
       <c r="C116" s="101" t="s">
         <v>180</v>
       </c>
-      <c r="D116" s="131" t="s">
+      <c r="D116" s="130" t="s">
         <v>188</v>
       </c>
       <c r="E116" s="84" t="s">
@@ -6880,8 +7008,9 @@
         <v>456</v>
       </c>
       <c r="N116" s="85"/>
-    </row>
-    <row r="117" spans="1:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="O116" s="85"/>
+    </row>
+    <row r="117" spans="1:15" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
       <c r="A117" s="61">
         <v>105</v>
       </c>
@@ -6914,8 +7043,9 @@
       <c r="N117" s="62" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="118" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O117" s="62"/>
+    </row>
+    <row r="118" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A118" s="61">
         <v>106</v>
       </c>
@@ -6948,8 +7078,9 @@
       <c r="N118" s="63" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="119" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O118" s="63"/>
+    </row>
+    <row r="119" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A119" s="61">
         <v>107</v>
       </c>
@@ -6982,8 +7113,9 @@
       <c r="N119" s="63" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="120" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O119" s="63"/>
+    </row>
+    <row r="120" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A120" s="61">
         <v>108</v>
       </c>
@@ -7016,8 +7148,9 @@
       <c r="N120" s="63" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="121" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O120" s="63"/>
+    </row>
+    <row r="121" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A121" s="61">
         <v>109</v>
       </c>
@@ -7050,8 +7183,9 @@
       <c r="N121" s="63" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="122" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O121" s="63"/>
+    </row>
+    <row r="122" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A122" s="61">
         <v>110</v>
       </c>
@@ -7084,8 +7218,9 @@
       <c r="N122" s="63" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="123" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O122" s="63"/>
+    </row>
+    <row r="123" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A123" s="61">
         <v>111</v>
       </c>
@@ -7118,8 +7253,9 @@
       <c r="N123" s="63" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="124" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O123" s="63"/>
+    </row>
+    <row r="124" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A124" s="61">
         <v>112</v>
       </c>
@@ -7152,8 +7288,9 @@
       <c r="N124" s="63" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="125" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O124" s="63"/>
+    </row>
+    <row r="125" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A125" s="61">
         <v>113</v>
       </c>
@@ -7186,8 +7323,9 @@
       <c r="N125" s="63" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="126" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O125" s="63"/>
+    </row>
+    <row r="126" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A126" s="61">
         <v>114</v>
       </c>
@@ -7220,8 +7358,9 @@
       <c r="N126" s="63" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="127" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O126" s="63"/>
+    </row>
+    <row r="127" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A127" s="61">
         <v>115</v>
       </c>
@@ -7254,8 +7393,9 @@
       <c r="N127" s="63" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="128" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O127" s="63"/>
+    </row>
+    <row r="128" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A128" s="61">
         <v>116</v>
       </c>
@@ -7288,8 +7428,9 @@
       <c r="N128" s="63" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="129" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O128" s="63"/>
+    </row>
+    <row r="129" spans="1:15" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A129" s="52">
         <v>117</v>
       </c>
@@ -7299,7 +7440,7 @@
       <c r="C129" s="104" t="s">
         <v>190</v>
       </c>
-      <c r="D129" s="138" t="s">
+      <c r="D129" s="137" t="s">
         <v>431</v>
       </c>
       <c r="E129" s="7" t="s">
@@ -7322,8 +7463,9 @@
       <c r="N129" s="64" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="130" spans="1:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="O129" s="64"/>
+    </row>
+    <row r="130" spans="1:15" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
       <c r="A130" s="61">
         <v>118</v>
       </c>
@@ -7356,8 +7498,9 @@
       <c r="N130" s="62" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="131" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O130" s="62"/>
+    </row>
+    <row r="131" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A131" s="61">
         <v>119</v>
       </c>
@@ -7390,8 +7533,9 @@
       <c r="N131" s="63" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="132" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O131" s="63"/>
+    </row>
+    <row r="132" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A132" s="61">
         <v>120</v>
       </c>
@@ -7424,8 +7568,9 @@
       <c r="N132" s="63" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="133" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O132" s="63"/>
+    </row>
+    <row r="133" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A133" s="61">
         <v>121</v>
       </c>
@@ -7458,8 +7603,9 @@
       <c r="N133" s="63" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="134" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O133" s="63"/>
+    </row>
+    <row r="134" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A134" s="61">
         <v>122</v>
       </c>
@@ -7492,8 +7638,9 @@
       <c r="N134" s="63" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="135" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O134" s="63"/>
+    </row>
+    <row r="135" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A135" s="61">
         <v>123</v>
       </c>
@@ -7526,8 +7673,9 @@
       <c r="N135" s="63" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="136" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O135" s="63"/>
+    </row>
+    <row r="136" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A136" s="61">
         <v>124</v>
       </c>
@@ -7560,8 +7708,9 @@
       <c r="N136" s="63" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="137" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O136" s="63"/>
+    </row>
+    <row r="137" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A137" s="61">
         <v>125</v>
       </c>
@@ -7594,8 +7743,9 @@
       <c r="N137" s="63" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="138" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O137" s="63"/>
+    </row>
+    <row r="138" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A138" s="61">
         <v>126</v>
       </c>
@@ -7628,8 +7778,9 @@
       <c r="N138" s="63" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="139" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O138" s="63"/>
+    </row>
+    <row r="139" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A139" s="61">
         <v>127</v>
       </c>
@@ -7662,8 +7813,9 @@
       <c r="N139" s="63" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="140" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O139" s="63"/>
+    </row>
+    <row r="140" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A140" s="61">
         <v>128</v>
       </c>
@@ -7696,8 +7848,9 @@
       <c r="N140" s="63" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="141" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O140" s="63"/>
+    </row>
+    <row r="141" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A141" s="61">
         <v>129</v>
       </c>
@@ -7730,8 +7883,9 @@
       <c r="N141" s="63" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="142" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O141" s="63"/>
+    </row>
+    <row r="142" spans="1:15" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A142" s="59">
         <v>130</v>
       </c>
@@ -7764,8 +7918,9 @@
       <c r="N142" s="65" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="143" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O142" s="65"/>
+    </row>
+    <row r="143" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A143" s="113">
         <v>131</v>
       </c>
@@ -7775,7 +7930,7 @@
       <c r="C143" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="D143" s="130" t="s">
+      <c r="D143" s="129" t="s">
         <v>336</v>
       </c>
       <c r="E143" s="2" t="s">
@@ -7800,8 +7955,9 @@
       <c r="N143" s="66" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="144" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O143" s="66"/>
+    </row>
+    <row r="144" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A144" s="113">
         <v>132</v>
       </c>
@@ -7811,7 +7967,7 @@
       <c r="C144" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="D144" s="130" t="s">
+      <c r="D144" s="129" t="s">
         <v>254</v>
       </c>
       <c r="E144" s="2" t="s">
@@ -7834,8 +7990,9 @@
       <c r="N144" s="66" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="145" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O144" s="66"/>
+    </row>
+    <row r="145" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A145" s="113">
         <v>133</v>
       </c>
@@ -7845,7 +8002,7 @@
       <c r="C145" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="D145" s="130" t="s">
+      <c r="D145" s="129" t="s">
         <v>255</v>
       </c>
       <c r="E145" s="2" t="s">
@@ -7868,8 +8025,9 @@
       <c r="N145" s="66" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="146" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O145" s="66"/>
+    </row>
+    <row r="146" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A146" s="113">
         <v>134</v>
       </c>
@@ -7879,7 +8037,7 @@
       <c r="C146" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="D146" s="130" t="s">
+      <c r="D146" s="129" t="s">
         <v>256</v>
       </c>
       <c r="E146" s="2" t="s">
@@ -7902,8 +8060,9 @@
       <c r="N146" s="66" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="147" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O146" s="66"/>
+    </row>
+    <row r="147" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A147" s="113">
         <v>135</v>
       </c>
@@ -7913,7 +8072,7 @@
       <c r="C147" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="D147" s="130" t="s">
+      <c r="D147" s="129" t="s">
         <v>257</v>
       </c>
       <c r="E147" s="2" t="s">
@@ -7936,8 +8095,9 @@
       <c r="N147" s="66" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="148" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O147" s="66"/>
+    </row>
+    <row r="148" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A148" s="113">
         <v>136</v>
       </c>
@@ -7947,7 +8107,7 @@
       <c r="C148" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="D148" s="130" t="s">
+      <c r="D148" s="129" t="s">
         <v>258</v>
       </c>
       <c r="E148" s="2" t="s">
@@ -7970,8 +8130,9 @@
       <c r="N148" s="66" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="149" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O148" s="66"/>
+    </row>
+    <row r="149" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A149" s="113">
         <v>137</v>
       </c>
@@ -7981,7 +8142,7 @@
       <c r="C149" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="D149" s="130" t="s">
+      <c r="D149" s="129" t="s">
         <v>259</v>
       </c>
       <c r="E149" s="2" t="s">
@@ -8004,8 +8165,9 @@
       <c r="N149" s="66" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="150" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O149" s="66"/>
+    </row>
+    <row r="150" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A150" s="113">
         <v>138</v>
       </c>
@@ -8015,7 +8177,7 @@
       <c r="C150" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="D150" s="130" t="s">
+      <c r="D150" s="129" t="s">
         <v>260</v>
       </c>
       <c r="E150" s="2" t="s">
@@ -8038,8 +8200,9 @@
       <c r="N150" s="66" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="151" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O150" s="66"/>
+    </row>
+    <row r="151" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A151" s="113">
         <v>139</v>
       </c>
@@ -8049,7 +8212,7 @@
       <c r="C151" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="D151" s="130" t="s">
+      <c r="D151" s="129" t="s">
         <v>261</v>
       </c>
       <c r="E151" s="2" t="s">
@@ -8072,8 +8235,9 @@
       <c r="N151" s="66" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="152" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O151" s="66"/>
+    </row>
+    <row r="152" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A152" s="113">
         <v>140</v>
       </c>
@@ -8083,7 +8247,7 @@
       <c r="C152" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="D152" s="130" t="s">
+      <c r="D152" s="129" t="s">
         <v>262</v>
       </c>
       <c r="E152" s="2" t="s">
@@ -8106,8 +8270,9 @@
       <c r="N152" s="66" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="153" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O152" s="66"/>
+    </row>
+    <row r="153" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A153" s="113">
         <v>141</v>
       </c>
@@ -8117,7 +8282,7 @@
       <c r="C153" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="D153" s="130" t="s">
+      <c r="D153" s="129" t="s">
         <v>263</v>
       </c>
       <c r="E153" s="2" t="s">
@@ -8140,8 +8305,9 @@
       <c r="N153" s="66" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="154" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O153" s="66"/>
+    </row>
+    <row r="154" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A154" s="113">
         <v>142</v>
       </c>
@@ -8151,7 +8317,7 @@
       <c r="C154" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="D154" s="130" t="s">
+      <c r="D154" s="129" t="s">
         <v>264</v>
       </c>
       <c r="E154" s="2" t="s">
@@ -8174,8 +8340,9 @@
       <c r="N154" s="66" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="155" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O154" s="66"/>
+    </row>
+    <row r="155" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A155" s="113">
         <v>143</v>
       </c>
@@ -8185,7 +8352,7 @@
       <c r="C155" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="D155" s="130" t="s">
+      <c r="D155" s="129" t="s">
         <v>265</v>
       </c>
       <c r="E155" s="2" t="s">
@@ -8208,8 +8375,9 @@
       <c r="N155" s="66" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="156" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O155" s="66"/>
+    </row>
+    <row r="156" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A156" s="113">
         <v>144</v>
       </c>
@@ -8219,7 +8387,7 @@
       <c r="C156" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="D156" s="130" t="s">
+      <c r="D156" s="129" t="s">
         <v>266</v>
       </c>
       <c r="E156" s="2" t="s">
@@ -8242,8 +8410,9 @@
       <c r="N156" s="66" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="157" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O156" s="66"/>
+    </row>
+    <row r="157" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A157" s="113">
         <v>145</v>
       </c>
@@ -8253,7 +8422,7 @@
       <c r="C157" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="D157" s="130" t="s">
+      <c r="D157" s="129" t="s">
         <v>267</v>
       </c>
       <c r="E157" s="2" t="s">
@@ -8276,8 +8445,9 @@
       <c r="N157" s="66" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="158" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O157" s="66"/>
+    </row>
+    <row r="158" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A158" s="113">
         <v>146</v>
       </c>
@@ -8287,7 +8457,7 @@
       <c r="C158" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="D158" s="130" t="s">
+      <c r="D158" s="129" t="s">
         <v>268</v>
       </c>
       <c r="E158" s="2" t="s">
@@ -8310,8 +8480,9 @@
       <c r="N158" s="66" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="159" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O158" s="66"/>
+    </row>
+    <row r="159" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A159" s="113">
         <v>147</v>
       </c>
@@ -8321,7 +8492,7 @@
       <c r="C159" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="D159" s="130" t="s">
+      <c r="D159" s="129" t="s">
         <v>269</v>
       </c>
       <c r="E159" s="2" t="s">
@@ -8344,8 +8515,9 @@
       <c r="N159" s="66" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="160" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O159" s="66"/>
+    </row>
+    <row r="160" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A160" s="113">
         <v>148</v>
       </c>
@@ -8355,7 +8527,7 @@
       <c r="C160" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="D160" s="130" t="s">
+      <c r="D160" s="129" t="s">
         <v>270</v>
       </c>
       <c r="E160" s="2" t="s">
@@ -8378,8 +8550,9 @@
       <c r="N160" s="66" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="161" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O160" s="66"/>
+    </row>
+    <row r="161" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A161" s="113">
         <v>149</v>
       </c>
@@ -8389,7 +8562,7 @@
       <c r="C161" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="D161" s="130" t="s">
+      <c r="D161" s="129" t="s">
         <v>271</v>
       </c>
       <c r="E161" s="2" t="s">
@@ -8412,8 +8585,9 @@
       <c r="N161" s="66" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="162" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O161" s="66"/>
+    </row>
+    <row r="162" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A162" s="113">
         <v>150</v>
       </c>
@@ -8423,7 +8597,7 @@
       <c r="C162" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="D162" s="130" t="s">
+      <c r="D162" s="129" t="s">
         <v>272</v>
       </c>
       <c r="E162" s="2" t="s">
@@ -8446,8 +8620,9 @@
       <c r="N162" s="66" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="163" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O162" s="66"/>
+    </row>
+    <row r="163" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A163" s="113">
         <v>151</v>
       </c>
@@ -8457,7 +8632,7 @@
       <c r="C163" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="D163" s="130" t="s">
+      <c r="D163" s="129" t="s">
         <v>273</v>
       </c>
       <c r="E163" s="2" t="s">
@@ -8480,8 +8655,9 @@
       <c r="N163" s="66" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="164" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O163" s="66"/>
+    </row>
+    <row r="164" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A164" s="113">
         <v>152</v>
       </c>
@@ -8491,7 +8667,7 @@
       <c r="C164" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="D164" s="130" t="s">
+      <c r="D164" s="129" t="s">
         <v>274</v>
       </c>
       <c r="E164" s="2" t="s">
@@ -8514,8 +8690,9 @@
       <c r="N164" s="66" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="165" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O164" s="66"/>
+    </row>
+    <row r="165" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A165" s="113">
         <v>153</v>
       </c>
@@ -8525,7 +8702,7 @@
       <c r="C165" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="D165" s="130" t="s">
+      <c r="D165" s="129" t="s">
         <v>275</v>
       </c>
       <c r="E165" s="2" t="s">
@@ -8548,8 +8725,9 @@
       <c r="N165" s="66" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="166" spans="1:14" s="83" customFormat="1" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O165" s="66"/>
+    </row>
+    <row r="166" spans="1:15" s="83" customFormat="1" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A166" s="114">
         <v>154</v>
       </c>
@@ -8559,7 +8737,7 @@
       <c r="C166" s="88" t="s">
         <v>252</v>
       </c>
-      <c r="D166" s="139" t="s">
+      <c r="D166" s="138" t="s">
         <v>276</v>
       </c>
       <c r="E166" s="86" t="s">
@@ -8582,8 +8760,9 @@
       <c r="N166" s="68" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="167" spans="1:14" ht="14.45" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="O166" s="68"/>
+    </row>
+    <row r="167" spans="1:15" ht="14.45" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
       <c r="A167" s="113">
         <v>155</v>
       </c>
@@ -8593,7 +8772,7 @@
       <c r="C167" s="5" t="s">
         <v>293</v>
       </c>
-      <c r="D167" s="130" t="s">
+      <c r="D167" s="129" t="s">
         <v>337</v>
       </c>
       <c r="E167" s="2" t="s">
@@ -8618,8 +8797,9 @@
       <c r="N167" s="66" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="168" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O167" s="66"/>
+    </row>
+    <row r="168" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A168" s="113">
         <v>156</v>
       </c>
@@ -8629,7 +8809,7 @@
       <c r="C168" s="5" t="s">
         <v>293</v>
       </c>
-      <c r="D168" s="130" t="s">
+      <c r="D168" s="129" t="s">
         <v>294</v>
       </c>
       <c r="E168" s="2" t="s">
@@ -8652,8 +8832,9 @@
       <c r="N168" s="66" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="169" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O168" s="66"/>
+    </row>
+    <row r="169" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A169" s="113">
         <v>157</v>
       </c>
@@ -8663,7 +8844,7 @@
       <c r="C169" s="5" t="s">
         <v>293</v>
       </c>
-      <c r="D169" s="130" t="s">
+      <c r="D169" s="129" t="s">
         <v>296</v>
       </c>
       <c r="E169" s="2" t="s">
@@ -8686,8 +8867,9 @@
       <c r="N169" s="66" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="170" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O169" s="66"/>
+    </row>
+    <row r="170" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A170" s="113">
         <v>158</v>
       </c>
@@ -8697,7 +8879,7 @@
       <c r="C170" s="5" t="s">
         <v>293</v>
       </c>
-      <c r="D170" s="130" t="s">
+      <c r="D170" s="129" t="s">
         <v>297</v>
       </c>
       <c r="E170" s="2" t="s">
@@ -8720,8 +8902,9 @@
       <c r="N170" s="66" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="171" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O170" s="66"/>
+    </row>
+    <row r="171" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A171" s="113">
         <v>159</v>
       </c>
@@ -8731,7 +8914,7 @@
       <c r="C171" s="5" t="s">
         <v>293</v>
       </c>
-      <c r="D171" s="130" t="s">
+      <c r="D171" s="129" t="s">
         <v>299</v>
       </c>
       <c r="E171" s="2" t="s">
@@ -8754,8 +8937,9 @@
       <c r="N171" s="66" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="172" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O171" s="66"/>
+    </row>
+    <row r="172" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A172" s="113">
         <v>160</v>
       </c>
@@ -8765,7 +8949,7 @@
       <c r="C172" s="5" t="s">
         <v>293</v>
       </c>
-      <c r="D172" s="130" t="s">
+      <c r="D172" s="129" t="s">
         <v>301</v>
       </c>
       <c r="E172" s="2" t="s">
@@ -8788,8 +8972,9 @@
       <c r="N172" s="66" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="173" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O172" s="66"/>
+    </row>
+    <row r="173" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A173" s="113">
         <v>161</v>
       </c>
@@ -8799,7 +8984,7 @@
       <c r="C173" s="5" t="s">
         <v>293</v>
       </c>
-      <c r="D173" s="130" t="s">
+      <c r="D173" s="129" t="s">
         <v>303</v>
       </c>
       <c r="E173" s="2" t="s">
@@ -8822,8 +9007,9 @@
       <c r="N173" s="66" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="174" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O173" s="66"/>
+    </row>
+    <row r="174" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A174" s="113">
         <v>162</v>
       </c>
@@ -8833,7 +9019,7 @@
       <c r="C174" s="5" t="s">
         <v>293</v>
       </c>
-      <c r="D174" s="130" t="s">
+      <c r="D174" s="129" t="s">
         <v>304</v>
       </c>
       <c r="E174" s="2" t="s">
@@ -8856,8 +9042,9 @@
       <c r="N174" s="66" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="175" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O174" s="66"/>
+    </row>
+    <row r="175" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A175" s="113">
         <v>163</v>
       </c>
@@ -8867,7 +9054,7 @@
       <c r="C175" s="5" t="s">
         <v>293</v>
       </c>
-      <c r="D175" s="130" t="s">
+      <c r="D175" s="129" t="s">
         <v>306</v>
       </c>
       <c r="E175" s="2" t="s">
@@ -8890,8 +9077,9 @@
       <c r="N175" s="66" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="176" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O175" s="66"/>
+    </row>
+    <row r="176" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A176" s="113">
         <v>164</v>
       </c>
@@ -8901,7 +9089,7 @@
       <c r="C176" s="5" t="s">
         <v>293</v>
       </c>
-      <c r="D176" s="130" t="s">
+      <c r="D176" s="129" t="s">
         <v>308</v>
       </c>
       <c r="E176" s="2" t="s">
@@ -8924,8 +9112,9 @@
       <c r="N176" s="66" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="177" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O176" s="66"/>
+    </row>
+    <row r="177" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A177" s="113">
         <v>165</v>
       </c>
@@ -8935,7 +9124,7 @@
       <c r="C177" s="5" t="s">
         <v>293</v>
       </c>
-      <c r="D177" s="130" t="s">
+      <c r="D177" s="129" t="s">
         <v>309</v>
       </c>
       <c r="E177" s="2" t="s">
@@ -8958,8 +9147,9 @@
       <c r="N177" s="66" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="178" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O177" s="66"/>
+    </row>
+    <row r="178" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A178" s="113">
         <v>166</v>
       </c>
@@ -8969,7 +9159,7 @@
       <c r="C178" s="5" t="s">
         <v>293</v>
       </c>
-      <c r="D178" s="130" t="s">
+      <c r="D178" s="129" t="s">
         <v>311</v>
       </c>
       <c r="E178" s="2" t="s">
@@ -8992,8 +9182,9 @@
       <c r="N178" s="66" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="179" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O178" s="66"/>
+    </row>
+    <row r="179" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A179" s="113">
         <v>167</v>
       </c>
@@ -9003,7 +9194,7 @@
       <c r="C179" s="5" t="s">
         <v>293</v>
       </c>
-      <c r="D179" s="130" t="s">
+      <c r="D179" s="129" t="s">
         <v>313</v>
       </c>
       <c r="E179" s="2" t="s">
@@ -9026,8 +9217,9 @@
       <c r="N179" s="66" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="180" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O179" s="66"/>
+    </row>
+    <row r="180" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A180" s="113">
         <v>168</v>
       </c>
@@ -9037,7 +9229,7 @@
       <c r="C180" s="5" t="s">
         <v>293</v>
       </c>
-      <c r="D180" s="130" t="s">
+      <c r="D180" s="129" t="s">
         <v>314</v>
       </c>
       <c r="E180" s="2" t="s">
@@ -9060,8 +9252,9 @@
       <c r="N180" s="66" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="181" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O180" s="66"/>
+    </row>
+    <row r="181" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A181" s="113">
         <v>169</v>
       </c>
@@ -9071,7 +9264,7 @@
       <c r="C181" s="5" t="s">
         <v>293</v>
       </c>
-      <c r="D181" s="130" t="s">
+      <c r="D181" s="129" t="s">
         <v>316</v>
       </c>
       <c r="E181" s="2" t="s">
@@ -9094,8 +9287,9 @@
       <c r="N181" s="66" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="182" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O181" s="66"/>
+    </row>
+    <row r="182" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A182" s="113">
         <v>170</v>
       </c>
@@ -9105,7 +9299,7 @@
       <c r="C182" s="5" t="s">
         <v>293</v>
       </c>
-      <c r="D182" s="130" t="s">
+      <c r="D182" s="129" t="s">
         <v>318</v>
       </c>
       <c r="E182" s="2" t="s">
@@ -9128,8 +9322,9 @@
       <c r="N182" s="66" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="183" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O182" s="66"/>
+    </row>
+    <row r="183" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A183" s="113">
         <v>171</v>
       </c>
@@ -9139,7 +9334,7 @@
       <c r="C183" s="5" t="s">
         <v>293</v>
       </c>
-      <c r="D183" s="130" t="s">
+      <c r="D183" s="129" t="s">
         <v>319</v>
       </c>
       <c r="E183" s="2" t="s">
@@ -9162,8 +9357,9 @@
       <c r="N183" s="66" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="184" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O183" s="66"/>
+    </row>
+    <row r="184" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A184" s="113">
         <v>172</v>
       </c>
@@ -9173,7 +9369,7 @@
       <c r="C184" s="5" t="s">
         <v>293</v>
       </c>
-      <c r="D184" s="130" t="s">
+      <c r="D184" s="129" t="s">
         <v>321</v>
       </c>
       <c r="E184" s="2" t="s">
@@ -9196,8 +9392,9 @@
       <c r="N184" s="66" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="185" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O184" s="66"/>
+    </row>
+    <row r="185" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A185" s="113">
         <v>173</v>
       </c>
@@ -9207,7 +9404,7 @@
       <c r="C185" s="5" t="s">
         <v>293</v>
       </c>
-      <c r="D185" s="130" t="s">
+      <c r="D185" s="129" t="s">
         <v>323</v>
       </c>
       <c r="E185" s="2" t="s">
@@ -9230,8 +9427,9 @@
       <c r="N185" s="66" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="186" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O185" s="66"/>
+    </row>
+    <row r="186" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A186" s="113">
         <v>174</v>
       </c>
@@ -9241,7 +9439,7 @@
       <c r="C186" s="5" t="s">
         <v>293</v>
       </c>
-      <c r="D186" s="130" t="s">
+      <c r="D186" s="129" t="s">
         <v>324</v>
       </c>
       <c r="E186" s="2" t="s">
@@ -9264,8 +9462,9 @@
       <c r="N186" s="66" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="187" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O186" s="66"/>
+    </row>
+    <row r="187" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A187" s="113">
         <v>175</v>
       </c>
@@ -9275,7 +9474,7 @@
       <c r="C187" s="5" t="s">
         <v>293</v>
       </c>
-      <c r="D187" s="130" t="s">
+      <c r="D187" s="129" t="s">
         <v>326</v>
       </c>
       <c r="E187" s="2" t="s">
@@ -9298,8 +9497,9 @@
       <c r="N187" s="66" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="188" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O187" s="66"/>
+    </row>
+    <row r="188" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A188" s="113">
         <v>176</v>
       </c>
@@ -9309,7 +9509,7 @@
       <c r="C188" s="5" t="s">
         <v>293</v>
       </c>
-      <c r="D188" s="130" t="s">
+      <c r="D188" s="129" t="s">
         <v>328</v>
       </c>
       <c r="E188" s="2" t="s">
@@ -9332,8 +9532,9 @@
       <c r="N188" s="66" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="189" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O188" s="66"/>
+    </row>
+    <row r="189" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A189" s="113">
         <v>177</v>
       </c>
@@ -9343,7 +9544,7 @@
       <c r="C189" s="5" t="s">
         <v>293</v>
       </c>
-      <c r="D189" s="130" t="s">
+      <c r="D189" s="129" t="s">
         <v>329</v>
       </c>
       <c r="E189" s="2" t="s">
@@ -9366,8 +9567,9 @@
       <c r="N189" s="66" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="190" spans="1:14" s="83" customFormat="1" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O189" s="66"/>
+    </row>
+    <row r="190" spans="1:15" s="83" customFormat="1" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A190" s="114">
         <v>178</v>
       </c>
@@ -9377,7 +9579,7 @@
       <c r="C190" s="88" t="s">
         <v>293</v>
       </c>
-      <c r="D190" s="139" t="s">
+      <c r="D190" s="138" t="s">
         <v>331</v>
       </c>
       <c r="E190" s="86" t="s">
@@ -9400,8 +9602,9 @@
       <c r="N190" s="68" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="191" spans="1:14" ht="14.45" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="O190" s="68"/>
+    </row>
+    <row r="191" spans="1:15" ht="14.45" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
       <c r="A191" s="113">
         <v>179</v>
       </c>
@@ -9411,7 +9614,7 @@
       <c r="C191" s="5" t="s">
         <v>334</v>
       </c>
-      <c r="D191" s="130" t="s">
+      <c r="D191" s="129" t="s">
         <v>338</v>
       </c>
       <c r="E191" s="2" t="s">
@@ -9436,8 +9639,9 @@
       <c r="N191" s="66" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="192" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O191" s="66"/>
+    </row>
+    <row r="192" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A192" s="113">
         <v>180</v>
       </c>
@@ -9447,7 +9651,7 @@
       <c r="C192" s="5" t="s">
         <v>334</v>
       </c>
-      <c r="D192" s="130" t="s">
+      <c r="D192" s="129" t="s">
         <v>341</v>
       </c>
       <c r="E192" s="2" t="s">
@@ -9470,8 +9674,9 @@
       <c r="N192" s="66" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="193" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O192" s="66"/>
+    </row>
+    <row r="193" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A193" s="113">
         <v>181</v>
       </c>
@@ -9481,7 +9686,7 @@
       <c r="C193" s="5" t="s">
         <v>334</v>
       </c>
-      <c r="D193" s="130" t="s">
+      <c r="D193" s="129" t="s">
         <v>342</v>
       </c>
       <c r="E193" s="2" t="s">
@@ -9504,8 +9709,9 @@
       <c r="N193" s="66" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="194" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O193" s="66"/>
+    </row>
+    <row r="194" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A194" s="113">
         <v>182</v>
       </c>
@@ -9515,7 +9721,7 @@
       <c r="C194" s="5" t="s">
         <v>334</v>
       </c>
-      <c r="D194" s="130" t="s">
+      <c r="D194" s="129" t="s">
         <v>343</v>
       </c>
       <c r="E194" s="2" t="s">
@@ -9538,8 +9744,9 @@
       <c r="N194" s="66" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="195" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O194" s="66"/>
+    </row>
+    <row r="195" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A195" s="113">
         <v>183</v>
       </c>
@@ -9549,7 +9756,7 @@
       <c r="C195" s="5" t="s">
         <v>334</v>
       </c>
-      <c r="D195" s="130" t="s">
+      <c r="D195" s="129" t="s">
         <v>344</v>
       </c>
       <c r="E195" s="2" t="s">
@@ -9572,8 +9779,9 @@
       <c r="N195" s="66" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="196" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O195" s="66"/>
+    </row>
+    <row r="196" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A196" s="113">
         <v>184</v>
       </c>
@@ -9583,7 +9791,7 @@
       <c r="C196" s="5" t="s">
         <v>334</v>
       </c>
-      <c r="D196" s="130" t="s">
+      <c r="D196" s="129" t="s">
         <v>345</v>
       </c>
       <c r="E196" s="2" t="s">
@@ -9606,8 +9814,9 @@
       <c r="N196" s="66" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="197" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O196" s="66"/>
+    </row>
+    <row r="197" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A197" s="113">
         <v>185</v>
       </c>
@@ -9617,7 +9826,7 @@
       <c r="C197" s="5" t="s">
         <v>334</v>
       </c>
-      <c r="D197" s="130" t="s">
+      <c r="D197" s="129" t="s">
         <v>346</v>
       </c>
       <c r="E197" s="2" t="s">
@@ -9640,8 +9849,9 @@
       <c r="N197" s="66" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="198" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O197" s="66"/>
+    </row>
+    <row r="198" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A198" s="113">
         <v>186</v>
       </c>
@@ -9651,7 +9861,7 @@
       <c r="C198" s="5" t="s">
         <v>334</v>
       </c>
-      <c r="D198" s="130" t="s">
+      <c r="D198" s="129" t="s">
         <v>347</v>
       </c>
       <c r="E198" s="2" t="s">
@@ -9674,8 +9884,9 @@
       <c r="N198" s="66" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="199" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O198" s="66"/>
+    </row>
+    <row r="199" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A199" s="113">
         <v>187</v>
       </c>
@@ -9685,7 +9896,7 @@
       <c r="C199" s="5" t="s">
         <v>334</v>
       </c>
-      <c r="D199" s="130" t="s">
+      <c r="D199" s="129" t="s">
         <v>348</v>
       </c>
       <c r="E199" s="2" t="s">
@@ -9708,8 +9919,9 @@
       <c r="N199" s="66" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="200" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O199" s="66"/>
+    </row>
+    <row r="200" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A200" s="113">
         <v>188</v>
       </c>
@@ -9719,7 +9931,7 @@
       <c r="C200" s="5" t="s">
         <v>334</v>
       </c>
-      <c r="D200" s="130" t="s">
+      <c r="D200" s="129" t="s">
         <v>349</v>
       </c>
       <c r="E200" s="2" t="s">
@@ -9742,8 +9954,9 @@
       <c r="N200" s="66" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="201" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O200" s="66"/>
+    </row>
+    <row r="201" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A201" s="113">
         <v>189</v>
       </c>
@@ -9753,7 +9966,7 @@
       <c r="C201" s="5" t="s">
         <v>334</v>
       </c>
-      <c r="D201" s="130" t="s">
+      <c r="D201" s="129" t="s">
         <v>350</v>
       </c>
       <c r="E201" s="2" t="s">
@@ -9776,8 +9989,9 @@
       <c r="N201" s="66" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="202" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O201" s="66"/>
+    </row>
+    <row r="202" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A202" s="113">
         <v>190</v>
       </c>
@@ -9787,7 +10001,7 @@
       <c r="C202" s="5" t="s">
         <v>334</v>
       </c>
-      <c r="D202" s="130" t="s">
+      <c r="D202" s="129" t="s">
         <v>351</v>
       </c>
       <c r="E202" s="2" t="s">
@@ -9810,8 +10024,9 @@
       <c r="N202" s="66" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="203" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O202" s="66"/>
+    </row>
+    <row r="203" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A203" s="113">
         <v>191</v>
       </c>
@@ -9821,7 +10036,7 @@
       <c r="C203" s="5" t="s">
         <v>334</v>
       </c>
-      <c r="D203" s="130" t="s">
+      <c r="D203" s="129" t="s">
         <v>352</v>
       </c>
       <c r="E203" s="2" t="s">
@@ -9844,8 +10059,9 @@
       <c r="N203" s="66" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="204" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O203" s="66"/>
+    </row>
+    <row r="204" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A204" s="113">
         <v>192</v>
       </c>
@@ -9855,7 +10071,7 @@
       <c r="C204" s="5" t="s">
         <v>334</v>
       </c>
-      <c r="D204" s="130" t="s">
+      <c r="D204" s="129" t="s">
         <v>353</v>
       </c>
       <c r="E204" s="2" t="s">
@@ -9878,8 +10094,9 @@
       <c r="N204" s="66" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="205" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O204" s="66"/>
+    </row>
+    <row r="205" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A205" s="113">
         <v>193</v>
       </c>
@@ -9889,7 +10106,7 @@
       <c r="C205" s="5" t="s">
         <v>334</v>
       </c>
-      <c r="D205" s="130" t="s">
+      <c r="D205" s="129" t="s">
         <v>354</v>
       </c>
       <c r="E205" s="2" t="s">
@@ -9912,8 +10129,9 @@
       <c r="N205" s="66" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="206" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O205" s="66"/>
+    </row>
+    <row r="206" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A206" s="113">
         <v>194</v>
       </c>
@@ -9923,7 +10141,7 @@
       <c r="C206" s="5" t="s">
         <v>334</v>
       </c>
-      <c r="D206" s="130" t="s">
+      <c r="D206" s="129" t="s">
         <v>355</v>
       </c>
       <c r="E206" s="2" t="s">
@@ -9946,8 +10164,9 @@
       <c r="N206" s="66" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="207" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O206" s="66"/>
+    </row>
+    <row r="207" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A207" s="113">
         <v>195</v>
       </c>
@@ -9957,7 +10176,7 @@
       <c r="C207" s="5" t="s">
         <v>334</v>
       </c>
-      <c r="D207" s="130" t="s">
+      <c r="D207" s="129" t="s">
         <v>356</v>
       </c>
       <c r="E207" s="2" t="s">
@@ -9980,8 +10199,9 @@
       <c r="N207" s="66" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="208" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O207" s="66"/>
+    </row>
+    <row r="208" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A208" s="113">
         <v>196</v>
       </c>
@@ -9991,7 +10211,7 @@
       <c r="C208" s="5" t="s">
         <v>334</v>
       </c>
-      <c r="D208" s="130" t="s">
+      <c r="D208" s="129" t="s">
         <v>357</v>
       </c>
       <c r="E208" s="2" t="s">
@@ -10014,8 +10234,9 @@
       <c r="N208" s="66" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="209" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O208" s="66"/>
+    </row>
+    <row r="209" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A209" s="113">
         <v>197</v>
       </c>
@@ -10025,7 +10246,7 @@
       <c r="C209" s="5" t="s">
         <v>334</v>
       </c>
-      <c r="D209" s="130" t="s">
+      <c r="D209" s="129" t="s">
         <v>358</v>
       </c>
       <c r="E209" s="2" t="s">
@@ -10048,8 +10269,9 @@
       <c r="N209" s="66" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="210" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O209" s="66"/>
+    </row>
+    <row r="210" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A210" s="113">
         <v>198</v>
       </c>
@@ -10059,7 +10281,7 @@
       <c r="C210" s="5" t="s">
         <v>334</v>
       </c>
-      <c r="D210" s="130" t="s">
+      <c r="D210" s="129" t="s">
         <v>359</v>
       </c>
       <c r="E210" s="2" t="s">
@@ -10082,8 +10304,9 @@
       <c r="N210" s="66" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="211" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O210" s="66"/>
+    </row>
+    <row r="211" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A211" s="113">
         <v>199</v>
       </c>
@@ -10093,7 +10316,7 @@
       <c r="C211" s="5" t="s">
         <v>334</v>
       </c>
-      <c r="D211" s="130" t="s">
+      <c r="D211" s="129" t="s">
         <v>360</v>
       </c>
       <c r="E211" s="2" t="s">
@@ -10116,8 +10339,9 @@
       <c r="N211" s="66" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="212" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O211" s="66"/>
+    </row>
+    <row r="212" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A212" s="113">
         <v>200</v>
       </c>
@@ -10127,7 +10351,7 @@
       <c r="C212" s="5" t="s">
         <v>334</v>
       </c>
-      <c r="D212" s="130" t="s">
+      <c r="D212" s="129" t="s">
         <v>361</v>
       </c>
       <c r="E212" s="2" t="s">
@@ -10150,8 +10374,9 @@
       <c r="N212" s="66" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="213" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O212" s="66"/>
+    </row>
+    <row r="213" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A213" s="113">
         <v>201</v>
       </c>
@@ -10161,7 +10386,7 @@
       <c r="C213" s="5" t="s">
         <v>334</v>
       </c>
-      <c r="D213" s="130" t="s">
+      <c r="D213" s="129" t="s">
         <v>362</v>
       </c>
       <c r="E213" s="2" t="s">
@@ -10184,8 +10409,9 @@
       <c r="N213" s="66" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="214" spans="1:14" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O213" s="66"/>
+    </row>
+    <row r="214" spans="1:15" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A214" s="114">
         <v>202</v>
       </c>
@@ -10195,7 +10421,7 @@
       <c r="C214" s="88" t="s">
         <v>334</v>
       </c>
-      <c r="D214" s="139" t="s">
+      <c r="D214" s="138" t="s">
         <v>363</v>
       </c>
       <c r="E214" s="86" t="s">
@@ -10218,8 +10444,9 @@
       <c r="N214" s="68" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="215" spans="1:14" ht="14.45" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="O214" s="68"/>
+    </row>
+    <row r="215" spans="1:15" ht="14.45" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
       <c r="A215" s="113">
         <v>203</v>
       </c>
@@ -10229,7 +10456,7 @@
       <c r="C215" s="5" t="s">
         <v>335</v>
       </c>
-      <c r="D215" s="130" t="s">
+      <c r="D215" s="129" t="s">
         <v>340</v>
       </c>
       <c r="E215" s="2" t="s">
@@ -10254,8 +10481,9 @@
       <c r="N215" s="66" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="216" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O215" s="66"/>
+    </row>
+    <row r="216" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A216" s="113">
         <v>204</v>
       </c>
@@ -10265,7 +10493,7 @@
       <c r="C216" s="5" t="s">
         <v>335</v>
       </c>
-      <c r="D216" s="130" t="s">
+      <c r="D216" s="129" t="s">
         <v>364</v>
       </c>
       <c r="E216" s="2" t="s">
@@ -10288,8 +10516,9 @@
       <c r="N216" s="66" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="217" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O216" s="66"/>
+    </row>
+    <row r="217" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A217" s="113">
         <v>205</v>
       </c>
@@ -10299,7 +10528,7 @@
       <c r="C217" s="5" t="s">
         <v>335</v>
       </c>
-      <c r="D217" s="130" t="s">
+      <c r="D217" s="129" t="s">
         <v>365</v>
       </c>
       <c r="E217" s="2" t="s">
@@ -10322,8 +10551,9 @@
       <c r="N217" s="66" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="218" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O217" s="66"/>
+    </row>
+    <row r="218" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A218" s="113">
         <v>206</v>
       </c>
@@ -10333,7 +10563,7 @@
       <c r="C218" s="5" t="s">
         <v>335</v>
       </c>
-      <c r="D218" s="130" t="s">
+      <c r="D218" s="129" t="s">
         <v>366</v>
       </c>
       <c r="E218" s="2" t="s">
@@ -10356,8 +10586,9 @@
       <c r="N218" s="66" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="219" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O218" s="66"/>
+    </row>
+    <row r="219" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A219" s="113">
         <v>207</v>
       </c>
@@ -10367,7 +10598,7 @@
       <c r="C219" s="5" t="s">
         <v>335</v>
       </c>
-      <c r="D219" s="130" t="s">
+      <c r="D219" s="129" t="s">
         <v>367</v>
       </c>
       <c r="E219" s="2" t="s">
@@ -10390,8 +10621,9 @@
       <c r="N219" s="66" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="220" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O219" s="66"/>
+    </row>
+    <row r="220" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A220" s="113">
         <v>208</v>
       </c>
@@ -10401,7 +10633,7 @@
       <c r="C220" s="5" t="s">
         <v>335</v>
       </c>
-      <c r="D220" s="130" t="s">
+      <c r="D220" s="129" t="s">
         <v>368</v>
       </c>
       <c r="E220" s="2" t="s">
@@ -10424,8 +10656,9 @@
       <c r="N220" s="66" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="221" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O220" s="66"/>
+    </row>
+    <row r="221" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A221" s="113">
         <v>209</v>
       </c>
@@ -10435,7 +10668,7 @@
       <c r="C221" s="5" t="s">
         <v>335</v>
       </c>
-      <c r="D221" s="130" t="s">
+      <c r="D221" s="129" t="s">
         <v>369</v>
       </c>
       <c r="E221" s="2" t="s">
@@ -10458,8 +10691,9 @@
       <c r="N221" s="66" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="222" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O221" s="66"/>
+    </row>
+    <row r="222" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A222" s="113">
         <v>210</v>
       </c>
@@ -10469,7 +10703,7 @@
       <c r="C222" s="5" t="s">
         <v>335</v>
       </c>
-      <c r="D222" s="130" t="s">
+      <c r="D222" s="129" t="s">
         <v>370</v>
       </c>
       <c r="E222" s="2" t="s">
@@ -10492,8 +10726,9 @@
       <c r="N222" s="66" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="223" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O222" s="66"/>
+    </row>
+    <row r="223" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A223" s="113">
         <v>211</v>
       </c>
@@ -10503,7 +10738,7 @@
       <c r="C223" s="5" t="s">
         <v>335</v>
       </c>
-      <c r="D223" s="130" t="s">
+      <c r="D223" s="129" t="s">
         <v>371</v>
       </c>
       <c r="E223" s="2" t="s">
@@ -10526,8 +10761,9 @@
       <c r="N223" s="66" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="224" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O223" s="66"/>
+    </row>
+    <row r="224" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A224" s="113">
         <v>212</v>
       </c>
@@ -10537,7 +10773,7 @@
       <c r="C224" s="5" t="s">
         <v>335</v>
       </c>
-      <c r="D224" s="130" t="s">
+      <c r="D224" s="129" t="s">
         <v>372</v>
       </c>
       <c r="E224" s="2" t="s">
@@ -10560,8 +10796,9 @@
       <c r="N224" s="66" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="225" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O224" s="66"/>
+    </row>
+    <row r="225" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A225" s="113">
         <v>213</v>
       </c>
@@ -10571,7 +10808,7 @@
       <c r="C225" s="5" t="s">
         <v>335</v>
       </c>
-      <c r="D225" s="130" t="s">
+      <c r="D225" s="129" t="s">
         <v>373</v>
       </c>
       <c r="E225" s="2" t="s">
@@ -10594,8 +10831,9 @@
       <c r="N225" s="66" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="226" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O225" s="66"/>
+    </row>
+    <row r="226" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A226" s="113">
         <v>214</v>
       </c>
@@ -10605,7 +10843,7 @@
       <c r="C226" s="5" t="s">
         <v>335</v>
       </c>
-      <c r="D226" s="130" t="s">
+      <c r="D226" s="129" t="s">
         <v>374</v>
       </c>
       <c r="E226" s="2" t="s">
@@ -10628,8 +10866,9 @@
       <c r="N226" s="66" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="227" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O226" s="66"/>
+    </row>
+    <row r="227" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A227" s="113">
         <v>215</v>
       </c>
@@ -10639,7 +10878,7 @@
       <c r="C227" s="5" t="s">
         <v>335</v>
       </c>
-      <c r="D227" s="130" t="s">
+      <c r="D227" s="129" t="s">
         <v>375</v>
       </c>
       <c r="E227" s="2" t="s">
@@ -10662,8 +10901,9 @@
       <c r="N227" s="66" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="228" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O227" s="66"/>
+    </row>
+    <row r="228" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A228" s="113">
         <v>216</v>
       </c>
@@ -10673,7 +10913,7 @@
       <c r="C228" s="5" t="s">
         <v>335</v>
       </c>
-      <c r="D228" s="130" t="s">
+      <c r="D228" s="129" t="s">
         <v>376</v>
       </c>
       <c r="E228" s="2" t="s">
@@ -10696,8 +10936,9 @@
       <c r="N228" s="66" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="229" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O228" s="66"/>
+    </row>
+    <row r="229" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A229" s="113">
         <v>217</v>
       </c>
@@ -10707,7 +10948,7 @@
       <c r="C229" s="5" t="s">
         <v>335</v>
       </c>
-      <c r="D229" s="130" t="s">
+      <c r="D229" s="129" t="s">
         <v>377</v>
       </c>
       <c r="E229" s="2" t="s">
@@ -10730,8 +10971,9 @@
       <c r="N229" s="66" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="230" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O229" s="66"/>
+    </row>
+    <row r="230" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A230" s="113">
         <v>218</v>
       </c>
@@ -10741,7 +10983,7 @@
       <c r="C230" s="5" t="s">
         <v>335</v>
       </c>
-      <c r="D230" s="130" t="s">
+      <c r="D230" s="129" t="s">
         <v>378</v>
       </c>
       <c r="E230" s="2" t="s">
@@ -10764,8 +11006,9 @@
       <c r="N230" s="66" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="231" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O230" s="66"/>
+    </row>
+    <row r="231" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A231" s="113">
         <v>219</v>
       </c>
@@ -10775,7 +11018,7 @@
       <c r="C231" s="5" t="s">
         <v>335</v>
       </c>
-      <c r="D231" s="130" t="s">
+      <c r="D231" s="129" t="s">
         <v>379</v>
       </c>
       <c r="E231" s="2" t="s">
@@ -10798,8 +11041,9 @@
       <c r="N231" s="66" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="232" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O231" s="66"/>
+    </row>
+    <row r="232" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A232" s="113">
         <v>220</v>
       </c>
@@ -10809,7 +11053,7 @@
       <c r="C232" s="5" t="s">
         <v>335</v>
       </c>
-      <c r="D232" s="130" t="s">
+      <c r="D232" s="129" t="s">
         <v>380</v>
       </c>
       <c r="E232" s="2" t="s">
@@ -10832,8 +11076,9 @@
       <c r="N232" s="66" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="233" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O232" s="66"/>
+    </row>
+    <row r="233" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A233" s="113">
         <v>221</v>
       </c>
@@ -10843,7 +11088,7 @@
       <c r="C233" s="5" t="s">
         <v>335</v>
       </c>
-      <c r="D233" s="130" t="s">
+      <c r="D233" s="129" t="s">
         <v>381</v>
       </c>
       <c r="E233" s="2" t="s">
@@ -10866,8 +11111,9 @@
       <c r="N233" s="66" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="234" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O233" s="66"/>
+    </row>
+    <row r="234" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A234" s="113">
         <v>222</v>
       </c>
@@ -10877,7 +11123,7 @@
       <c r="C234" s="5" t="s">
         <v>335</v>
       </c>
-      <c r="D234" s="130" t="s">
+      <c r="D234" s="129" t="s">
         <v>382</v>
       </c>
       <c r="E234" s="2" t="s">
@@ -10900,8 +11146,9 @@
       <c r="N234" s="66" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="235" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O234" s="66"/>
+    </row>
+    <row r="235" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A235" s="113">
         <v>223</v>
       </c>
@@ -10911,7 +11158,7 @@
       <c r="C235" s="5" t="s">
         <v>335</v>
       </c>
-      <c r="D235" s="130" t="s">
+      <c r="D235" s="129" t="s">
         <v>383</v>
       </c>
       <c r="E235" s="2" t="s">
@@ -10934,8 +11181,9 @@
       <c r="N235" s="66" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="236" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O235" s="66"/>
+    </row>
+    <row r="236" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A236" s="113">
         <v>224</v>
       </c>
@@ -10945,7 +11193,7 @@
       <c r="C236" s="5" t="s">
         <v>335</v>
       </c>
-      <c r="D236" s="130" t="s">
+      <c r="D236" s="129" t="s">
         <v>384</v>
       </c>
       <c r="E236" s="2" t="s">
@@ -10968,8 +11216,9 @@
       <c r="N236" s="66" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="237" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O236" s="66"/>
+    </row>
+    <row r="237" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A237" s="113">
         <v>225</v>
       </c>
@@ -10979,7 +11228,7 @@
       <c r="C237" s="5" t="s">
         <v>335</v>
       </c>
-      <c r="D237" s="130" t="s">
+      <c r="D237" s="129" t="s">
         <v>385</v>
       </c>
       <c r="E237" s="2" t="s">
@@ -11002,8 +11251,9 @@
       <c r="N237" s="66" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="238" spans="1:14" s="26" customFormat="1" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O237" s="66"/>
+    </row>
+    <row r="238" spans="1:15" s="26" customFormat="1" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A238" s="115">
         <v>226</v>
       </c>
@@ -11013,7 +11263,7 @@
       <c r="C238" s="106" t="s">
         <v>335</v>
       </c>
-      <c r="D238" s="140" t="s">
+      <c r="D238" s="139" t="s">
         <v>386</v>
       </c>
       <c r="E238" s="89" t="s">
@@ -11036,6 +11286,7 @@
       <c r="N238" s="69" t="s">
         <v>456</v>
       </c>
+      <c r="O238" s="69"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:L119" xr:uid="{00000000-0001-0000-0000-000000000000}"/>

</xml_diff>

<commit_message>
unique dummy export aliases
</commit_message>
<xml_diff>
--- a/dataland-framework-toolbox/inputs/eu-taxonomy-financials/eu-taxonomy-financials.xlsx
+++ b/dataland-framework-toolbox/inputs/eu-taxonomy-financials/eu-taxonomy-financials.xlsx
@@ -5,18 +5,18 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d93542\Dataland\dataland-framework-toolbox\inputs\eu-taxonomy-financials\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d91596\Dataland\dataland-framework-toolbox\inputs\eu-taxonomy-financials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E09757E-17E1-4FD6-B163-750252256F3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9195CB34-243B-4922-8496-BB0BDE48C754}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-5145" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Framework Data Model" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Framework Data Model'!$A$1:$M$119</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Framework Data Model'!$A$1:$M$238</definedName>
     <definedName name="IQ_CH">110000</definedName>
     <definedName name="IQ_CQ">5000</definedName>
     <definedName name="IQ_CY">10000</definedName>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2180" uniqueCount="576">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2180" uniqueCount="642">
   <si>
     <t>Field Identifier</t>
   </si>
@@ -1460,9 +1460,6 @@
     <t>Substantial Contribution to CCM in Percent - Of which Enabling</t>
   </si>
   <si>
-    <t>Substantial Contribution to CCM in Percent - Of which Transitional</t>
-  </si>
-  <si>
     <t>Share of Turnover-based KPI substantially contributing to CCM in Percent - Aligned</t>
   </si>
   <si>
@@ -1529,21 +1526,6 @@
     <t>CapEx-based Proportion of Revenue substantially contributing to CCM - Of which Enabling</t>
   </si>
   <si>
-    <t>Substantial Contribution to CCA in Percent - Eligible</t>
-  </si>
-  <si>
-    <t>Substantial Contribution to CCA in Percent - Aligned</t>
-  </si>
-  <si>
-    <t>Substantial Contribution to CCA in Percent - Of which Use of Proceeds</t>
-  </si>
-  <si>
-    <t>Substantial Contribution to CCA in Percent - Of which Enabling</t>
-  </si>
-  <si>
-    <t>Substantial Contribution to CCA in Percent - Of which Adapting</t>
-  </si>
-  <si>
     <t>Share of Turnover-based KPI substantially contributing to CCA in Percent - Aligned</t>
   </si>
   <si>
@@ -1592,18 +1574,6 @@
     <t>CapEx-based Proportion of Revenue substantially contributing to CCA - Of which Enabling</t>
   </si>
   <si>
-    <t>Substantial Contribution to Sustainable Use and Protection of WTR in Percent - Eligible</t>
-  </si>
-  <si>
-    <t>Substantial Contribution to Sustainable Use and Protection of WTR in Percent - Aligned</t>
-  </si>
-  <si>
-    <t>Substantial Contribution to Sustainable Use and Protection of WTR in Percent - Of which Use of Proceeds</t>
-  </si>
-  <si>
-    <t>Substantial Contribution to Sustainable Use and Protection of WTR in Percent - Of which Enabling</t>
-  </si>
-  <si>
     <t>Share of Turnover-based KPI substantially contributing to Sustainable Use and Protection of WTR in Percent - Aligned</t>
   </si>
   <si>
@@ -1652,18 +1622,6 @@
     <t>CapEx-based Proportion of Revenue substantially contributing to Sustainable Use and Protection of WTR - Of which Enabling</t>
   </si>
   <si>
-    <t>Substantial Contribution to CE in Percent - Eligible</t>
-  </si>
-  <si>
-    <t>Substantial Contribution to CE in Percent - Aligned</t>
-  </si>
-  <si>
-    <t>Substantial Contribution to CE in Percent - Of which Use of Proceeds</t>
-  </si>
-  <si>
-    <t>Substantial Contribution to CE in Percent - Of which Enabling</t>
-  </si>
-  <si>
     <t>Share of Turnover-based KPI substantially contributing to CE in Percent - Aligned</t>
   </si>
   <si>
@@ -1676,18 +1634,6 @@
     <t>Share of CapEx-based KPI substantially contributing to CE in Percent - Of which Enabling</t>
   </si>
   <si>
-    <t>Substantial Contribution to PPC in Percent - Eligible</t>
-  </si>
-  <si>
-    <t>Substantial Contribution to PPC in Percent - Aligned</t>
-  </si>
-  <si>
-    <t>Substantial Contribution to PPC in Percent - Of which Use of Proceeds</t>
-  </si>
-  <si>
-    <t>Substantial Contribution to PPC in Percent - Of which Enabling</t>
-  </si>
-  <si>
     <t>Share of Turnover-based KPI substantially contributing to PPC in Percent - Aligned</t>
   </si>
   <si>
@@ -1736,18 +1682,6 @@
     <t>CapEx-based Proportion of Revenue substantially contributing to PPC - Of which Enabling</t>
   </si>
   <si>
-    <t>Substantial Contribution to BIO in Percent - Eligible</t>
-  </si>
-  <si>
-    <t>Substantial Contribution to BIO in Percent - Aligned</t>
-  </si>
-  <si>
-    <t>Substantial Contribution to BIO in Percent - Of which Use of Proceeds</t>
-  </si>
-  <si>
-    <t>Substantial Contribution to BIO in Percent - Of which Enabling</t>
-  </si>
-  <si>
     <t>Share of Turnover-based KPI substantially contributing to BIO in Percent - Aligned</t>
   </si>
   <si>
@@ -1794,6 +1728,270 @@
   </si>
   <si>
     <t>CapEx-based Proportion of Revenue substantially contributing to BIO - Of which Enabling</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to CCM in Percent - Eligible TO</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to CCM in Percent - Aligned TO</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to CCM in Percent - Of which Use of Proceeds TO</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to CCM in Percent - Of which Enabling TO</t>
+  </si>
+  <si>
+    <t>Share of CapEx-based KPI substantially contributing to BIO in Percent - Of which Enabling Insurance</t>
+  </si>
+  <si>
+    <t>Total of Absolute Premiums of Taxonomy-aligned Activities Insurance</t>
+  </si>
+  <si>
+    <t>Total of Absolute Premiums of Taxonomy-eligible but Taxonomy-non-aligned Activities Insurance</t>
+  </si>
+  <si>
+    <t>Total of Absolute Premiums of Taxonomy-non-eligible Activities Insurance</t>
+  </si>
+  <si>
+    <t>Proportion of Absolute Premiums of Taxonomy-aligned Activities Insurance</t>
+  </si>
+  <si>
+    <t>Proportion of Absolute Premiums of Taxonomy-eligible but Taxonomy-non-aligned Activities Insurance</t>
+  </si>
+  <si>
+    <t>Proportion of Absolute Premiums of Taxonomy-non-eligible Activities Insurance</t>
+  </si>
+  <si>
+    <t>Weighted Average Value of all Investments - Turnover-based in Percent Insurance</t>
+  </si>
+  <si>
+    <t>Weighted Average Value of all Investments - CapEx-based in Percent Insurance</t>
+  </si>
+  <si>
+    <t>Weighted Average Value of all Investments - Turnover-based monetary amount Insurance</t>
+  </si>
+  <si>
+    <t>Weighted Average Value of all Investments - CapEx-based monetary amount Insurance</t>
+  </si>
+  <si>
+    <t>Share of Turnover-based KPI substantially contributing to CCM in Percent - Aligned Insurance</t>
+  </si>
+  <si>
+    <t>Share of Turnover-based KPI substantially contributing to CCM in Percent - Of which Enabling Insurance</t>
+  </si>
+  <si>
+    <t>Share of Turnover-based KPI substantially contributing to CCM in Percent - Of which Transitional Insurance</t>
+  </si>
+  <si>
+    <t>Share of Turnover-based KPI substantially contributing to CCA in Percent - Aligned Insurance</t>
+  </si>
+  <si>
+    <t>Share of Turnover-based KPI substantially contributing to CCA in Percent - Of which Enabling Insurance</t>
+  </si>
+  <si>
+    <t>Share of Turnover-based KPI substantially contributing to Sustainable Use and Protection of WTR in Percent - Aligned Insurance</t>
+  </si>
+  <si>
+    <t>Share of Turnover-based KPI substantially contributing to Sustainable Use and Protection of WTR in Percent - Of which Enabling Insurance</t>
+  </si>
+  <si>
+    <t>Share of Turnover-based KPI substantially contributing to CE in Percent - Aligned Insurance</t>
+  </si>
+  <si>
+    <t>Share of Turnover-based KPI substantially contributing to CE in Percent - Of which Enabling Insurance</t>
+  </si>
+  <si>
+    <t>Share of Turnover-based KPI substantially contributing to PPC in Percent - Aligned Insurance</t>
+  </si>
+  <si>
+    <t>Share of Turnover-based KPI substantially contributing to PPC in Percent - Of which Enabling Insurance</t>
+  </si>
+  <si>
+    <t>Share of Turnover-based KPI substantially contributing to BIO in Percent - Aligned Insurance</t>
+  </si>
+  <si>
+    <t>Share of Turnover-based KPI substantially contributing to BIO in Percent - Of which Enabling Insurance</t>
+  </si>
+  <si>
+    <t>Share of CapEx-based KPI substantially contributing to CCM in Percent - Aligned Insurance</t>
+  </si>
+  <si>
+    <t>Share of CapEx-based KPI substantially contributing to CCM in Percent - Of which Enabling Insurance</t>
+  </si>
+  <si>
+    <t>Share of CapEx-based KPI substantially contributing to CCM in Percent - Of which Transitional Insurance</t>
+  </si>
+  <si>
+    <t>Share of CapEx-based KPI substantially contributing to CCA in Percent - Aligned Insurance</t>
+  </si>
+  <si>
+    <t>Share of CapEx-based KPI substantially contributing to CCA in Percent - Of which Enabling Insurance</t>
+  </si>
+  <si>
+    <t>Share of CapEx-based KPI substantially contributing to Sustainable Use and Protection of WTR in Percent - Aligned Insurance</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to CCM in Percent - Of which Transitional Capex</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to CCA in Percent - Eligible Capex</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to CCA in Percent - Aligned Capex</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to CCA in Percent - Of which Use of Proceeds Capex</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to CCA in Percent - Of which Enabling Capex</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to CCA in Percent - Of which Adapting Capex</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to Sustainable Use and Protection of WTR in Percent - Eligible Capex</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to Sustainable Use and Protection of WTR in Percent - Aligned Capex</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to Sustainable Use and Protection of WTR in Percent - Of which Use of Proceeds Capex</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to Sustainable Use and Protection of WTR in Percent - Of which Enabling Capex</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to CE in Percent - Eligible Capex</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to CE in Percent - Aligned Capex</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to CE in Percent - Of which Use of Proceeds Capex</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to CE in Percent - Of which Enabling Capex</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to PPC in Percent - Eligible Capex</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to PPC in Percent - Aligned Capex</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to PPC in Percent - Of which Use of Proceeds Capex</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to PPC in Percent - Of which Enabling Capex</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to BIO in Percent - Eligible Capex</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to BIO in Percent - Aligned Capex</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to BIO in Percent - Of which Use of Proceeds Capex</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to BIO in Percent - Of which Enabling Capex</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to any of the six Environmental Objectives in Percent - Eligible Capex</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to any of the six Environmental Objectives in Percent - Aligned Capex</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to any of the six Environmental Objectives in Percent - Of which Use of Proceeds Capex</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to any of the six Environmental Objectives in Percent - Of which Enabling Capex</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to any of the six Environmental Objectives in Percent - Of which Transitional Capex</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to CCM in Percent - Of which Transitional TO</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to CCA in Percent - Eligible TO</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to CCA in Percent - Aligned TO</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to CCA in Percent - Of which Use of Proceeds TO</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to CCA in Percent - Of which Enabling TO</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to CCA in Percent - Of which Adapting TO</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to Sustainable Use and Protection of WTR in Percent - Eligible TO</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to Sustainable Use and Protection of WTR in Percent - Aligned TO</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to Sustainable Use and Protection of WTR in Percent - Of which Use of Proceeds TO</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to Sustainable Use and Protection of WTR in Percent - Of which Enabling TO</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to CE in Percent - Eligible TO</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to CE in Percent - Aligned TO</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to CE in Percent - Of which Use of Proceeds TO</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to CE in Percent - Of which Enabling TO</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to PPC in Percent - Eligible TO</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to PPC in Percent - Aligned TO</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to PPC in Percent - Of which Use of Proceeds TO</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to PPC in Percent - Of which Enabling TO</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to BIO in Percent - Eligible TO</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to BIO in Percent - Aligned TO</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to BIO in Percent - Of which Use of Proceeds TO</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to BIO in Percent - Of which Enabling TO</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to any of the six Environmental Objectives in Percent - Eligible TO</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to any of the six Environmental Objectives in Percent - Aligned TO</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to any of the six Environmental Objectives in Percent - Of which Use of Proceeds TO</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to any of the six Environmental Objectives in Percent - Of which Enabling TO</t>
+  </si>
+  <si>
+    <t>Substantial Contribution to any of the six Environmental Objectives in Percent - Of which Transitional TO</t>
   </si>
 </sst>
 </file>
@@ -3025,7 +3223,18 @@
     <cellStyle name="Normal 5" xfId="5" xr:uid="{D1778BAD-A850-47A1-8820-D9F50BDF158C}"/>
     <cellStyle name="Normal 6" xfId="7" xr:uid="{9099DBD5-D38C-44AB-975C-276D53FC48EC}"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
@@ -3289,27 +3498,27 @@
   <dimension ref="A1:P238"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="E49" sqref="E49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="12.36328125" customWidth="1"/>
-    <col min="3" max="3" width="71.6328125" customWidth="1"/>
-    <col min="4" max="5" width="117.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="71.59765625" customWidth="1"/>
+    <col min="4" max="5" width="117.796875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="92" customWidth="1"/>
-    <col min="7" max="7" width="36.36328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.81640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.36328125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.7265625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.26953125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.6328125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.08984375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="26.36328125" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="30.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="36.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.73046875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.265625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.59765625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.06640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="30.265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="107" t="s">
         <v>0</v>
       </c>
@@ -3359,7 +3568,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A2" s="108">
         <v>1</v>
       </c>
@@ -3395,7 +3604,7 @@
       <c r="O2" s="34"/>
       <c r="P2" s="34"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A3" s="108">
         <v>2</v>
       </c>
@@ -3431,7 +3640,7 @@
       <c r="O3" s="34"/>
       <c r="P3" s="34"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A4" s="108">
         <v>3</v>
       </c>
@@ -3465,7 +3674,7 @@
       <c r="O4" s="34"/>
       <c r="P4" s="34"/>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A5" s="108">
         <v>4</v>
       </c>
@@ -3503,7 +3712,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A6" s="108">
         <v>5</v>
       </c>
@@ -3539,7 +3748,7 @@
       <c r="O6" s="34"/>
       <c r="P6" s="34"/>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A7" s="108">
         <v>6</v>
       </c>
@@ -3573,7 +3782,7 @@
       <c r="O7" s="34"/>
       <c r="P7" s="34"/>
     </row>
-    <row r="8" spans="1:16" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:16" s="1" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A8" s="109">
         <v>7</v>
       </c>
@@ -3607,7 +3816,7 @@
       <c r="O8" s="11"/>
       <c r="P8" s="11"/>
     </row>
-    <row r="9" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A9" s="73">
         <v>8</v>
       </c>
@@ -3647,7 +3856,7 @@
       </c>
       <c r="P9" s="42"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A10" s="73">
         <v>9</v>
       </c>
@@ -3687,7 +3896,7 @@
       </c>
       <c r="P10" s="34"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A11" s="73">
         <v>9.1</v>
       </c>
@@ -3727,7 +3936,7 @@
       </c>
       <c r="P11" s="34"/>
     </row>
-    <row r="12" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A12" s="72" t="s">
         <v>105</v>
       </c>
@@ -3767,7 +3976,7 @@
       </c>
       <c r="P12" s="42"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A13" s="72" t="s">
         <v>106</v>
       </c>
@@ -3807,7 +4016,7 @@
       </c>
       <c r="P13" s="34"/>
     </row>
-    <row r="14" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:16" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A14" s="110" t="s">
         <v>107</v>
       </c>
@@ -3847,7 +4056,7 @@
       </c>
       <c r="P14" s="41"/>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A15" s="72">
         <v>10</v>
       </c>
@@ -3861,7 +4070,7 @@
         <v>46</v>
       </c>
       <c r="E15" s="119" t="s">
-        <v>460</v>
+        <v>554</v>
       </c>
       <c r="F15" s="14" t="s">
         <v>52</v>
@@ -3885,7 +4094,7 @@
       </c>
       <c r="P15" s="34"/>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A16" s="72">
         <v>10.1</v>
       </c>
@@ -3899,7 +4108,7 @@
         <v>35</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>461</v>
+        <v>555</v>
       </c>
       <c r="F16" s="15" t="s">
         <v>53</v>
@@ -3923,7 +4132,7 @@
       </c>
       <c r="P16" s="34"/>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A17" s="72" t="s">
         <v>108</v>
       </c>
@@ -3937,7 +4146,7 @@
         <v>66</v>
       </c>
       <c r="E17" s="14" t="s">
-        <v>462</v>
+        <v>556</v>
       </c>
       <c r="F17" s="15" t="s">
         <v>72</v>
@@ -3961,7 +4170,7 @@
       </c>
       <c r="P17" s="34"/>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A18" s="72" t="s">
         <v>109</v>
       </c>
@@ -3975,7 +4184,7 @@
         <v>149</v>
       </c>
       <c r="E18" s="14" t="s">
-        <v>463</v>
+        <v>557</v>
       </c>
       <c r="F18" s="15" t="s">
         <v>54</v>
@@ -3999,7 +4208,7 @@
       </c>
       <c r="P18" s="34"/>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A19" s="72" t="s">
         <v>110</v>
       </c>
@@ -4013,7 +4222,7 @@
         <v>156</v>
       </c>
       <c r="E19" s="14" t="s">
-        <v>464</v>
+        <v>615</v>
       </c>
       <c r="F19" s="15" t="s">
         <v>55</v>
@@ -4037,7 +4246,7 @@
       </c>
       <c r="P19" s="34"/>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A20" s="72">
         <v>11</v>
       </c>
@@ -4051,7 +4260,7 @@
         <v>36</v>
       </c>
       <c r="E20" s="14" t="s">
-        <v>487</v>
+        <v>616</v>
       </c>
       <c r="F20" s="15" t="s">
         <v>60</v>
@@ -4075,7 +4284,7 @@
       </c>
       <c r="P20" s="34"/>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A21" s="72">
         <v>11.1</v>
       </c>
@@ -4089,7 +4298,7 @@
         <v>37</v>
       </c>
       <c r="E21" s="14" t="s">
-        <v>488</v>
+        <v>617</v>
       </c>
       <c r="F21" s="15" t="s">
         <v>61</v>
@@ -4113,7 +4322,7 @@
       </c>
       <c r="P21" s="34"/>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A22" s="72" t="s">
         <v>111</v>
       </c>
@@ -4127,7 +4336,7 @@
         <v>67</v>
       </c>
       <c r="E22" s="14" t="s">
-        <v>489</v>
+        <v>618</v>
       </c>
       <c r="F22" s="15" t="s">
         <v>73</v>
@@ -4151,7 +4360,7 @@
       </c>
       <c r="P22" s="34"/>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A23" s="72" t="s">
         <v>112</v>
       </c>
@@ -4165,7 +4374,7 @@
         <v>150</v>
       </c>
       <c r="E23" s="124" t="s">
-        <v>490</v>
+        <v>619</v>
       </c>
       <c r="F23" s="16" t="s">
         <v>62</v>
@@ -4189,7 +4398,7 @@
       </c>
       <c r="P23" s="34"/>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A24" s="72" t="s">
         <v>175</v>
       </c>
@@ -4203,7 +4412,7 @@
         <v>177</v>
       </c>
       <c r="E24" s="124" t="s">
-        <v>491</v>
+        <v>620</v>
       </c>
       <c r="F24" s="16" t="s">
         <v>176</v>
@@ -4227,7 +4436,7 @@
       </c>
       <c r="P24" s="34"/>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A25" s="72">
         <v>12</v>
       </c>
@@ -4241,7 +4450,7 @@
         <v>38</v>
       </c>
       <c r="E25" s="124" t="s">
-        <v>508</v>
+        <v>621</v>
       </c>
       <c r="F25" s="16" t="s">
         <v>165</v>
@@ -4265,7 +4474,7 @@
       </c>
       <c r="P25" s="34"/>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A26" s="72">
         <v>12.1</v>
       </c>
@@ -4279,7 +4488,7 @@
         <v>39</v>
       </c>
       <c r="E26" s="124" t="s">
-        <v>509</v>
+        <v>622</v>
       </c>
       <c r="F26" s="16" t="s">
         <v>166</v>
@@ -4303,7 +4512,7 @@
       </c>
       <c r="P26" s="34"/>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A27" s="72" t="s">
         <v>113</v>
       </c>
@@ -4317,7 +4526,7 @@
         <v>68</v>
       </c>
       <c r="E27" s="124" t="s">
-        <v>510</v>
+        <v>623</v>
       </c>
       <c r="F27" s="16" t="s">
         <v>167</v>
@@ -4341,7 +4550,7 @@
       </c>
       <c r="P27" s="34"/>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A28" s="72" t="s">
         <v>114</v>
       </c>
@@ -4355,7 +4564,7 @@
         <v>151</v>
       </c>
       <c r="E28" s="124" t="s">
-        <v>511</v>
+        <v>624</v>
       </c>
       <c r="F28" s="16" t="s">
         <v>168</v>
@@ -4379,7 +4588,7 @@
       </c>
       <c r="P28" s="34"/>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A29" s="72">
         <v>13</v>
       </c>
@@ -4393,7 +4602,7 @@
         <v>40</v>
       </c>
       <c r="E29" s="124" t="s">
-        <v>528</v>
+        <v>625</v>
       </c>
       <c r="F29" s="16" t="s">
         <v>74</v>
@@ -4417,7 +4626,7 @@
       </c>
       <c r="P29" s="34"/>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A30" s="72">
         <v>13.1</v>
       </c>
@@ -4431,7 +4640,7 @@
         <v>41</v>
       </c>
       <c r="E30" s="124" t="s">
-        <v>529</v>
+        <v>626</v>
       </c>
       <c r="F30" s="16" t="s">
         <v>75</v>
@@ -4455,7 +4664,7 @@
       </c>
       <c r="P30" s="34"/>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A31" s="72" t="s">
         <v>115</v>
       </c>
@@ -4469,7 +4678,7 @@
         <v>69</v>
       </c>
       <c r="E31" s="124" t="s">
-        <v>530</v>
+        <v>627</v>
       </c>
       <c r="F31" s="16" t="s">
         <v>76</v>
@@ -4493,7 +4702,7 @@
       </c>
       <c r="P31" s="34"/>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A32" s="72" t="s">
         <v>116</v>
       </c>
@@ -4507,7 +4716,7 @@
         <v>152</v>
       </c>
       <c r="E32" s="124" t="s">
-        <v>531</v>
+        <v>628</v>
       </c>
       <c r="F32" s="16" t="s">
         <v>77</v>
@@ -4531,7 +4740,7 @@
       </c>
       <c r="P32" s="34"/>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A33" s="72">
         <v>14</v>
       </c>
@@ -4545,7 +4754,7 @@
         <v>42</v>
       </c>
       <c r="E33" s="124" t="s">
-        <v>536</v>
+        <v>629</v>
       </c>
       <c r="F33" s="16" t="s">
         <v>81</v>
@@ -4569,7 +4778,7 @@
       </c>
       <c r="P33" s="34"/>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A34" s="72">
         <v>14.1</v>
       </c>
@@ -4583,7 +4792,7 @@
         <v>43</v>
       </c>
       <c r="E34" s="124" t="s">
-        <v>537</v>
+        <v>630</v>
       </c>
       <c r="F34" s="16" t="s">
         <v>82</v>
@@ -4607,7 +4816,7 @@
       </c>
       <c r="P34" s="34"/>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A35" s="72" t="s">
         <v>117</v>
       </c>
@@ -4621,7 +4830,7 @@
         <v>70</v>
       </c>
       <c r="E35" s="124" t="s">
-        <v>538</v>
+        <v>631</v>
       </c>
       <c r="F35" s="16" t="s">
         <v>83</v>
@@ -4645,7 +4854,7 @@
       </c>
       <c r="P35" s="34"/>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A36" s="72" t="s">
         <v>118</v>
       </c>
@@ -4659,7 +4868,7 @@
         <v>153</v>
       </c>
       <c r="E36" s="124" t="s">
-        <v>539</v>
+        <v>632</v>
       </c>
       <c r="F36" s="16" t="s">
         <v>84</v>
@@ -4683,7 +4892,7 @@
       </c>
       <c r="P36" s="34"/>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A37" s="72">
         <v>15</v>
       </c>
@@ -4697,7 +4906,7 @@
         <v>44</v>
       </c>
       <c r="E37" s="124" t="s">
-        <v>556</v>
+        <v>633</v>
       </c>
       <c r="F37" s="16" t="s">
         <v>88</v>
@@ -4721,7 +4930,7 @@
       </c>
       <c r="P37" s="34"/>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A38" s="72">
         <v>15.1</v>
       </c>
@@ -4735,7 +4944,7 @@
         <v>45</v>
       </c>
       <c r="E38" s="124" t="s">
-        <v>557</v>
+        <v>634</v>
       </c>
       <c r="F38" s="16" t="s">
         <v>89</v>
@@ -4759,7 +4968,7 @@
       </c>
       <c r="P38" s="34"/>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A39" s="43" t="s">
         <v>119</v>
       </c>
@@ -4773,7 +4982,7 @@
         <v>71</v>
       </c>
       <c r="E39" s="125" t="s">
-        <v>558</v>
+        <v>635</v>
       </c>
       <c r="F39" s="17" t="s">
         <v>90</v>
@@ -4797,7 +5006,7 @@
       </c>
       <c r="P39" s="45"/>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A40" s="72" t="s">
         <v>120</v>
       </c>
@@ -4811,7 +5020,7 @@
         <v>154</v>
       </c>
       <c r="E40" s="126" t="s">
-        <v>559</v>
+        <v>636</v>
       </c>
       <c r="F40" s="30" t="s">
         <v>91</v>
@@ -4835,7 +5044,7 @@
       </c>
       <c r="P40" s="46"/>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A41" s="72">
         <v>16</v>
       </c>
@@ -4849,7 +5058,7 @@
         <v>123</v>
       </c>
       <c r="E41" s="124" t="s">
-        <v>123</v>
+        <v>637</v>
       </c>
       <c r="F41" s="16" t="s">
         <v>169</v>
@@ -4873,7 +5082,7 @@
       </c>
       <c r="P41" s="34"/>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A42" s="72">
         <v>16.100000000000001</v>
       </c>
@@ -4887,7 +5096,7 @@
         <v>124</v>
       </c>
       <c r="E42" s="124" t="s">
-        <v>124</v>
+        <v>638</v>
       </c>
       <c r="F42" s="16" t="s">
         <v>126</v>
@@ -4911,7 +5120,7 @@
       </c>
       <c r="P42" s="34"/>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A43" s="43" t="s">
         <v>121</v>
       </c>
@@ -4925,7 +5134,7 @@
         <v>125</v>
       </c>
       <c r="E43" s="74" t="s">
-        <v>125</v>
+        <v>639</v>
       </c>
       <c r="F43" s="17" t="s">
         <v>127</v>
@@ -4949,7 +5158,7 @@
       </c>
       <c r="P43" s="45"/>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A44" s="43" t="s">
         <v>122</v>
       </c>
@@ -4963,7 +5172,7 @@
         <v>155</v>
       </c>
       <c r="E44" s="126" t="s">
-        <v>155</v>
+        <v>640</v>
       </c>
       <c r="F44" s="30" t="s">
         <v>147</v>
@@ -4987,7 +5196,7 @@
       </c>
       <c r="P44" s="46"/>
     </row>
-    <row r="45" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:16" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A45" s="111" t="s">
         <v>159</v>
       </c>
@@ -5001,7 +5210,7 @@
         <v>157</v>
       </c>
       <c r="E45" s="127" t="s">
-        <v>157</v>
+        <v>641</v>
       </c>
       <c r="F45" s="18" t="s">
         <v>128</v>
@@ -5025,7 +5234,7 @@
       </c>
       <c r="P45" s="50"/>
     </row>
-    <row r="46" spans="1:16" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:16" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
       <c r="A46" s="72">
         <v>20</v>
       </c>
@@ -5063,7 +5272,7 @@
       </c>
       <c r="P46" s="34"/>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A47" s="72">
         <v>20.100000000000001</v>
       </c>
@@ -5101,7 +5310,7 @@
       </c>
       <c r="P47" s="34"/>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A48" s="72" t="s">
         <v>129</v>
       </c>
@@ -5139,7 +5348,7 @@
       </c>
       <c r="P48" s="34"/>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A49" s="72" t="s">
         <v>130</v>
       </c>
@@ -5177,7 +5386,7 @@
       </c>
       <c r="P49" s="34"/>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A50" s="72" t="s">
         <v>131</v>
       </c>
@@ -5191,7 +5400,7 @@
         <v>156</v>
       </c>
       <c r="E50" s="14" t="s">
-        <v>464</v>
+        <v>588</v>
       </c>
       <c r="F50" s="16" t="s">
         <v>59</v>
@@ -5215,7 +5424,7 @@
       </c>
       <c r="P50" s="34"/>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A51" s="72">
         <v>21</v>
       </c>
@@ -5229,7 +5438,7 @@
         <v>36</v>
       </c>
       <c r="E51" s="14" t="s">
-        <v>487</v>
+        <v>589</v>
       </c>
       <c r="F51" s="16" t="s">
         <v>63</v>
@@ -5253,7 +5462,7 @@
       </c>
       <c r="P51" s="34"/>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A52" s="72">
         <v>21.1</v>
       </c>
@@ -5267,7 +5476,7 @@
         <v>37</v>
       </c>
       <c r="E52" s="14" t="s">
-        <v>488</v>
+        <v>590</v>
       </c>
       <c r="F52" s="16" t="s">
         <v>64</v>
@@ -5291,7 +5500,7 @@
       </c>
       <c r="P52" s="34"/>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A53" s="72" t="s">
         <v>132</v>
       </c>
@@ -5305,7 +5514,7 @@
         <v>67</v>
       </c>
       <c r="E53" s="14" t="s">
-        <v>489</v>
+        <v>591</v>
       </c>
       <c r="F53" s="16" t="s">
         <v>73</v>
@@ -5329,7 +5538,7 @@
       </c>
       <c r="P53" s="34"/>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A54" s="72" t="s">
         <v>133</v>
       </c>
@@ -5343,7 +5552,7 @@
         <v>150</v>
       </c>
       <c r="E54" s="124" t="s">
-        <v>490</v>
+        <v>592</v>
       </c>
       <c r="F54" s="16" t="s">
         <v>65</v>
@@ -5367,7 +5576,7 @@
       </c>
       <c r="P54" s="34"/>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A55" s="72" t="s">
         <v>178</v>
       </c>
@@ -5381,7 +5590,7 @@
         <v>177</v>
       </c>
       <c r="E55" s="124" t="s">
-        <v>491</v>
+        <v>593</v>
       </c>
       <c r="F55" s="16" t="s">
         <v>179</v>
@@ -5405,7 +5614,7 @@
       </c>
       <c r="P55" s="34"/>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A56" s="72">
         <v>22</v>
       </c>
@@ -5419,7 +5628,7 @@
         <v>38</v>
       </c>
       <c r="E56" s="124" t="s">
-        <v>508</v>
+        <v>594</v>
       </c>
       <c r="F56" s="16" t="s">
         <v>170</v>
@@ -5443,7 +5652,7 @@
       </c>
       <c r="P56" s="34"/>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A57" s="72">
         <v>22.1</v>
       </c>
@@ -5457,7 +5666,7 @@
         <v>39</v>
       </c>
       <c r="E57" s="124" t="s">
-        <v>509</v>
+        <v>595</v>
       </c>
       <c r="F57" s="16" t="s">
         <v>171</v>
@@ -5481,7 +5690,7 @@
       </c>
       <c r="P57" s="34"/>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A58" s="72" t="s">
         <v>134</v>
       </c>
@@ -5495,7 +5704,7 @@
         <v>68</v>
       </c>
       <c r="E58" s="124" t="s">
-        <v>510</v>
+        <v>596</v>
       </c>
       <c r="F58" s="15" t="s">
         <v>167</v>
@@ -5519,7 +5728,7 @@
       </c>
       <c r="P58" s="34"/>
     </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A59" s="72" t="s">
         <v>135</v>
       </c>
@@ -5533,7 +5742,7 @@
         <v>151</v>
       </c>
       <c r="E59" s="124" t="s">
-        <v>511</v>
+        <v>597</v>
       </c>
       <c r="F59" s="15" t="s">
         <v>172</v>
@@ -5557,7 +5766,7 @@
       </c>
       <c r="P59" s="34"/>
     </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A60" s="72">
         <v>23</v>
       </c>
@@ -5571,7 +5780,7 @@
         <v>40</v>
       </c>
       <c r="E60" s="124" t="s">
-        <v>528</v>
+        <v>598</v>
       </c>
       <c r="F60" s="15" t="s">
         <v>78</v>
@@ -5595,7 +5804,7 @@
       </c>
       <c r="P60" s="34"/>
     </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A61" s="72">
         <v>23.1</v>
       </c>
@@ -5609,7 +5818,7 @@
         <v>41</v>
       </c>
       <c r="E61" s="124" t="s">
-        <v>529</v>
+        <v>599</v>
       </c>
       <c r="F61" s="15" t="s">
         <v>79</v>
@@ -5633,7 +5842,7 @@
       </c>
       <c r="P61" s="34"/>
     </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A62" s="72" t="s">
         <v>136</v>
       </c>
@@ -5647,7 +5856,7 @@
         <v>69</v>
       </c>
       <c r="E62" s="124" t="s">
-        <v>530</v>
+        <v>600</v>
       </c>
       <c r="F62" s="15" t="s">
         <v>76</v>
@@ -5671,7 +5880,7 @@
       </c>
       <c r="P62" s="34"/>
     </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A63" s="72" t="s">
         <v>137</v>
       </c>
@@ -5685,7 +5894,7 @@
         <v>152</v>
       </c>
       <c r="E63" s="124" t="s">
-        <v>531</v>
+        <v>601</v>
       </c>
       <c r="F63" s="15" t="s">
         <v>80</v>
@@ -5709,7 +5918,7 @@
       </c>
       <c r="P63" s="34"/>
     </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A64" s="72">
         <v>24</v>
       </c>
@@ -5723,7 +5932,7 @@
         <v>42</v>
       </c>
       <c r="E64" s="124" t="s">
-        <v>536</v>
+        <v>602</v>
       </c>
       <c r="F64" s="15" t="s">
         <v>85</v>
@@ -5747,7 +5956,7 @@
       </c>
       <c r="P64" s="34"/>
     </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A65" s="72">
         <v>24.1</v>
       </c>
@@ -5761,7 +5970,7 @@
         <v>43</v>
       </c>
       <c r="E65" s="124" t="s">
-        <v>537</v>
+        <v>603</v>
       </c>
       <c r="F65" s="15" t="s">
         <v>86</v>
@@ -5785,7 +5994,7 @@
       </c>
       <c r="P65" s="34"/>
     </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A66" s="72" t="s">
         <v>138</v>
       </c>
@@ -5799,7 +6008,7 @@
         <v>70</v>
       </c>
       <c r="E66" s="124" t="s">
-        <v>538</v>
+        <v>604</v>
       </c>
       <c r="F66" s="15" t="s">
         <v>83</v>
@@ -5823,7 +6032,7 @@
       </c>
       <c r="P66" s="34"/>
     </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A67" s="72" t="s">
         <v>139</v>
       </c>
@@ -5837,7 +6046,7 @@
         <v>153</v>
       </c>
       <c r="E67" s="124" t="s">
-        <v>539</v>
+        <v>605</v>
       </c>
       <c r="F67" s="15" t="s">
         <v>87</v>
@@ -5861,7 +6070,7 @@
       </c>
       <c r="P67" s="34"/>
     </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A68" s="72">
         <v>25</v>
       </c>
@@ -5875,7 +6084,7 @@
         <v>44</v>
       </c>
       <c r="E68" s="124" t="s">
-        <v>556</v>
+        <v>606</v>
       </c>
       <c r="F68" s="15" t="s">
         <v>92</v>
@@ -5899,7 +6108,7 @@
       </c>
       <c r="P68" s="34"/>
     </row>
-    <row r="69" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A69" s="72">
         <v>25.1</v>
       </c>
@@ -5913,7 +6122,7 @@
         <v>45</v>
       </c>
       <c r="E69" s="124" t="s">
-        <v>557</v>
+        <v>607</v>
       </c>
       <c r="F69" s="15" t="s">
         <v>93</v>
@@ -5937,7 +6146,7 @@
       </c>
       <c r="P69" s="34"/>
     </row>
-    <row r="70" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A70" s="43" t="s">
         <v>140</v>
       </c>
@@ -5951,7 +6160,7 @@
         <v>71</v>
       </c>
       <c r="E70" s="125" t="s">
-        <v>558</v>
+        <v>608</v>
       </c>
       <c r="F70" s="15" t="s">
         <v>90</v>
@@ -5975,7 +6184,7 @@
       </c>
       <c r="P70" s="34"/>
     </row>
-    <row r="71" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A71" s="72" t="s">
         <v>141</v>
       </c>
@@ -5989,7 +6198,7 @@
         <v>154</v>
       </c>
       <c r="E71" s="126" t="s">
-        <v>559</v>
+        <v>609</v>
       </c>
       <c r="F71" s="15" t="s">
         <v>173</v>
@@ -6013,7 +6222,7 @@
       </c>
       <c r="P71" s="34"/>
     </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A72" s="72">
         <v>26</v>
       </c>
@@ -6027,7 +6236,7 @@
         <v>123</v>
       </c>
       <c r="E72" s="124" t="s">
-        <v>123</v>
+        <v>610</v>
       </c>
       <c r="F72" s="16" t="s">
         <v>174</v>
@@ -6051,7 +6260,7 @@
       </c>
       <c r="P72" s="34"/>
     </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A73" s="72">
         <v>26.1</v>
       </c>
@@ -6065,7 +6274,7 @@
         <v>124</v>
       </c>
       <c r="E73" s="124" t="s">
-        <v>124</v>
+        <v>611</v>
       </c>
       <c r="F73" s="16" t="s">
         <v>145</v>
@@ -6089,7 +6298,7 @@
       </c>
       <c r="P73" s="34"/>
     </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A74" s="43" t="s">
         <v>142</v>
       </c>
@@ -6103,7 +6312,7 @@
         <v>125</v>
       </c>
       <c r="E74" s="74" t="s">
-        <v>125</v>
+        <v>612</v>
       </c>
       <c r="F74" s="17" t="s">
         <v>127</v>
@@ -6127,7 +6336,7 @@
       </c>
       <c r="P74" s="34"/>
     </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A75" s="72" t="s">
         <v>143</v>
       </c>
@@ -6141,7 +6350,7 @@
         <v>155</v>
       </c>
       <c r="E75" s="126" t="s">
-        <v>155</v>
+        <v>613</v>
       </c>
       <c r="F75" s="30" t="s">
         <v>148</v>
@@ -6165,7 +6374,7 @@
       </c>
       <c r="P75" s="34"/>
     </row>
-    <row r="76" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="76" spans="1:16" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A76" s="110" t="s">
         <v>144</v>
       </c>
@@ -6179,7 +6388,7 @@
         <v>157</v>
       </c>
       <c r="E76" s="128" t="s">
-        <v>157</v>
+        <v>614</v>
       </c>
       <c r="F76" s="70" t="s">
         <v>146</v>
@@ -6203,7 +6412,7 @@
       </c>
       <c r="P76" s="41"/>
     </row>
-    <row r="77" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A77" s="56">
         <v>65</v>
       </c>
@@ -6239,7 +6448,7 @@
       <c r="O77" s="34"/>
       <c r="P77" s="34"/>
     </row>
-    <row r="78" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A78" s="56">
         <v>66</v>
       </c>
@@ -6275,7 +6484,7 @@
       <c r="O78" s="34"/>
       <c r="P78" s="34"/>
     </row>
-    <row r="79" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A79" s="56">
         <v>67</v>
       </c>
@@ -6313,7 +6522,7 @@
       <c r="O79" s="34"/>
       <c r="P79" s="34"/>
     </row>
-    <row r="80" spans="1:16" ht="14.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="80" spans="1:16" ht="14.55" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A80" s="112">
         <v>68</v>
       </c>
@@ -6351,7 +6560,7 @@
       <c r="O80" s="85"/>
       <c r="P80" s="85"/>
     </row>
-    <row r="81" spans="1:16" ht="14.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:16" ht="14.55" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
       <c r="A81" s="56">
         <v>69</v>
       </c>
@@ -6365,7 +6574,7 @@
         <v>419</v>
       </c>
       <c r="E81" s="129" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="F81" s="71" t="s">
         <v>191</v>
@@ -6389,7 +6598,7 @@
       </c>
       <c r="P81" s="34"/>
     </row>
-    <row r="82" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A82" s="56">
         <v>70</v>
       </c>
@@ -6403,7 +6612,7 @@
         <v>420</v>
       </c>
       <c r="E82" s="129" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="F82" s="71" t="s">
         <v>192</v>
@@ -6427,7 +6636,7 @@
       </c>
       <c r="P82" s="34"/>
     </row>
-    <row r="83" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A83" s="56">
         <v>71</v>
       </c>
@@ -6441,7 +6650,7 @@
         <v>421</v>
       </c>
       <c r="E83" s="129" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="F83" s="71" t="s">
         <v>193</v>
@@ -6465,7 +6674,7 @@
       </c>
       <c r="P83" s="34"/>
     </row>
-    <row r="84" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A84" s="56">
         <v>72</v>
       </c>
@@ -6479,7 +6688,7 @@
         <v>422</v>
       </c>
       <c r="E84" s="129" t="s">
-        <v>492</v>
+        <v>486</v>
       </c>
       <c r="F84" s="71" t="s">
         <v>445</v>
@@ -6503,7 +6712,7 @@
       </c>
       <c r="P84" s="34"/>
     </row>
-    <row r="85" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A85" s="56">
         <v>73</v>
       </c>
@@ -6517,7 +6726,7 @@
         <v>423</v>
       </c>
       <c r="E85" s="129" t="s">
-        <v>493</v>
+        <v>487</v>
       </c>
       <c r="F85" s="71" t="s">
         <v>446</v>
@@ -6541,7 +6750,7 @@
       </c>
       <c r="P85" s="34"/>
     </row>
-    <row r="86" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A86" s="56">
         <v>74</v>
       </c>
@@ -6555,7 +6764,7 @@
         <v>424</v>
       </c>
       <c r="E86" s="129" t="s">
-        <v>512</v>
+        <v>502</v>
       </c>
       <c r="F86" s="2" t="s">
         <v>194</v>
@@ -6579,7 +6788,7 @@
       </c>
       <c r="P86" s="34"/>
     </row>
-    <row r="87" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A87" s="56">
         <v>75</v>
       </c>
@@ -6593,7 +6802,7 @@
         <v>425</v>
       </c>
       <c r="E87" s="129" t="s">
-        <v>513</v>
+        <v>503</v>
       </c>
       <c r="F87" s="2" t="s">
         <v>195</v>
@@ -6617,7 +6826,7 @@
       </c>
       <c r="P87" s="34"/>
     </row>
-    <row r="88" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A88" s="56">
         <v>76</v>
       </c>
@@ -6631,7 +6840,7 @@
         <v>426</v>
       </c>
       <c r="E88" s="129" t="s">
-        <v>532</v>
+        <v>518</v>
       </c>
       <c r="F88" s="2" t="s">
         <v>196</v>
@@ -6655,7 +6864,7 @@
       </c>
       <c r="P88" s="34"/>
     </row>
-    <row r="89" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A89" s="56">
         <v>77</v>
       </c>
@@ -6669,7 +6878,7 @@
         <v>427</v>
       </c>
       <c r="E89" s="129" t="s">
-        <v>533</v>
+        <v>519</v>
       </c>
       <c r="F89" s="2" t="s">
         <v>197</v>
@@ -6693,7 +6902,7 @@
       </c>
       <c r="P89" s="34"/>
     </row>
-    <row r="90" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A90" s="56">
         <v>78</v>
       </c>
@@ -6707,7 +6916,7 @@
         <v>428</v>
       </c>
       <c r="E90" s="129" t="s">
-        <v>540</v>
+        <v>522</v>
       </c>
       <c r="F90" s="2" t="s">
         <v>198</v>
@@ -6731,7 +6940,7 @@
       </c>
       <c r="P90" s="34"/>
     </row>
-    <row r="91" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A91" s="56">
         <v>79</v>
       </c>
@@ -6745,7 +6954,7 @@
         <v>429</v>
       </c>
       <c r="E91" s="129" t="s">
-        <v>541</v>
+        <v>523</v>
       </c>
       <c r="F91" s="2" t="s">
         <v>199</v>
@@ -6769,7 +6978,7 @@
       </c>
       <c r="P91" s="34"/>
     </row>
-    <row r="92" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A92" s="56">
         <v>80</v>
       </c>
@@ -6783,7 +6992,7 @@
         <v>430</v>
       </c>
       <c r="E92" s="131" t="s">
-        <v>560</v>
+        <v>538</v>
       </c>
       <c r="F92" s="4" t="s">
         <v>200</v>
@@ -6807,7 +7016,7 @@
       </c>
       <c r="P92" s="45"/>
     </row>
-    <row r="93" spans="1:16" ht="14.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="93" spans="1:16" ht="14.55" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A93" s="52">
         <v>81</v>
       </c>
@@ -6821,7 +7030,7 @@
         <v>431</v>
       </c>
       <c r="E93" s="132" t="s">
-        <v>561</v>
+        <v>539</v>
       </c>
       <c r="F93" s="24" t="s">
         <v>201</v>
@@ -6845,7 +7054,7 @@
       </c>
       <c r="P93" s="55"/>
     </row>
-    <row r="94" spans="1:16" ht="14.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:16" ht="14.55" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
       <c r="A94" s="56">
         <v>82</v>
       </c>
@@ -6859,7 +7068,7 @@
         <v>432</v>
       </c>
       <c r="E94" s="129" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="F94" s="71" t="s">
         <v>241</v>
@@ -6883,7 +7092,7 @@
       </c>
       <c r="P94" s="57"/>
     </row>
-    <row r="95" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A95" s="56">
         <v>83</v>
       </c>
@@ -6897,7 +7106,7 @@
         <v>433</v>
       </c>
       <c r="E95" s="129" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="F95" s="71" t="s">
         <v>202</v>
@@ -6921,7 +7130,7 @@
       </c>
       <c r="P95" s="58"/>
     </row>
-    <row r="96" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A96" s="56">
         <v>84</v>
       </c>
@@ -6935,7 +7144,7 @@
         <v>434</v>
       </c>
       <c r="E96" s="129" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="F96" s="71" t="s">
         <v>203</v>
@@ -6959,7 +7168,7 @@
       </c>
       <c r="P96" s="58"/>
     </row>
-    <row r="97" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A97" s="56">
         <v>85</v>
       </c>
@@ -6973,7 +7182,7 @@
         <v>435</v>
       </c>
       <c r="E97" s="129" t="s">
-        <v>494</v>
+        <v>488</v>
       </c>
       <c r="F97" s="71" t="s">
         <v>447</v>
@@ -6997,7 +7206,7 @@
       </c>
       <c r="P97" s="58"/>
     </row>
-    <row r="98" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A98" s="56">
         <v>86</v>
       </c>
@@ -7011,7 +7220,7 @@
         <v>436</v>
       </c>
       <c r="E98" s="129" t="s">
-        <v>495</v>
+        <v>489</v>
       </c>
       <c r="F98" s="71" t="s">
         <v>448</v>
@@ -7035,7 +7244,7 @@
       </c>
       <c r="P98" s="58"/>
     </row>
-    <row r="99" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A99" s="56">
         <v>87</v>
       </c>
@@ -7049,7 +7258,7 @@
         <v>437</v>
       </c>
       <c r="E99" s="129" t="s">
-        <v>514</v>
+        <v>504</v>
       </c>
       <c r="F99" s="2" t="s">
         <v>204</v>
@@ -7073,7 +7282,7 @@
       </c>
       <c r="P99" s="58"/>
     </row>
-    <row r="100" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A100" s="56">
         <v>88</v>
       </c>
@@ -7087,7 +7296,7 @@
         <v>438</v>
       </c>
       <c r="E100" s="129" t="s">
-        <v>515</v>
+        <v>505</v>
       </c>
       <c r="F100" s="2" t="s">
         <v>205</v>
@@ -7111,7 +7320,7 @@
       </c>
       <c r="P100" s="58"/>
     </row>
-    <row r="101" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A101" s="56">
         <v>89</v>
       </c>
@@ -7125,7 +7334,7 @@
         <v>439</v>
       </c>
       <c r="E101" s="129" t="s">
-        <v>534</v>
+        <v>520</v>
       </c>
       <c r="F101" s="2" t="s">
         <v>206</v>
@@ -7149,7 +7358,7 @@
       </c>
       <c r="P101" s="58"/>
     </row>
-    <row r="102" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A102" s="56">
         <v>90</v>
       </c>
@@ -7163,7 +7372,7 @@
         <v>440</v>
       </c>
       <c r="E102" s="129" t="s">
-        <v>535</v>
+        <v>521</v>
       </c>
       <c r="F102" s="2" t="s">
         <v>207</v>
@@ -7187,7 +7396,7 @@
       </c>
       <c r="P102" s="58"/>
     </row>
-    <row r="103" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A103" s="56">
         <v>91</v>
       </c>
@@ -7201,7 +7410,7 @@
         <v>441</v>
       </c>
       <c r="E103" s="129" t="s">
-        <v>542</v>
+        <v>524</v>
       </c>
       <c r="F103" s="2" t="s">
         <v>208</v>
@@ -7225,7 +7434,7 @@
       </c>
       <c r="P103" s="58"/>
     </row>
-    <row r="104" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A104" s="56">
         <v>92</v>
       </c>
@@ -7239,7 +7448,7 @@
         <v>442</v>
       </c>
       <c r="E104" s="129" t="s">
-        <v>543</v>
+        <v>525</v>
       </c>
       <c r="F104" s="2" t="s">
         <v>209</v>
@@ -7263,7 +7472,7 @@
       </c>
       <c r="P104" s="58"/>
     </row>
-    <row r="105" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A105" s="56">
         <v>93</v>
       </c>
@@ -7277,7 +7486,7 @@
         <v>443</v>
       </c>
       <c r="E105" s="131" t="s">
-        <v>562</v>
+        <v>540</v>
       </c>
       <c r="F105" s="4" t="s">
         <v>210</v>
@@ -7301,7 +7510,7 @@
       </c>
       <c r="P105" s="58"/>
     </row>
-    <row r="106" spans="1:16" ht="14.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="106" spans="1:16" ht="14.55" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A106" s="59">
         <v>94</v>
       </c>
@@ -7315,7 +7524,7 @@
         <v>444</v>
       </c>
       <c r="E106" s="133" t="s">
-        <v>563</v>
+        <v>541</v>
       </c>
       <c r="F106" s="76" t="s">
         <v>211</v>
@@ -7339,7 +7548,7 @@
       </c>
       <c r="P106" s="60"/>
     </row>
-    <row r="107" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A107" s="77">
         <v>95</v>
       </c>
@@ -7377,7 +7586,7 @@
       <c r="O107" s="79"/>
       <c r="P107" s="79"/>
     </row>
-    <row r="108" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A108" s="75">
         <v>96</v>
       </c>
@@ -7415,7 +7624,7 @@
       <c r="O108" s="62"/>
       <c r="P108" s="62"/>
     </row>
-    <row r="109" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A109" s="75">
         <v>97</v>
       </c>
@@ -7453,7 +7662,7 @@
       <c r="O109" s="62"/>
       <c r="P109" s="62"/>
     </row>
-    <row r="110" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A110" s="75">
         <v>98</v>
       </c>
@@ -7489,7 +7698,7 @@
       <c r="O110" s="62"/>
       <c r="P110" s="62"/>
     </row>
-    <row r="111" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A111" s="75">
         <v>99</v>
       </c>
@@ -7525,7 +7734,7 @@
       <c r="O111" s="62"/>
       <c r="P111" s="62"/>
     </row>
-    <row r="112" spans="1:16" ht="14.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="112" spans="1:16" ht="14.55" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A112" s="52">
         <v>100</v>
       </c>
@@ -7561,7 +7770,7 @@
       <c r="O112" s="81"/>
       <c r="P112" s="81"/>
     </row>
-    <row r="113" spans="1:16" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:16" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
       <c r="A113" s="75">
         <v>101</v>
       </c>
@@ -7575,7 +7784,7 @@
         <v>185</v>
       </c>
       <c r="E113" s="129" t="s">
-        <v>185</v>
+        <v>558</v>
       </c>
       <c r="F113" s="71" t="s">
         <v>225</v>
@@ -7597,7 +7806,7 @@
       <c r="O113" s="34"/>
       <c r="P113" s="34"/>
     </row>
-    <row r="114" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A114" s="75">
         <v>102</v>
       </c>
@@ -7611,7 +7820,7 @@
         <v>186</v>
       </c>
       <c r="E114" s="129" t="s">
-        <v>186</v>
+        <v>559</v>
       </c>
       <c r="F114" s="71" t="s">
         <v>226</v>
@@ -7633,7 +7842,7 @@
       <c r="O114" s="34"/>
       <c r="P114" s="34"/>
     </row>
-    <row r="115" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A115" s="75">
         <v>103</v>
       </c>
@@ -7647,7 +7856,7 @@
         <v>187</v>
       </c>
       <c r="E115" s="129" t="s">
-        <v>187</v>
+        <v>560</v>
       </c>
       <c r="F115" s="71" t="s">
         <v>227</v>
@@ -7671,7 +7880,7 @@
       <c r="O115" s="34"/>
       <c r="P115" s="34"/>
     </row>
-    <row r="116" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="116" spans="1:16" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A116" s="52">
         <v>104</v>
       </c>
@@ -7685,7 +7894,7 @@
         <v>188</v>
       </c>
       <c r="E116" s="130" t="s">
-        <v>188</v>
+        <v>561</v>
       </c>
       <c r="F116" s="84" t="s">
         <v>228</v>
@@ -7709,7 +7918,7 @@
       <c r="O116" s="85"/>
       <c r="P116" s="85"/>
     </row>
-    <row r="117" spans="1:16" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:16" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
       <c r="A117" s="61">
         <v>105</v>
       </c>
@@ -7723,7 +7932,7 @@
         <v>419</v>
       </c>
       <c r="E117" s="20" t="s">
-        <v>465</v>
+        <v>562</v>
       </c>
       <c r="F117" s="6" t="s">
         <v>229</v>
@@ -7747,7 +7956,7 @@
       </c>
       <c r="P117" s="62"/>
     </row>
-    <row r="118" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A118" s="61">
         <v>106</v>
       </c>
@@ -7761,7 +7970,7 @@
         <v>420</v>
       </c>
       <c r="E118" s="21" t="s">
-        <v>466</v>
+        <v>563</v>
       </c>
       <c r="F118" s="3" t="s">
         <v>230</v>
@@ -7785,7 +7994,7 @@
       </c>
       <c r="P118" s="63"/>
     </row>
-    <row r="119" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A119" s="61">
         <v>107</v>
       </c>
@@ -7799,7 +8008,7 @@
         <v>421</v>
       </c>
       <c r="E119" s="21" t="s">
-        <v>467</v>
+        <v>564</v>
       </c>
       <c r="F119" s="3" t="s">
         <v>231</v>
@@ -7823,7 +8032,7 @@
       </c>
       <c r="P119" s="63"/>
     </row>
-    <row r="120" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A120" s="61">
         <v>108</v>
       </c>
@@ -7837,7 +8046,7 @@
         <v>422</v>
       </c>
       <c r="E120" s="21" t="s">
-        <v>492</v>
+        <v>565</v>
       </c>
       <c r="F120" s="3" t="s">
         <v>449</v>
@@ -7861,7 +8070,7 @@
       </c>
       <c r="P120" s="63"/>
     </row>
-    <row r="121" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A121" s="61">
         <v>109</v>
       </c>
@@ -7875,7 +8084,7 @@
         <v>423</v>
       </c>
       <c r="E121" s="21" t="s">
-        <v>493</v>
+        <v>566</v>
       </c>
       <c r="F121" s="3" t="s">
         <v>450</v>
@@ -7899,7 +8108,7 @@
       </c>
       <c r="P121" s="63"/>
     </row>
-    <row r="122" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A122" s="61">
         <v>110</v>
       </c>
@@ -7913,7 +8122,7 @@
         <v>424</v>
       </c>
       <c r="E122" s="21" t="s">
-        <v>512</v>
+        <v>567</v>
       </c>
       <c r="F122" s="3" t="s">
         <v>232</v>
@@ -7937,7 +8146,7 @@
       </c>
       <c r="P122" s="63"/>
     </row>
-    <row r="123" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A123" s="61">
         <v>111</v>
       </c>
@@ -7951,7 +8160,7 @@
         <v>425</v>
       </c>
       <c r="E123" s="21" t="s">
-        <v>513</v>
+        <v>568</v>
       </c>
       <c r="F123" s="3" t="s">
         <v>233</v>
@@ -7975,7 +8184,7 @@
       </c>
       <c r="P123" s="63"/>
     </row>
-    <row r="124" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A124" s="61">
         <v>112</v>
       </c>
@@ -7989,7 +8198,7 @@
         <v>426</v>
       </c>
       <c r="E124" s="21" t="s">
-        <v>532</v>
+        <v>569</v>
       </c>
       <c r="F124" s="3" t="s">
         <v>234</v>
@@ -8013,7 +8222,7 @@
       </c>
       <c r="P124" s="63"/>
     </row>
-    <row r="125" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A125" s="61">
         <v>113</v>
       </c>
@@ -8027,7 +8236,7 @@
         <v>427</v>
       </c>
       <c r="E125" s="21" t="s">
-        <v>533</v>
+        <v>570</v>
       </c>
       <c r="F125" s="3" t="s">
         <v>235</v>
@@ -8051,7 +8260,7 @@
       </c>
       <c r="P125" s="63"/>
     </row>
-    <row r="126" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A126" s="61">
         <v>114</v>
       </c>
@@ -8065,7 +8274,7 @@
         <v>428</v>
       </c>
       <c r="E126" s="21" t="s">
-        <v>540</v>
+        <v>571</v>
       </c>
       <c r="F126" s="3" t="s">
         <v>236</v>
@@ -8089,7 +8298,7 @@
       </c>
       <c r="P126" s="63"/>
     </row>
-    <row r="127" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A127" s="61">
         <v>115</v>
       </c>
@@ -8103,7 +8312,7 @@
         <v>429</v>
       </c>
       <c r="E127" s="21" t="s">
-        <v>541</v>
+        <v>572</v>
       </c>
       <c r="F127" s="3" t="s">
         <v>237</v>
@@ -8127,7 +8336,7 @@
       </c>
       <c r="P127" s="63"/>
     </row>
-    <row r="128" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A128" s="61">
         <v>116</v>
       </c>
@@ -8141,7 +8350,7 @@
         <v>430</v>
       </c>
       <c r="E128" s="21" t="s">
-        <v>560</v>
+        <v>573</v>
       </c>
       <c r="F128" s="3" t="s">
         <v>238</v>
@@ -8165,7 +8374,7 @@
       </c>
       <c r="P128" s="63"/>
     </row>
-    <row r="129" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="129" spans="1:16" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A129" s="52">
         <v>117</v>
       </c>
@@ -8179,7 +8388,7 @@
         <v>431</v>
       </c>
       <c r="E129" s="137" t="s">
-        <v>561</v>
+        <v>574</v>
       </c>
       <c r="F129" s="7" t="s">
         <v>239</v>
@@ -8203,7 +8412,7 @@
       </c>
       <c r="P129" s="64"/>
     </row>
-    <row r="130" spans="1:16" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:16" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
       <c r="A130" s="61">
         <v>118</v>
       </c>
@@ -8217,7 +8426,7 @@
         <v>432</v>
       </c>
       <c r="E130" s="20" t="s">
-        <v>468</v>
+        <v>575</v>
       </c>
       <c r="F130" s="6" t="s">
         <v>240</v>
@@ -8241,7 +8450,7 @@
       </c>
       <c r="P130" s="62"/>
     </row>
-    <row r="131" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A131" s="61">
         <v>119</v>
       </c>
@@ -8255,7 +8464,7 @@
         <v>433</v>
       </c>
       <c r="E131" s="21" t="s">
-        <v>469</v>
+        <v>576</v>
       </c>
       <c r="F131" s="3" t="s">
         <v>242</v>
@@ -8279,7 +8488,7 @@
       </c>
       <c r="P131" s="63"/>
     </row>
-    <row r="132" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A132" s="61">
         <v>120</v>
       </c>
@@ -8293,7 +8502,7 @@
         <v>434</v>
       </c>
       <c r="E132" s="21" t="s">
-        <v>470</v>
+        <v>577</v>
       </c>
       <c r="F132" s="3" t="s">
         <v>243</v>
@@ -8317,7 +8526,7 @@
       </c>
       <c r="P132" s="63"/>
     </row>
-    <row r="133" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A133" s="61">
         <v>121</v>
       </c>
@@ -8331,7 +8540,7 @@
         <v>435</v>
       </c>
       <c r="E133" s="21" t="s">
-        <v>494</v>
+        <v>578</v>
       </c>
       <c r="F133" s="3" t="s">
         <v>451</v>
@@ -8355,7 +8564,7 @@
       </c>
       <c r="P133" s="63"/>
     </row>
-    <row r="134" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A134" s="61">
         <v>122</v>
       </c>
@@ -8369,7 +8578,7 @@
         <v>436</v>
       </c>
       <c r="E134" s="21" t="s">
-        <v>495</v>
+        <v>579</v>
       </c>
       <c r="F134" s="3" t="s">
         <v>452</v>
@@ -8393,7 +8602,7 @@
       </c>
       <c r="P134" s="63"/>
     </row>
-    <row r="135" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A135" s="61">
         <v>123</v>
       </c>
@@ -8407,7 +8616,7 @@
         <v>437</v>
       </c>
       <c r="E135" s="21" t="s">
-        <v>514</v>
+        <v>580</v>
       </c>
       <c r="F135" s="3" t="s">
         <v>244</v>
@@ -8431,7 +8640,7 @@
       </c>
       <c r="P135" s="63"/>
     </row>
-    <row r="136" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A136" s="61">
         <v>124</v>
       </c>
@@ -8445,7 +8654,7 @@
         <v>438</v>
       </c>
       <c r="E136" s="21" t="s">
-        <v>515</v>
+        <v>581</v>
       </c>
       <c r="F136" s="3" t="s">
         <v>245</v>
@@ -8469,7 +8678,7 @@
       </c>
       <c r="P136" s="63"/>
     </row>
-    <row r="137" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A137" s="61">
         <v>125</v>
       </c>
@@ -8483,7 +8692,7 @@
         <v>439</v>
       </c>
       <c r="E137" s="21" t="s">
-        <v>534</v>
+        <v>582</v>
       </c>
       <c r="F137" s="3" t="s">
         <v>246</v>
@@ -8507,7 +8716,7 @@
       </c>
       <c r="P137" s="63"/>
     </row>
-    <row r="138" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A138" s="61">
         <v>126</v>
       </c>
@@ -8521,7 +8730,7 @@
         <v>440</v>
       </c>
       <c r="E138" s="21" t="s">
-        <v>535</v>
+        <v>583</v>
       </c>
       <c r="F138" s="3" t="s">
         <v>247</v>
@@ -8545,7 +8754,7 @@
       </c>
       <c r="P138" s="63"/>
     </row>
-    <row r="139" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A139" s="61">
         <v>127</v>
       </c>
@@ -8559,7 +8768,7 @@
         <v>441</v>
       </c>
       <c r="E139" s="21" t="s">
-        <v>542</v>
+        <v>584</v>
       </c>
       <c r="F139" s="3" t="s">
         <v>248</v>
@@ -8583,7 +8792,7 @@
       </c>
       <c r="P139" s="63"/>
     </row>
-    <row r="140" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A140" s="61">
         <v>128</v>
       </c>
@@ -8597,7 +8806,7 @@
         <v>442</v>
       </c>
       <c r="E140" s="21" t="s">
-        <v>543</v>
+        <v>585</v>
       </c>
       <c r="F140" s="3" t="s">
         <v>249</v>
@@ -8621,7 +8830,7 @@
       </c>
       <c r="P140" s="63"/>
     </row>
-    <row r="141" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A141" s="61">
         <v>129</v>
       </c>
@@ -8635,7 +8844,7 @@
         <v>443</v>
       </c>
       <c r="E141" s="21" t="s">
-        <v>562</v>
+        <v>586</v>
       </c>
       <c r="F141" s="3" t="s">
         <v>250</v>
@@ -8659,7 +8868,7 @@
       </c>
       <c r="P141" s="63"/>
     </row>
-    <row r="142" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="142" spans="1:16" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A142" s="59">
         <v>130</v>
       </c>
@@ -8673,7 +8882,7 @@
         <v>444</v>
       </c>
       <c r="E142" s="23" t="s">
-        <v>563</v>
+        <v>587</v>
       </c>
       <c r="F142" s="8" t="s">
         <v>251</v>
@@ -8697,7 +8906,7 @@
       </c>
       <c r="P142" s="65"/>
     </row>
-    <row r="143" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A143" s="113">
         <v>131</v>
       </c>
@@ -8737,7 +8946,7 @@
       </c>
       <c r="P143" s="66"/>
     </row>
-    <row r="144" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A144" s="113">
         <v>132</v>
       </c>
@@ -8751,7 +8960,7 @@
         <v>254</v>
       </c>
       <c r="E144" s="129" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="F144" s="2" t="s">
         <v>277</v>
@@ -8775,7 +8984,7 @@
       </c>
       <c r="P144" s="66"/>
     </row>
-    <row r="145" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A145" s="113">
         <v>133</v>
       </c>
@@ -8789,7 +8998,7 @@
         <v>255</v>
       </c>
       <c r="E145" s="129" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="F145" s="2" t="s">
         <v>277</v>
@@ -8813,7 +9022,7 @@
       </c>
       <c r="P145" s="66"/>
     </row>
-    <row r="146" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A146" s="113">
         <v>134</v>
       </c>
@@ -8827,7 +9036,7 @@
         <v>256</v>
       </c>
       <c r="E146" s="129" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="F146" s="2" t="s">
         <v>278</v>
@@ -8851,7 +9060,7 @@
       </c>
       <c r="P146" s="66"/>
     </row>
-    <row r="147" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A147" s="113">
         <v>135</v>
       </c>
@@ -8865,7 +9074,7 @@
         <v>257</v>
       </c>
       <c r="E147" s="129" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="F147" s="2" t="s">
         <v>279</v>
@@ -8889,7 +9098,7 @@
       </c>
       <c r="P147" s="66"/>
     </row>
-    <row r="148" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A148" s="113">
         <v>136</v>
       </c>
@@ -8903,7 +9112,7 @@
         <v>258</v>
       </c>
       <c r="E148" s="129" t="s">
-        <v>496</v>
+        <v>490</v>
       </c>
       <c r="F148" s="2" t="s">
         <v>280</v>
@@ -8927,7 +9136,7 @@
       </c>
       <c r="P148" s="66"/>
     </row>
-    <row r="149" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A149" s="113">
         <v>137</v>
       </c>
@@ -8941,7 +9150,7 @@
         <v>259</v>
       </c>
       <c r="E149" s="129" t="s">
-        <v>497</v>
+        <v>491</v>
       </c>
       <c r="F149" s="2" t="s">
         <v>280</v>
@@ -8965,7 +9174,7 @@
       </c>
       <c r="P149" s="66"/>
     </row>
-    <row r="150" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A150" s="113">
         <v>138</v>
       </c>
@@ -8979,7 +9188,7 @@
         <v>260</v>
       </c>
       <c r="E150" s="129" t="s">
-        <v>498</v>
+        <v>492</v>
       </c>
       <c r="F150" s="2" t="s">
         <v>281</v>
@@ -9003,7 +9212,7 @@
       </c>
       <c r="P150" s="66"/>
     </row>
-    <row r="151" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A151" s="113">
         <v>139</v>
       </c>
@@ -9017,7 +9226,7 @@
         <v>261</v>
       </c>
       <c r="E151" s="129" t="s">
-        <v>516</v>
+        <v>506</v>
       </c>
       <c r="F151" s="2" t="s">
         <v>282</v>
@@ -9041,7 +9250,7 @@
       </c>
       <c r="P151" s="66"/>
     </row>
-    <row r="152" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A152" s="113">
         <v>140</v>
       </c>
@@ -9055,7 +9264,7 @@
         <v>262</v>
       </c>
       <c r="E152" s="129" t="s">
-        <v>517</v>
+        <v>507</v>
       </c>
       <c r="F152" s="2" t="s">
         <v>282</v>
@@ -9079,7 +9288,7 @@
       </c>
       <c r="P152" s="66"/>
     </row>
-    <row r="153" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A153" s="113">
         <v>141</v>
       </c>
@@ -9093,7 +9302,7 @@
         <v>263</v>
       </c>
       <c r="E153" s="129" t="s">
-        <v>518</v>
+        <v>508</v>
       </c>
       <c r="F153" s="2" t="s">
         <v>283</v>
@@ -9117,7 +9326,7 @@
       </c>
       <c r="P153" s="66"/>
     </row>
-    <row r="154" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A154" s="113">
         <v>142</v>
       </c>
@@ -9155,7 +9364,7 @@
       </c>
       <c r="P154" s="66"/>
     </row>
-    <row r="155" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A155" s="113">
         <v>143</v>
       </c>
@@ -9193,7 +9402,7 @@
       </c>
       <c r="P155" s="66"/>
     </row>
-    <row r="156" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A156" s="113">
         <v>144</v>
       </c>
@@ -9231,7 +9440,7 @@
       </c>
       <c r="P156" s="66"/>
     </row>
-    <row r="157" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A157" s="113">
         <v>145</v>
       </c>
@@ -9245,7 +9454,7 @@
         <v>267</v>
       </c>
       <c r="E157" s="129" t="s">
-        <v>544</v>
+        <v>526</v>
       </c>
       <c r="F157" s="2" t="s">
         <v>286</v>
@@ -9269,7 +9478,7 @@
       </c>
       <c r="P157" s="66"/>
     </row>
-    <row r="158" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A158" s="113">
         <v>146</v>
       </c>
@@ -9283,7 +9492,7 @@
         <v>268</v>
       </c>
       <c r="E158" s="129" t="s">
-        <v>545</v>
+        <v>527</v>
       </c>
       <c r="F158" s="2" t="s">
         <v>286</v>
@@ -9307,7 +9516,7 @@
       </c>
       <c r="P158" s="66"/>
     </row>
-    <row r="159" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A159" s="113">
         <v>147</v>
       </c>
@@ -9321,7 +9530,7 @@
         <v>269</v>
       </c>
       <c r="E159" s="129" t="s">
-        <v>546</v>
+        <v>528</v>
       </c>
       <c r="F159" s="2" t="s">
         <v>287</v>
@@ -9345,7 +9554,7 @@
       </c>
       <c r="P159" s="66"/>
     </row>
-    <row r="160" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A160" s="113">
         <v>148</v>
       </c>
@@ -9359,7 +9568,7 @@
         <v>270</v>
       </c>
       <c r="E160" s="129" t="s">
-        <v>564</v>
+        <v>542</v>
       </c>
       <c r="F160" s="2" t="s">
         <v>288</v>
@@ -9383,7 +9592,7 @@
       </c>
       <c r="P160" s="66"/>
     </row>
-    <row r="161" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A161" s="113">
         <v>149</v>
       </c>
@@ -9397,7 +9606,7 @@
         <v>271</v>
       </c>
       <c r="E161" s="129" t="s">
-        <v>565</v>
+        <v>543</v>
       </c>
       <c r="F161" s="2" t="s">
         <v>288</v>
@@ -9421,7 +9630,7 @@
       </c>
       <c r="P161" s="66"/>
     </row>
-    <row r="162" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A162" s="113">
         <v>150</v>
       </c>
@@ -9435,7 +9644,7 @@
         <v>272</v>
       </c>
       <c r="E162" s="129" t="s">
-        <v>566</v>
+        <v>544</v>
       </c>
       <c r="F162" s="2" t="s">
         <v>289</v>
@@ -9459,7 +9668,7 @@
       </c>
       <c r="P162" s="66"/>
     </row>
-    <row r="163" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A163" s="113">
         <v>151</v>
       </c>
@@ -9497,7 +9706,7 @@
       </c>
       <c r="P163" s="66"/>
     </row>
-    <row r="164" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A164" s="113">
         <v>152</v>
       </c>
@@ -9535,7 +9744,7 @@
       </c>
       <c r="P164" s="66"/>
     </row>
-    <row r="165" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A165" s="113">
         <v>153</v>
       </c>
@@ -9573,7 +9782,7 @@
       </c>
       <c r="P165" s="66"/>
     </row>
-    <row r="166" spans="1:16" s="83" customFormat="1" ht="14.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="166" spans="1:16" s="83" customFormat="1" ht="14.55" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A166" s="114">
         <v>154</v>
       </c>
@@ -9611,7 +9820,7 @@
       </c>
       <c r="P166" s="68"/>
     </row>
-    <row r="167" spans="1:16" ht="14.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:16" ht="14.55" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
       <c r="A167" s="113">
         <v>155</v>
       </c>
@@ -9651,7 +9860,7 @@
       </c>
       <c r="P167" s="66"/>
     </row>
-    <row r="168" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A168" s="113">
         <v>156</v>
       </c>
@@ -9665,7 +9874,7 @@
         <v>294</v>
       </c>
       <c r="E168" s="129" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="F168" s="2" t="s">
         <v>295</v>
@@ -9689,7 +9898,7 @@
       </c>
       <c r="P168" s="66"/>
     </row>
-    <row r="169" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A169" s="113">
         <v>157</v>
       </c>
@@ -9703,7 +9912,7 @@
         <v>296</v>
       </c>
       <c r="E169" s="129" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="F169" s="2" t="s">
         <v>295</v>
@@ -9727,7 +9936,7 @@
       </c>
       <c r="P169" s="66"/>
     </row>
-    <row r="170" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A170" s="113">
         <v>158</v>
       </c>
@@ -9741,7 +9950,7 @@
         <v>297</v>
       </c>
       <c r="E170" s="129" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="F170" s="2" t="s">
         <v>298</v>
@@ -9765,7 +9974,7 @@
       </c>
       <c r="P170" s="66"/>
     </row>
-    <row r="171" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A171" s="113">
         <v>159</v>
       </c>
@@ -9779,7 +9988,7 @@
         <v>299</v>
       </c>
       <c r="E171" s="129" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="F171" s="2" t="s">
         <v>300</v>
@@ -9803,7 +10012,7 @@
       </c>
       <c r="P171" s="66"/>
     </row>
-    <row r="172" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A172" s="113">
         <v>160</v>
       </c>
@@ -9817,7 +10026,7 @@
         <v>301</v>
       </c>
       <c r="E172" s="129" t="s">
-        <v>499</v>
+        <v>493</v>
       </c>
       <c r="F172" s="2" t="s">
         <v>302</v>
@@ -9841,7 +10050,7 @@
       </c>
       <c r="P172" s="66"/>
     </row>
-    <row r="173" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A173" s="113">
         <v>161</v>
       </c>
@@ -9855,7 +10064,7 @@
         <v>303</v>
       </c>
       <c r="E173" s="129" t="s">
-        <v>500</v>
+        <v>494</v>
       </c>
       <c r="F173" s="2" t="s">
         <v>302</v>
@@ -9879,7 +10088,7 @@
       </c>
       <c r="P173" s="66"/>
     </row>
-    <row r="174" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A174" s="113">
         <v>162</v>
       </c>
@@ -9893,7 +10102,7 @@
         <v>304</v>
       </c>
       <c r="E174" s="129" t="s">
-        <v>501</v>
+        <v>495</v>
       </c>
       <c r="F174" s="2" t="s">
         <v>305</v>
@@ -9917,7 +10126,7 @@
       </c>
       <c r="P174" s="66"/>
     </row>
-    <row r="175" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A175" s="113">
         <v>163</v>
       </c>
@@ -9931,7 +10140,7 @@
         <v>306</v>
       </c>
       <c r="E175" s="129" t="s">
-        <v>519</v>
+        <v>509</v>
       </c>
       <c r="F175" s="2" t="s">
         <v>307</v>
@@ -9955,7 +10164,7 @@
       </c>
       <c r="P175" s="66"/>
     </row>
-    <row r="176" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A176" s="113">
         <v>164</v>
       </c>
@@ -9969,7 +10178,7 @@
         <v>308</v>
       </c>
       <c r="E176" s="129" t="s">
-        <v>520</v>
+        <v>510</v>
       </c>
       <c r="F176" s="2" t="s">
         <v>307</v>
@@ -9993,7 +10202,7 @@
       </c>
       <c r="P176" s="66"/>
     </row>
-    <row r="177" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A177" s="113">
         <v>165</v>
       </c>
@@ -10007,7 +10216,7 @@
         <v>309</v>
       </c>
       <c r="E177" s="129" t="s">
-        <v>521</v>
+        <v>511</v>
       </c>
       <c r="F177" s="2" t="s">
         <v>310</v>
@@ -10031,7 +10240,7 @@
       </c>
       <c r="P177" s="66"/>
     </row>
-    <row r="178" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A178" s="113">
         <v>166</v>
       </c>
@@ -10069,7 +10278,7 @@
       </c>
       <c r="P178" s="66"/>
     </row>
-    <row r="179" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A179" s="113">
         <v>167</v>
       </c>
@@ -10107,7 +10316,7 @@
       </c>
       <c r="P179" s="66"/>
     </row>
-    <row r="180" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A180" s="113">
         <v>168</v>
       </c>
@@ -10145,7 +10354,7 @@
       </c>
       <c r="P180" s="66"/>
     </row>
-    <row r="181" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A181" s="113">
         <v>169</v>
       </c>
@@ -10159,7 +10368,7 @@
         <v>316</v>
       </c>
       <c r="E181" s="129" t="s">
-        <v>547</v>
+        <v>529</v>
       </c>
       <c r="F181" s="2" t="s">
         <v>317</v>
@@ -10183,7 +10392,7 @@
       </c>
       <c r="P181" s="66"/>
     </row>
-    <row r="182" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A182" s="113">
         <v>170</v>
       </c>
@@ -10197,7 +10406,7 @@
         <v>318</v>
       </c>
       <c r="E182" s="129" t="s">
-        <v>548</v>
+        <v>530</v>
       </c>
       <c r="F182" s="2" t="s">
         <v>317</v>
@@ -10221,7 +10430,7 @@
       </c>
       <c r="P182" s="66"/>
     </row>
-    <row r="183" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A183" s="113">
         <v>171</v>
       </c>
@@ -10235,7 +10444,7 @@
         <v>319</v>
       </c>
       <c r="E183" s="129" t="s">
-        <v>549</v>
+        <v>531</v>
       </c>
       <c r="F183" s="2" t="s">
         <v>320</v>
@@ -10259,7 +10468,7 @@
       </c>
       <c r="P183" s="66"/>
     </row>
-    <row r="184" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A184" s="113">
         <v>172</v>
       </c>
@@ -10273,7 +10482,7 @@
         <v>321</v>
       </c>
       <c r="E184" s="129" t="s">
-        <v>567</v>
+        <v>545</v>
       </c>
       <c r="F184" s="2" t="s">
         <v>322</v>
@@ -10297,7 +10506,7 @@
       </c>
       <c r="P184" s="66"/>
     </row>
-    <row r="185" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A185" s="113">
         <v>173</v>
       </c>
@@ -10311,7 +10520,7 @@
         <v>323</v>
       </c>
       <c r="E185" s="129" t="s">
-        <v>568</v>
+        <v>546</v>
       </c>
       <c r="F185" s="2" t="s">
         <v>322</v>
@@ -10335,7 +10544,7 @@
       </c>
       <c r="P185" s="66"/>
     </row>
-    <row r="186" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A186" s="113">
         <v>174</v>
       </c>
@@ -10349,7 +10558,7 @@
         <v>324</v>
       </c>
       <c r="E186" s="129" t="s">
-        <v>569</v>
+        <v>547</v>
       </c>
       <c r="F186" s="2" t="s">
         <v>325</v>
@@ -10373,7 +10582,7 @@
       </c>
       <c r="P186" s="66"/>
     </row>
-    <row r="187" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A187" s="113">
         <v>175</v>
       </c>
@@ -10411,7 +10620,7 @@
       </c>
       <c r="P187" s="66"/>
     </row>
-    <row r="188" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A188" s="113">
         <v>176</v>
       </c>
@@ -10449,7 +10658,7 @@
       </c>
       <c r="P188" s="66"/>
     </row>
-    <row r="189" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A189" s="113">
         <v>177</v>
       </c>
@@ -10487,7 +10696,7 @@
       </c>
       <c r="P189" s="66"/>
     </row>
-    <row r="190" spans="1:16" s="83" customFormat="1" ht="14.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="190" spans="1:16" s="83" customFormat="1" ht="14.55" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A190" s="114">
         <v>178</v>
       </c>
@@ -10525,7 +10734,7 @@
       </c>
       <c r="P190" s="68"/>
     </row>
-    <row r="191" spans="1:16" ht="14.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:16" ht="14.55" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
       <c r="A191" s="113">
         <v>179</v>
       </c>
@@ -10565,7 +10774,7 @@
       </c>
       <c r="P191" s="66"/>
     </row>
-    <row r="192" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A192" s="113">
         <v>180</v>
       </c>
@@ -10579,7 +10788,7 @@
         <v>341</v>
       </c>
       <c r="E192" s="129" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="F192" s="2" t="s">
         <v>387</v>
@@ -10603,7 +10812,7 @@
       </c>
       <c r="P192" s="66"/>
     </row>
-    <row r="193" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A193" s="113">
         <v>181</v>
       </c>
@@ -10617,7 +10826,7 @@
         <v>342</v>
       </c>
       <c r="E193" s="129" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="F193" s="2" t="s">
         <v>387</v>
@@ -10641,7 +10850,7 @@
       </c>
       <c r="P193" s="66"/>
     </row>
-    <row r="194" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A194" s="113">
         <v>182</v>
       </c>
@@ -10655,7 +10864,7 @@
         <v>343</v>
       </c>
       <c r="E194" s="129" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="F194" s="2" t="s">
         <v>388</v>
@@ -10679,7 +10888,7 @@
       </c>
       <c r="P194" s="66"/>
     </row>
-    <row r="195" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A195" s="113">
         <v>183</v>
       </c>
@@ -10693,7 +10902,7 @@
         <v>344</v>
       </c>
       <c r="E195" s="129" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="F195" s="2" t="s">
         <v>389</v>
@@ -10717,7 +10926,7 @@
       </c>
       <c r="P195" s="66"/>
     </row>
-    <row r="196" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A196" s="113">
         <v>184</v>
       </c>
@@ -10731,7 +10940,7 @@
         <v>345</v>
       </c>
       <c r="E196" s="129" t="s">
-        <v>502</v>
+        <v>496</v>
       </c>
       <c r="F196" s="2" t="s">
         <v>390</v>
@@ -10755,7 +10964,7 @@
       </c>
       <c r="P196" s="66"/>
     </row>
-    <row r="197" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A197" s="113">
         <v>185</v>
       </c>
@@ -10769,7 +10978,7 @@
         <v>346</v>
       </c>
       <c r="E197" s="129" t="s">
-        <v>503</v>
+        <v>497</v>
       </c>
       <c r="F197" s="2" t="s">
         <v>390</v>
@@ -10793,7 +11002,7 @@
       </c>
       <c r="P197" s="66"/>
     </row>
-    <row r="198" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A198" s="113">
         <v>186</v>
       </c>
@@ -10807,7 +11016,7 @@
         <v>347</v>
       </c>
       <c r="E198" s="129" t="s">
-        <v>504</v>
+        <v>498</v>
       </c>
       <c r="F198" s="2" t="s">
         <v>391</v>
@@ -10831,7 +11040,7 @@
       </c>
       <c r="P198" s="66"/>
     </row>
-    <row r="199" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A199" s="113">
         <v>187</v>
       </c>
@@ -10845,7 +11054,7 @@
         <v>348</v>
       </c>
       <c r="E199" s="129" t="s">
-        <v>522</v>
+        <v>512</v>
       </c>
       <c r="F199" s="2" t="s">
         <v>392</v>
@@ -10869,7 +11078,7 @@
       </c>
       <c r="P199" s="66"/>
     </row>
-    <row r="200" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A200" s="113">
         <v>188</v>
       </c>
@@ -10883,7 +11092,7 @@
         <v>349</v>
       </c>
       <c r="E200" s="129" t="s">
-        <v>523</v>
+        <v>513</v>
       </c>
       <c r="F200" s="2" t="s">
         <v>392</v>
@@ -10907,7 +11116,7 @@
       </c>
       <c r="P200" s="66"/>
     </row>
-    <row r="201" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A201" s="113">
         <v>189</v>
       </c>
@@ -10921,7 +11130,7 @@
         <v>350</v>
       </c>
       <c r="E201" s="129" t="s">
-        <v>524</v>
+        <v>514</v>
       </c>
       <c r="F201" s="2" t="s">
         <v>393</v>
@@ -10945,7 +11154,7 @@
       </c>
       <c r="P201" s="66"/>
     </row>
-    <row r="202" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A202" s="113">
         <v>190</v>
       </c>
@@ -10983,7 +11192,7 @@
       </c>
       <c r="P202" s="66"/>
     </row>
-    <row r="203" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A203" s="113">
         <v>191</v>
       </c>
@@ -11021,7 +11230,7 @@
       </c>
       <c r="P203" s="66"/>
     </row>
-    <row r="204" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A204" s="113">
         <v>192</v>
       </c>
@@ -11059,7 +11268,7 @@
       </c>
       <c r="P204" s="66"/>
     </row>
-    <row r="205" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A205" s="113">
         <v>193</v>
       </c>
@@ -11073,7 +11282,7 @@
         <v>354</v>
       </c>
       <c r="E205" s="129" t="s">
-        <v>550</v>
+        <v>532</v>
       </c>
       <c r="F205" s="2" t="s">
         <v>396</v>
@@ -11097,7 +11306,7 @@
       </c>
       <c r="P205" s="66"/>
     </row>
-    <row r="206" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A206" s="113">
         <v>194</v>
       </c>
@@ -11111,7 +11320,7 @@
         <v>355</v>
       </c>
       <c r="E206" s="129" t="s">
-        <v>551</v>
+        <v>533</v>
       </c>
       <c r="F206" s="2" t="s">
         <v>396</v>
@@ -11135,7 +11344,7 @@
       </c>
       <c r="P206" s="66"/>
     </row>
-    <row r="207" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A207" s="113">
         <v>195</v>
       </c>
@@ -11149,7 +11358,7 @@
         <v>356</v>
       </c>
       <c r="E207" s="129" t="s">
-        <v>552</v>
+        <v>534</v>
       </c>
       <c r="F207" s="2" t="s">
         <v>397</v>
@@ -11173,7 +11382,7 @@
       </c>
       <c r="P207" s="66"/>
     </row>
-    <row r="208" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A208" s="113">
         <v>196</v>
       </c>
@@ -11187,7 +11396,7 @@
         <v>357</v>
       </c>
       <c r="E208" s="129" t="s">
-        <v>570</v>
+        <v>548</v>
       </c>
       <c r="F208" s="2" t="s">
         <v>398</v>
@@ -11211,7 +11420,7 @@
       </c>
       <c r="P208" s="66"/>
     </row>
-    <row r="209" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A209" s="113">
         <v>197</v>
       </c>
@@ -11225,7 +11434,7 @@
         <v>358</v>
       </c>
       <c r="E209" s="129" t="s">
-        <v>571</v>
+        <v>549</v>
       </c>
       <c r="F209" s="2" t="s">
         <v>398</v>
@@ -11249,7 +11458,7 @@
       </c>
       <c r="P209" s="66"/>
     </row>
-    <row r="210" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A210" s="113">
         <v>198</v>
       </c>
@@ -11263,7 +11472,7 @@
         <v>359</v>
       </c>
       <c r="E210" s="129" t="s">
-        <v>572</v>
+        <v>550</v>
       </c>
       <c r="F210" s="2" t="s">
         <v>399</v>
@@ -11287,7 +11496,7 @@
       </c>
       <c r="P210" s="66"/>
     </row>
-    <row r="211" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A211" s="113">
         <v>199</v>
       </c>
@@ -11325,7 +11534,7 @@
       </c>
       <c r="P211" s="66"/>
     </row>
-    <row r="212" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A212" s="113">
         <v>200</v>
       </c>
@@ -11363,7 +11572,7 @@
       </c>
       <c r="P212" s="66"/>
     </row>
-    <row r="213" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A213" s="113">
         <v>201</v>
       </c>
@@ -11401,7 +11610,7 @@
       </c>
       <c r="P213" s="66"/>
     </row>
-    <row r="214" spans="1:16" ht="14.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="214" spans="1:16" ht="14.55" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A214" s="114">
         <v>202</v>
       </c>
@@ -11439,7 +11648,7 @@
       </c>
       <c r="P214" s="68"/>
     </row>
-    <row r="215" spans="1:16" ht="14.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:16" ht="14.55" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
       <c r="A215" s="113">
         <v>203</v>
       </c>
@@ -11479,7 +11688,7 @@
       </c>
       <c r="P215" s="66"/>
     </row>
-    <row r="216" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A216" s="113">
         <v>204</v>
       </c>
@@ -11493,7 +11702,7 @@
         <v>364</v>
       </c>
       <c r="E216" s="129" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="F216" s="2" t="s">
         <v>403</v>
@@ -11517,7 +11726,7 @@
       </c>
       <c r="P216" s="66"/>
     </row>
-    <row r="217" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A217" s="113">
         <v>205</v>
       </c>
@@ -11531,7 +11740,7 @@
         <v>365</v>
       </c>
       <c r="E217" s="129" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="F217" s="2" t="s">
         <v>403</v>
@@ -11555,7 +11764,7 @@
       </c>
       <c r="P217" s="66"/>
     </row>
-    <row r="218" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A218" s="113">
         <v>206</v>
       </c>
@@ -11569,7 +11778,7 @@
         <v>366</v>
       </c>
       <c r="E218" s="129" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="F218" s="2" t="s">
         <v>404</v>
@@ -11593,7 +11802,7 @@
       </c>
       <c r="P218" s="66"/>
     </row>
-    <row r="219" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A219" s="113">
         <v>207</v>
       </c>
@@ -11607,7 +11816,7 @@
         <v>367</v>
       </c>
       <c r="E219" s="129" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="F219" s="2" t="s">
         <v>405</v>
@@ -11631,7 +11840,7 @@
       </c>
       <c r="P219" s="66"/>
     </row>
-    <row r="220" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A220" s="113">
         <v>208</v>
       </c>
@@ -11645,7 +11854,7 @@
         <v>368</v>
       </c>
       <c r="E220" s="129" t="s">
-        <v>505</v>
+        <v>499</v>
       </c>
       <c r="F220" s="2" t="s">
         <v>406</v>
@@ -11669,7 +11878,7 @@
       </c>
       <c r="P220" s="66"/>
     </row>
-    <row r="221" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A221" s="113">
         <v>209</v>
       </c>
@@ -11683,7 +11892,7 @@
         <v>369</v>
       </c>
       <c r="E221" s="129" t="s">
-        <v>506</v>
+        <v>500</v>
       </c>
       <c r="F221" s="2" t="s">
         <v>406</v>
@@ -11707,7 +11916,7 @@
       </c>
       <c r="P221" s="66"/>
     </row>
-    <row r="222" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A222" s="113">
         <v>210</v>
       </c>
@@ -11721,7 +11930,7 @@
         <v>370</v>
       </c>
       <c r="E222" s="129" t="s">
-        <v>507</v>
+        <v>501</v>
       </c>
       <c r="F222" s="2" t="s">
         <v>407</v>
@@ -11745,7 +11954,7 @@
       </c>
       <c r="P222" s="66"/>
     </row>
-    <row r="223" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A223" s="113">
         <v>211</v>
       </c>
@@ -11759,7 +11968,7 @@
         <v>371</v>
       </c>
       <c r="E223" s="129" t="s">
-        <v>525</v>
+        <v>515</v>
       </c>
       <c r="F223" s="2" t="s">
         <v>408</v>
@@ -11783,7 +11992,7 @@
       </c>
       <c r="P223" s="66"/>
     </row>
-    <row r="224" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A224" s="113">
         <v>212</v>
       </c>
@@ -11797,7 +12006,7 @@
         <v>372</v>
       </c>
       <c r="E224" s="129" t="s">
-        <v>526</v>
+        <v>516</v>
       </c>
       <c r="F224" s="2" t="s">
         <v>408</v>
@@ -11821,7 +12030,7 @@
       </c>
       <c r="P224" s="66"/>
     </row>
-    <row r="225" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A225" s="113">
         <v>213</v>
       </c>
@@ -11835,7 +12044,7 @@
         <v>373</v>
       </c>
       <c r="E225" s="129" t="s">
-        <v>527</v>
+        <v>517</v>
       </c>
       <c r="F225" s="2" t="s">
         <v>409</v>
@@ -11859,7 +12068,7 @@
       </c>
       <c r="P225" s="66"/>
     </row>
-    <row r="226" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A226" s="113">
         <v>214</v>
       </c>
@@ -11897,7 +12106,7 @@
       </c>
       <c r="P226" s="66"/>
     </row>
-    <row r="227" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A227" s="113">
         <v>215</v>
       </c>
@@ -11935,7 +12144,7 @@
       </c>
       <c r="P227" s="66"/>
     </row>
-    <row r="228" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A228" s="113">
         <v>216</v>
       </c>
@@ -11973,7 +12182,7 @@
       </c>
       <c r="P228" s="66"/>
     </row>
-    <row r="229" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A229" s="113">
         <v>217</v>
       </c>
@@ -11987,7 +12196,7 @@
         <v>377</v>
       </c>
       <c r="E229" s="129" t="s">
-        <v>553</v>
+        <v>535</v>
       </c>
       <c r="F229" s="2" t="s">
         <v>412</v>
@@ -12011,7 +12220,7 @@
       </c>
       <c r="P229" s="66"/>
     </row>
-    <row r="230" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A230" s="113">
         <v>218</v>
       </c>
@@ -12025,7 +12234,7 @@
         <v>378</v>
       </c>
       <c r="E230" s="129" t="s">
-        <v>554</v>
+        <v>536</v>
       </c>
       <c r="F230" s="2" t="s">
         <v>412</v>
@@ -12049,7 +12258,7 @@
       </c>
       <c r="P230" s="66"/>
     </row>
-    <row r="231" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A231" s="113">
         <v>219</v>
       </c>
@@ -12063,7 +12272,7 @@
         <v>379</v>
       </c>
       <c r="E231" s="129" t="s">
-        <v>555</v>
+        <v>537</v>
       </c>
       <c r="F231" s="2" t="s">
         <v>413</v>
@@ -12087,7 +12296,7 @@
       </c>
       <c r="P231" s="66"/>
     </row>
-    <row r="232" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A232" s="113">
         <v>220</v>
       </c>
@@ -12101,7 +12310,7 @@
         <v>380</v>
       </c>
       <c r="E232" s="129" t="s">
-        <v>573</v>
+        <v>551</v>
       </c>
       <c r="F232" s="2" t="s">
         <v>414</v>
@@ -12125,7 +12334,7 @@
       </c>
       <c r="P232" s="66"/>
     </row>
-    <row r="233" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A233" s="113">
         <v>221</v>
       </c>
@@ -12139,7 +12348,7 @@
         <v>381</v>
       </c>
       <c r="E233" s="129" t="s">
-        <v>574</v>
+        <v>552</v>
       </c>
       <c r="F233" s="2" t="s">
         <v>414</v>
@@ -12163,7 +12372,7 @@
       </c>
       <c r="P233" s="66"/>
     </row>
-    <row r="234" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A234" s="113">
         <v>222</v>
       </c>
@@ -12177,7 +12386,7 @@
         <v>382</v>
       </c>
       <c r="E234" s="129" t="s">
-        <v>575</v>
+        <v>553</v>
       </c>
       <c r="F234" s="2" t="s">
         <v>415</v>
@@ -12201,7 +12410,7 @@
       </c>
       <c r="P234" s="66"/>
     </row>
-    <row r="235" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A235" s="113">
         <v>223</v>
       </c>
@@ -12239,7 +12448,7 @@
       </c>
       <c r="P235" s="66"/>
     </row>
-    <row r="236" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A236" s="113">
         <v>224</v>
       </c>
@@ -12277,7 +12486,7 @@
       </c>
       <c r="P236" s="66"/>
     </row>
-    <row r="237" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A237" s="113">
         <v>225</v>
       </c>
@@ -12315,7 +12524,7 @@
       </c>
       <c r="P237" s="66"/>
     </row>
-    <row r="238" spans="1:16" s="26" customFormat="1" ht="14.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="238" spans="1:16" s="26" customFormat="1" ht="14.55" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A238" s="115">
         <v>226</v>
       </c>
@@ -12354,8 +12563,11 @@
       <c r="P238" s="69"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M119" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:M238" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <phoneticPr fontId="7" type="noConversion"/>
+  <conditionalFormatting sqref="E1:E1048576">
+    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Add assurance as extended datapoint
</commit_message>
<xml_diff>
--- a/dataland-framework-toolbox/inputs/eu-taxonomy-financials/eu-taxonomy-financials.xlsx
+++ b/dataland-framework-toolbox/inputs/eu-taxonomy-financials/eu-taxonomy-financials.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d93542\Dataland\dataland-framework-toolbox\inputs\eu-taxonomy-financials\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d93545\Desktop\Dataland\Dataland\dataland-framework-toolbox\inputs\eu-taxonomy-financials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5128F844-C87B-4590-A7AD-F78B0FAE5EFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D51E76A9-3BAE-48AC-9D23-BFEACEA4D2FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-5145" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="50865" yWindow="4920" windowWidth="28800" windowHeight="15225" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Framework Data Model" sheetId="1" r:id="rId1"/>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2180" uniqueCount="697">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2181" uniqueCount="697">
   <si>
     <t>Field Identifier</t>
   </si>
@@ -3662,8 +3662,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P238"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3973,7 +3973,9 @@
         <v>14</v>
       </c>
       <c r="I8" s="24"/>
-      <c r="J8" s="24"/>
+      <c r="J8" s="17" t="s">
+        <v>24</v>
+      </c>
       <c r="K8" s="24"/>
       <c r="L8" s="24"/>
       <c r="M8" s="3"/>

</xml_diff>